<commit_message>
add RKI data downloaded 2021-01-03--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Nowcasting_Zahlen.xlsx
+++ b/rki-data/RKI-Nowcasting_Zahlen.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61D97A5-4086-4D85-8396-DAC4972E324F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-01-02\Nowcast\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{87A9A508-C702-48DD-9C53-0F20F7B4F28F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24420" windowHeight="11565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="1" r:id="rId1"/>
@@ -27,7 +32,7 @@
     <t>Ergebnisse des Nowcastings und der Schätzung der Reproduktionszahl R</t>
   </si>
   <si>
-    <t>Datenstand: 31.12.2020, 00:00 Uhr</t>
+    <t>Datenstand: 02.01.2021, 00:00 Uhr</t>
   </si>
   <si>
     <t>Die Ergebnisse des Nowcastings, also die Schätzung der Anzahl von COVID-19 Neuerkrankungen wird dargestellt mit einem gleitenden 4-Tages-Mittelwert.</t>
@@ -36,7 +41,7 @@
     <t>Dabei wird jeder Wert mit den Werten der 3 vorhergehenden Tage gemittelt.</t>
   </si>
   <si>
-    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 31.12.2020 dargestellten Nowcasting-Kurve.</t>
+    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 02.01.2021 dargestellten Nowcasting-Kurve.</t>
   </si>
   <si>
     <t>Der letzte Schätzwert der Reproduktionszahl R wird ebenfalls im gleichen Lagebericht erwähnt.</t>
@@ -138,10 +143,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -554,7 +559,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -562,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M341"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -578,10 +582,10 @@
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -9319,10 +9323,10 @@
         <v>44106</v>
       </c>
       <c r="B216">
-        <v>3372</v>
+        <v>3373</v>
       </c>
       <c r="C216">
-        <v>3301</v>
+        <v>3298</v>
       </c>
       <c r="D216">
         <v>3438</v>
@@ -9363,13 +9367,13 @@
         <v>3357</v>
       </c>
       <c r="C217">
-        <v>3291</v>
+        <v>3290</v>
       </c>
       <c r="D217">
         <v>3440</v>
       </c>
       <c r="E217">
-        <v>3130</v>
+        <v>3131</v>
       </c>
       <c r="F217">
         <v>3057</v>
@@ -9404,7 +9408,7 @@
         <v>3420</v>
       </c>
       <c r="C218">
-        <v>3352</v>
+        <v>3353</v>
       </c>
       <c r="D218">
         <v>3472</v>
@@ -9445,19 +9449,19 @@
         <v>4758</v>
       </c>
       <c r="C219">
-        <v>4677</v>
+        <v>4676</v>
       </c>
       <c r="D219">
-        <v>4843</v>
+        <v>4846</v>
       </c>
       <c r="E219">
         <v>3727</v>
       </c>
       <c r="F219">
-        <v>3655</v>
+        <v>3654</v>
       </c>
       <c r="G219">
-        <v>3798</v>
+        <v>3799</v>
       </c>
       <c r="H219">
         <v>1.33</v>
@@ -9486,10 +9490,10 @@
         <v>4794</v>
       </c>
       <c r="C220">
-        <v>4701</v>
+        <v>4703</v>
       </c>
       <c r="D220">
-        <v>4888</v>
+        <v>4885</v>
       </c>
       <c r="E220">
         <v>4082</v>
@@ -9524,22 +9528,22 @@
         <v>44111</v>
       </c>
       <c r="B221">
-        <v>4913</v>
+        <v>4912</v>
       </c>
       <c r="C221">
-        <v>4832</v>
+        <v>4824</v>
       </c>
       <c r="D221">
-        <v>5006</v>
+        <v>5002</v>
       </c>
       <c r="E221">
         <v>4471</v>
       </c>
       <c r="F221">
-        <v>4390</v>
+        <v>4389</v>
       </c>
       <c r="G221">
-        <v>4552</v>
+        <v>4551</v>
       </c>
       <c r="H221">
         <v>1.43</v>
@@ -9568,7 +9572,7 @@
         <v>4979</v>
       </c>
       <c r="C222">
-        <v>4885</v>
+        <v>4887</v>
       </c>
       <c r="D222">
         <v>5078</v>
@@ -9577,10 +9581,10 @@
         <v>4861</v>
       </c>
       <c r="F222">
-        <v>4774</v>
+        <v>4772</v>
       </c>
       <c r="G222">
-        <v>4954</v>
+        <v>4953</v>
       </c>
       <c r="H222">
         <v>1.48</v>
@@ -9606,10 +9610,10 @@
         <v>44113</v>
       </c>
       <c r="B223">
-        <v>5380</v>
+        <v>5379</v>
       </c>
       <c r="C223">
-        <v>5301</v>
+        <v>5307</v>
       </c>
       <c r="D223">
         <v>5465</v>
@@ -9621,7 +9625,7 @@
         <v>4930</v>
       </c>
       <c r="G223">
-        <v>5109</v>
+        <v>5107</v>
       </c>
       <c r="H223">
         <v>1.35</v>
@@ -9636,7 +9640,7 @@
         <v>1.32</v>
       </c>
       <c r="L223">
-        <v>1.3</v>
+        <v>1.31</v>
       </c>
       <c r="M223">
         <v>1.32</v>
@@ -9647,13 +9651,13 @@
         <v>44114</v>
       </c>
       <c r="B224">
-        <v>5311</v>
+        <v>5310</v>
       </c>
       <c r="C224">
-        <v>5212</v>
+        <v>5211</v>
       </c>
       <c r="D224">
-        <v>5392</v>
+        <v>5386</v>
       </c>
       <c r="E224">
         <v>5145</v>
@@ -9662,7 +9666,7 @@
         <v>5057</v>
       </c>
       <c r="G224">
-        <v>5235</v>
+        <v>5232</v>
       </c>
       <c r="H224">
         <v>1.26</v>
@@ -9688,22 +9692,22 @@
         <v>44115</v>
       </c>
       <c r="B225">
-        <v>5500</v>
+        <v>5499</v>
       </c>
       <c r="C225">
-        <v>5386</v>
+        <v>5382</v>
       </c>
       <c r="D225">
-        <v>5575</v>
+        <v>5573</v>
       </c>
       <c r="E225">
         <v>5292</v>
       </c>
       <c r="F225">
-        <v>5196</v>
+        <v>5197</v>
       </c>
       <c r="G225">
-        <v>5377</v>
+        <v>5375</v>
       </c>
       <c r="H225">
         <v>1.18</v>
@@ -9729,22 +9733,22 @@
         <v>44116</v>
       </c>
       <c r="B226">
-        <v>7499</v>
+        <v>7498</v>
       </c>
       <c r="C226">
-        <v>7400</v>
+        <v>7392</v>
       </c>
       <c r="D226">
-        <v>7610</v>
+        <v>7602</v>
       </c>
       <c r="E226">
         <v>5922</v>
       </c>
       <c r="F226">
-        <v>5824</v>
+        <v>5823</v>
       </c>
       <c r="G226">
-        <v>6010</v>
+        <v>6006</v>
       </c>
       <c r="H226">
         <v>1.22</v>
@@ -9753,7 +9757,7 @@
         <v>1.2</v>
       </c>
       <c r="J226">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="K226">
         <v>1.31</v>
@@ -9770,22 +9774,22 @@
         <v>44117</v>
       </c>
       <c r="B227">
-        <v>7856</v>
+        <v>7855</v>
       </c>
       <c r="C227">
-        <v>7748</v>
+        <v>7749</v>
       </c>
       <c r="D227">
-        <v>7965</v>
+        <v>7961</v>
       </c>
       <c r="E227">
         <v>6541</v>
       </c>
       <c r="F227">
-        <v>6436</v>
+        <v>6433</v>
       </c>
       <c r="G227">
-        <v>6635</v>
+        <v>6630</v>
       </c>
       <c r="H227">
         <v>1.3</v>
@@ -9811,22 +9815,22 @@
         <v>44118</v>
       </c>
       <c r="B228">
-        <v>8438</v>
+        <v>8437</v>
       </c>
       <c r="C228">
-        <v>8301</v>
+        <v>8290</v>
       </c>
       <c r="D228">
-        <v>8579</v>
+        <v>8576</v>
       </c>
       <c r="E228">
-        <v>7323</v>
+        <v>7322</v>
       </c>
       <c r="F228">
-        <v>7208</v>
+        <v>7203</v>
       </c>
       <c r="G228">
-        <v>7432</v>
+        <v>7428</v>
       </c>
       <c r="H228">
         <v>1.42</v>
@@ -9852,22 +9856,22 @@
         <v>44119</v>
       </c>
       <c r="B229">
-        <v>8695</v>
+        <v>8692</v>
       </c>
       <c r="C229">
-        <v>8572</v>
+        <v>8588</v>
       </c>
       <c r="D229">
-        <v>8831</v>
+        <v>8817</v>
       </c>
       <c r="E229">
-        <v>8122</v>
+        <v>8121</v>
       </c>
       <c r="F229">
         <v>8005</v>
       </c>
       <c r="G229">
-        <v>8246</v>
+        <v>8239</v>
       </c>
       <c r="H229">
         <v>1.53</v>
@@ -9893,22 +9897,22 @@
         <v>44120</v>
       </c>
       <c r="B230">
-        <v>9553</v>
+        <v>9559</v>
       </c>
       <c r="C230">
-        <v>9420</v>
+        <v>9404</v>
       </c>
       <c r="D230">
-        <v>9679</v>
+        <v>9674</v>
       </c>
       <c r="E230">
         <v>8636</v>
       </c>
       <c r="F230">
-        <v>8510</v>
+        <v>8508</v>
       </c>
       <c r="G230">
-        <v>8763</v>
+        <v>8757</v>
       </c>
       <c r="H230">
         <v>1.46</v>
@@ -9934,22 +9938,22 @@
         <v>44121</v>
       </c>
       <c r="B231">
-        <v>9361</v>
+        <v>9358</v>
       </c>
       <c r="C231">
-        <v>9238</v>
+        <v>9220</v>
       </c>
       <c r="D231">
-        <v>9490</v>
+        <v>9488</v>
       </c>
       <c r="E231">
-        <v>9012</v>
+        <v>9011</v>
       </c>
       <c r="F231">
-        <v>8883</v>
+        <v>8876</v>
       </c>
       <c r="G231">
-        <v>9144</v>
+        <v>9139</v>
       </c>
       <c r="H231">
         <v>1.38</v>
@@ -9975,22 +9979,22 @@
         <v>44122</v>
       </c>
       <c r="B232">
-        <v>10456</v>
+        <v>10457</v>
       </c>
       <c r="C232">
-        <v>10337</v>
+        <v>10334</v>
       </c>
       <c r="D232">
-        <v>10632</v>
+        <v>10622</v>
       </c>
       <c r="E232">
         <v>9516</v>
       </c>
       <c r="F232">
-        <v>9392</v>
+        <v>9386</v>
       </c>
       <c r="G232">
-        <v>9658</v>
+        <v>9650</v>
       </c>
       <c r="H232">
         <v>1.3</v>
@@ -10016,22 +10020,22 @@
         <v>44123</v>
       </c>
       <c r="B233">
-        <v>13818</v>
+        <v>13826</v>
       </c>
       <c r="C233">
-        <v>13670</v>
+        <v>13664</v>
       </c>
       <c r="D233">
-        <v>13977</v>
+        <v>13978</v>
       </c>
       <c r="E233">
-        <v>10797</v>
+        <v>10800</v>
       </c>
       <c r="F233">
-        <v>10666</v>
+        <v>10655</v>
       </c>
       <c r="G233">
-        <v>10944</v>
+        <v>10941</v>
       </c>
       <c r="H233">
         <v>1.33</v>
@@ -10057,22 +10061,22 @@
         <v>44124</v>
       </c>
       <c r="B234">
-        <v>14824</v>
+        <v>14820</v>
       </c>
       <c r="C234">
-        <v>14648</v>
+        <v>14634</v>
       </c>
       <c r="D234">
-        <v>14977</v>
+        <v>14949</v>
       </c>
       <c r="E234">
         <v>12115</v>
       </c>
       <c r="F234">
-        <v>11973</v>
+        <v>11963</v>
       </c>
       <c r="G234">
-        <v>12269</v>
+        <v>12259</v>
       </c>
       <c r="H234">
         <v>1.4</v>
@@ -10098,22 +10102,22 @@
         <v>44125</v>
       </c>
       <c r="B235">
-        <v>15393</v>
+        <v>15394</v>
       </c>
       <c r="C235">
-        <v>15223</v>
+        <v>15227</v>
       </c>
       <c r="D235">
-        <v>15560</v>
+        <v>15570</v>
       </c>
       <c r="E235">
-        <v>13623</v>
+        <v>13624</v>
       </c>
       <c r="F235">
-        <v>13469</v>
+        <v>13464</v>
       </c>
       <c r="G235">
-        <v>13786</v>
+        <v>13780</v>
       </c>
       <c r="H235">
         <v>1.51</v>
@@ -10139,22 +10143,22 @@
         <v>44126</v>
       </c>
       <c r="B236">
-        <v>15038</v>
+        <v>15032</v>
       </c>
       <c r="C236">
-        <v>14855</v>
+        <v>14858</v>
       </c>
       <c r="D236">
-        <v>15208</v>
+        <v>15188</v>
       </c>
       <c r="E236">
         <v>14768</v>
       </c>
       <c r="F236">
-        <v>14599</v>
+        <v>14596</v>
       </c>
       <c r="G236">
-        <v>14930</v>
+        <v>14921</v>
       </c>
       <c r="H236">
         <v>1.55</v>
@@ -10163,7 +10167,7 @@
         <v>1.54</v>
       </c>
       <c r="J236">
-        <v>1.57</v>
+        <v>1.56</v>
       </c>
       <c r="K236">
         <v>1.39</v>
@@ -10180,22 +10184,22 @@
         <v>44127</v>
       </c>
       <c r="B237">
-        <v>15845</v>
+        <v>15853</v>
       </c>
       <c r="C237">
-        <v>15654</v>
+        <v>15649</v>
       </c>
       <c r="D237">
-        <v>15986</v>
+        <v>16039</v>
       </c>
       <c r="E237">
         <v>15275</v>
       </c>
       <c r="F237">
-        <v>15095</v>
+        <v>15092</v>
       </c>
       <c r="G237">
-        <v>15433</v>
+        <v>15436</v>
       </c>
       <c r="H237">
         <v>1.41</v>
@@ -10221,22 +10225,22 @@
         <v>44128</v>
       </c>
       <c r="B238">
-        <v>15077</v>
+        <v>15088</v>
       </c>
       <c r="C238">
-        <v>14913</v>
+        <v>14916</v>
       </c>
       <c r="D238">
-        <v>15251</v>
+        <v>15236</v>
       </c>
       <c r="E238">
-        <v>15338</v>
+        <v>15342</v>
       </c>
       <c r="F238">
-        <v>15161</v>
+        <v>15162</v>
       </c>
       <c r="G238">
-        <v>15501</v>
+        <v>15508</v>
       </c>
       <c r="H238">
         <v>1.27</v>
@@ -10262,22 +10266,22 @@
         <v>44129</v>
       </c>
       <c r="B239">
-        <v>15647</v>
+        <v>15654</v>
       </c>
       <c r="C239">
-        <v>15491</v>
+        <v>15479</v>
       </c>
       <c r="D239">
-        <v>15776</v>
+        <v>15845</v>
       </c>
       <c r="E239">
-        <v>15402</v>
+        <v>15407</v>
       </c>
       <c r="F239">
-        <v>15228</v>
+        <v>15225</v>
       </c>
       <c r="G239">
-        <v>15555</v>
+        <v>15577</v>
       </c>
       <c r="H239">
         <v>1.1299999999999999</v>
@@ -10303,22 +10307,22 @@
         <v>44130</v>
       </c>
       <c r="B240">
-        <v>19210</v>
+        <v>19202</v>
       </c>
       <c r="C240">
-        <v>19032</v>
+        <v>19047</v>
       </c>
       <c r="D240">
-        <v>19369</v>
+        <v>19379</v>
       </c>
       <c r="E240">
-        <v>16445</v>
+        <v>16449</v>
       </c>
       <c r="F240">
-        <v>16272</v>
+        <v>16273</v>
       </c>
       <c r="G240">
-        <v>16595</v>
+        <v>16625</v>
       </c>
       <c r="H240">
         <v>1.1100000000000001</v>
@@ -10336,7 +10340,7 @@
         <v>1.2</v>
       </c>
       <c r="M240">
-        <v>1.22</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="241" spans="1:13">
@@ -10344,22 +10348,22 @@
         <v>44131</v>
       </c>
       <c r="B241">
-        <v>18414</v>
+        <v>18417</v>
       </c>
       <c r="C241">
-        <v>18236</v>
+        <v>18256</v>
       </c>
       <c r="D241">
-        <v>18588</v>
+        <v>18617</v>
       </c>
       <c r="E241">
-        <v>17087</v>
+        <v>17090</v>
       </c>
       <c r="F241">
-        <v>16918</v>
+        <v>16924</v>
       </c>
       <c r="G241">
-        <v>17246</v>
+        <v>17269</v>
       </c>
       <c r="H241">
         <v>1.1200000000000001</v>
@@ -10385,22 +10389,22 @@
         <v>44132</v>
       </c>
       <c r="B242">
-        <v>18099</v>
+        <v>18090</v>
       </c>
       <c r="C242">
-        <v>17915</v>
+        <v>17890</v>
       </c>
       <c r="D242">
-        <v>18268</v>
+        <v>18276</v>
       </c>
       <c r="E242">
-        <v>17843</v>
+        <v>17841</v>
       </c>
       <c r="F242">
         <v>17668</v>
       </c>
       <c r="G242">
-        <v>18000</v>
+        <v>18029</v>
       </c>
       <c r="H242">
         <v>1.1599999999999999</v>
@@ -10426,22 +10430,22 @@
         <v>44133</v>
       </c>
       <c r="B243">
-        <v>16806</v>
+        <v>16811</v>
       </c>
       <c r="C243">
-        <v>16650</v>
+        <v>16595</v>
       </c>
       <c r="D243">
-        <v>17021</v>
+        <v>16994</v>
       </c>
       <c r="E243">
-        <v>18132</v>
+        <v>18130</v>
       </c>
       <c r="F243">
-        <v>17958</v>
+        <v>17947</v>
       </c>
       <c r="G243">
-        <v>18311</v>
+        <v>18316</v>
       </c>
       <c r="H243">
         <v>1.18</v>
@@ -10450,7 +10454,7 @@
         <v>1.17</v>
       </c>
       <c r="J243">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="K243">
         <v>1.0900000000000001</v>
@@ -10467,28 +10471,28 @@
         <v>44134</v>
       </c>
       <c r="B244">
-        <v>17256</v>
+        <v>17247</v>
       </c>
       <c r="C244">
-        <v>17108</v>
+        <v>17091</v>
       </c>
       <c r="D244">
-        <v>17446</v>
+        <v>17386</v>
       </c>
       <c r="E244">
-        <v>17644</v>
+        <v>17641</v>
       </c>
       <c r="F244">
-        <v>17477</v>
+        <v>17458</v>
       </c>
       <c r="G244">
-        <v>17831</v>
+        <v>17818</v>
       </c>
       <c r="H244">
         <v>1.07</v>
       </c>
       <c r="I244">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="J244">
         <v>1.08</v>
@@ -10508,22 +10512,22 @@
         <v>44135</v>
       </c>
       <c r="B245">
-        <v>15597</v>
+        <v>15613</v>
       </c>
       <c r="C245">
-        <v>15457</v>
+        <v>15410</v>
       </c>
       <c r="D245">
-        <v>15749</v>
+        <v>15779</v>
       </c>
       <c r="E245">
         <v>16940</v>
       </c>
       <c r="F245">
-        <v>16782</v>
+        <v>16746</v>
       </c>
       <c r="G245">
-        <v>17121</v>
+        <v>17108</v>
       </c>
       <c r="H245">
         <v>0.99</v>
@@ -10549,22 +10553,22 @@
         <v>44136</v>
       </c>
       <c r="B246">
-        <v>16647</v>
+        <v>16655</v>
       </c>
       <c r="C246">
-        <v>16457</v>
+        <v>16493</v>
       </c>
       <c r="D246">
-        <v>16827</v>
+        <v>16837</v>
       </c>
       <c r="E246">
-        <v>16576</v>
+        <v>16582</v>
       </c>
       <c r="F246">
-        <v>16418</v>
+        <v>16397</v>
       </c>
       <c r="G246">
-        <v>16760</v>
+        <v>16749</v>
       </c>
       <c r="H246">
         <v>0.93</v>
@@ -10579,7 +10583,7 @@
         <v>1.04</v>
       </c>
       <c r="L246">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="M246">
         <v>1.04</v>
@@ -10590,19 +10594,19 @@
         <v>44137</v>
       </c>
       <c r="B247">
-        <v>20975</v>
+        <v>20967</v>
       </c>
       <c r="C247">
-        <v>20796</v>
+        <v>20782</v>
       </c>
       <c r="D247">
-        <v>21147</v>
+        <v>21166</v>
       </c>
       <c r="E247">
-        <v>17619</v>
+        <v>17621</v>
       </c>
       <c r="F247">
-        <v>17454</v>
+        <v>17444</v>
       </c>
       <c r="G247">
         <v>17792</v>
@@ -10631,22 +10635,22 @@
         <v>44138</v>
       </c>
       <c r="B248">
-        <v>19033</v>
+        <v>19018</v>
       </c>
       <c r="C248">
-        <v>18846</v>
+        <v>18842</v>
       </c>
       <c r="D248">
-        <v>19196</v>
+        <v>19200</v>
       </c>
       <c r="E248">
         <v>18063</v>
       </c>
       <c r="F248">
-        <v>17889</v>
+        <v>17882</v>
       </c>
       <c r="G248">
-        <v>18229</v>
+        <v>18245</v>
       </c>
       <c r="H248">
         <v>1.02</v>
@@ -10672,19 +10676,19 @@
         <v>44139</v>
       </c>
       <c r="B249">
-        <v>18014</v>
+        <v>18021</v>
       </c>
       <c r="C249">
-        <v>17816</v>
+        <v>17853</v>
       </c>
       <c r="D249">
-        <v>18207</v>
+        <v>18173</v>
       </c>
       <c r="E249">
-        <v>18667</v>
+        <v>18665</v>
       </c>
       <c r="F249">
-        <v>18479</v>
+        <v>18493</v>
       </c>
       <c r="G249">
         <v>18844</v>
@@ -10713,28 +10717,28 @@
         <v>44140</v>
       </c>
       <c r="B250">
-        <v>16540</v>
+        <v>16539</v>
       </c>
       <c r="C250">
-        <v>16382</v>
+        <v>16371</v>
       </c>
       <c r="D250">
-        <v>16711</v>
+        <v>16729</v>
       </c>
       <c r="E250">
-        <v>18641</v>
+        <v>18636</v>
       </c>
       <c r="F250">
-        <v>18460</v>
+        <v>18462</v>
       </c>
       <c r="G250">
-        <v>18815</v>
+        <v>18817</v>
       </c>
       <c r="H250">
         <v>1.1200000000000001</v>
       </c>
       <c r="I250">
-        <v>1.1100000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="J250">
         <v>1.1299999999999999</v>
@@ -10754,22 +10758,22 @@
         <v>44141</v>
       </c>
       <c r="B251">
-        <v>16109</v>
+        <v>16124</v>
       </c>
       <c r="C251">
-        <v>15944</v>
+        <v>15971</v>
       </c>
       <c r="D251">
-        <v>16271</v>
+        <v>16312</v>
       </c>
       <c r="E251">
-        <v>17424</v>
+        <v>17425</v>
       </c>
       <c r="F251">
-        <v>17247</v>
+        <v>17259</v>
       </c>
       <c r="G251">
-        <v>17596</v>
+        <v>17603</v>
       </c>
       <c r="H251">
         <v>0.99</v>
@@ -10795,19 +10799,19 @@
         <v>44142</v>
       </c>
       <c r="B252">
-        <v>15054</v>
+        <v>15049</v>
       </c>
       <c r="C252">
-        <v>14891</v>
+        <v>14901</v>
       </c>
       <c r="D252">
-        <v>15227</v>
+        <v>15204</v>
       </c>
       <c r="E252">
-        <v>16429</v>
+        <v>16433</v>
       </c>
       <c r="F252">
-        <v>16258</v>
+        <v>16274</v>
       </c>
       <c r="G252">
         <v>16604</v>
@@ -10839,19 +10843,19 @@
         <v>15143</v>
       </c>
       <c r="C253">
-        <v>14970</v>
+        <v>14942</v>
       </c>
       <c r="D253">
-        <v>15317</v>
+        <v>15322</v>
       </c>
       <c r="E253">
-        <v>15712</v>
+        <v>15714</v>
       </c>
       <c r="F253">
-        <v>15547</v>
+        <v>15546</v>
       </c>
       <c r="G253">
-        <v>15881</v>
+        <v>15892</v>
       </c>
       <c r="H253">
         <v>0.84</v>
@@ -10866,7 +10870,7 @@
         <v>0.96</v>
       </c>
       <c r="L253">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="M253">
         <v>0.96</v>
@@ -10877,22 +10881,22 @@
         <v>44144</v>
       </c>
       <c r="B254">
-        <v>19039</v>
+        <v>19037</v>
       </c>
       <c r="C254">
-        <v>18861</v>
+        <v>18852</v>
       </c>
       <c r="D254">
-        <v>19222</v>
+        <v>19282</v>
       </c>
       <c r="E254">
-        <v>16336</v>
+        <v>16338</v>
       </c>
       <c r="F254">
         <v>16166</v>
       </c>
       <c r="G254">
-        <v>16509</v>
+        <v>16530</v>
       </c>
       <c r="H254">
         <v>0.88</v>
@@ -10918,19 +10922,19 @@
         <v>44145</v>
       </c>
       <c r="B255">
-        <v>18438</v>
+        <v>18431</v>
       </c>
       <c r="C255">
-        <v>18223</v>
+        <v>18229</v>
       </c>
       <c r="D255">
-        <v>18646</v>
+        <v>18606</v>
       </c>
       <c r="E255">
-        <v>16919</v>
+        <v>16915</v>
       </c>
       <c r="F255">
-        <v>16736</v>
+        <v>16731</v>
       </c>
       <c r="G255">
         <v>17103</v>
@@ -10959,28 +10963,28 @@
         <v>44146</v>
       </c>
       <c r="B256">
-        <v>17905</v>
+        <v>17922</v>
       </c>
       <c r="C256">
-        <v>17718</v>
+        <v>17725</v>
       </c>
       <c r="D256">
-        <v>18090</v>
+        <v>18099</v>
       </c>
       <c r="E256">
-        <v>17631</v>
+        <v>17633</v>
       </c>
       <c r="F256">
-        <v>17443</v>
+        <v>17437</v>
       </c>
       <c r="G256">
-        <v>17819</v>
+        <v>17827</v>
       </c>
       <c r="H256">
         <v>1.07</v>
       </c>
       <c r="I256">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="J256">
         <v>1.08</v>
@@ -11000,22 +11004,22 @@
         <v>44147</v>
       </c>
       <c r="B257">
-        <v>17647</v>
+        <v>17651</v>
       </c>
       <c r="C257">
-        <v>17469</v>
+        <v>17473</v>
       </c>
       <c r="D257">
-        <v>17815</v>
+        <v>17848</v>
       </c>
       <c r="E257">
-        <v>18257</v>
+        <v>18261</v>
       </c>
       <c r="F257">
-        <v>18067</v>
+        <v>18070</v>
       </c>
       <c r="G257">
-        <v>18443</v>
+        <v>18459</v>
       </c>
       <c r="H257">
         <v>1.1599999999999999</v>
@@ -11041,22 +11045,22 @@
         <v>44148</v>
       </c>
       <c r="B258">
-        <v>18352</v>
+        <v>18350</v>
       </c>
       <c r="C258">
-        <v>18192</v>
+        <v>18178</v>
       </c>
       <c r="D258">
-        <v>18530</v>
+        <v>18539</v>
       </c>
       <c r="E258">
-        <v>18085</v>
+        <v>18089</v>
       </c>
       <c r="F258">
-        <v>17900</v>
+        <v>17901</v>
       </c>
       <c r="G258">
-        <v>18270</v>
+        <v>18273</v>
       </c>
       <c r="H258">
         <v>1.1100000000000001</v>
@@ -11065,7 +11069,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J258">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="K258">
         <v>1.04</v>
@@ -11082,22 +11086,22 @@
         <v>44149</v>
       </c>
       <c r="B259">
-        <v>16320</v>
+        <v>16316</v>
       </c>
       <c r="C259">
-        <v>16107</v>
+        <v>16162</v>
       </c>
       <c r="D259">
-        <v>16497</v>
+        <v>16501</v>
       </c>
       <c r="E259">
-        <v>17556</v>
+        <v>17560</v>
       </c>
       <c r="F259">
-        <v>17371</v>
+        <v>17384</v>
       </c>
       <c r="G259">
-        <v>17733</v>
+        <v>17746</v>
       </c>
       <c r="H259">
         <v>1.04</v>
@@ -11106,7 +11110,7 @@
         <v>1.03</v>
       </c>
       <c r="J259">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
       <c r="K259">
         <v>1.05</v>
@@ -11123,22 +11127,22 @@
         <v>44150</v>
       </c>
       <c r="B260">
-        <v>16481</v>
+        <v>16488</v>
       </c>
       <c r="C260">
-        <v>16315</v>
+        <v>16319</v>
       </c>
       <c r="D260">
-        <v>16684</v>
+        <v>16672</v>
       </c>
       <c r="E260">
-        <v>17200</v>
+        <v>17201</v>
       </c>
       <c r="F260">
-        <v>17020</v>
+        <v>17033</v>
       </c>
       <c r="G260">
-        <v>17381</v>
+        <v>17390</v>
       </c>
       <c r="H260">
         <v>0.98</v>
@@ -11164,22 +11168,22 @@
         <v>44151</v>
       </c>
       <c r="B261">
-        <v>20482</v>
+        <v>20459</v>
       </c>
       <c r="C261">
-        <v>20261</v>
+        <v>20268</v>
       </c>
       <c r="D261">
-        <v>20659</v>
+        <v>20646</v>
       </c>
       <c r="E261">
-        <v>17909</v>
+        <v>17903</v>
       </c>
       <c r="F261">
-        <v>17718</v>
+        <v>17732</v>
       </c>
       <c r="G261">
-        <v>18092</v>
+        <v>18089</v>
       </c>
       <c r="H261">
         <v>0.98</v>
@@ -11205,25 +11209,25 @@
         <v>44152</v>
       </c>
       <c r="B262">
-        <v>19445</v>
+        <v>19440</v>
       </c>
       <c r="C262">
-        <v>19259</v>
+        <v>19214</v>
       </c>
       <c r="D262">
-        <v>19615</v>
+        <v>19603</v>
       </c>
       <c r="E262">
-        <v>18182</v>
+        <v>18176</v>
       </c>
       <c r="F262">
-        <v>17985</v>
+        <v>17991</v>
       </c>
       <c r="G262">
-        <v>18364</v>
+        <v>18355</v>
       </c>
       <c r="H262">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="I262">
         <v>1</v>
@@ -11246,22 +11250,22 @@
         <v>44153</v>
       </c>
       <c r="B263">
-        <v>18608</v>
+        <v>18606</v>
       </c>
       <c r="C263">
-        <v>18441</v>
+        <v>18423</v>
       </c>
       <c r="D263">
-        <v>18813</v>
+        <v>18811</v>
       </c>
       <c r="E263">
-        <v>18754</v>
+        <v>18748</v>
       </c>
       <c r="F263">
-        <v>18569</v>
+        <v>18556</v>
       </c>
       <c r="G263">
-        <v>18943</v>
+        <v>18933</v>
       </c>
       <c r="H263">
         <v>1.07</v>
@@ -11287,22 +11291,22 @@
         <v>44154</v>
       </c>
       <c r="B264">
-        <v>17287</v>
+        <v>17282</v>
       </c>
       <c r="C264">
-        <v>17107</v>
+        <v>17092</v>
       </c>
       <c r="D264">
-        <v>17483</v>
+        <v>17484</v>
       </c>
       <c r="E264">
-        <v>18955</v>
+        <v>18947</v>
       </c>
       <c r="F264">
-        <v>18767</v>
+        <v>18749</v>
       </c>
       <c r="G264">
-        <v>19142</v>
+        <v>19136</v>
       </c>
       <c r="H264">
         <v>1.1000000000000001</v>
@@ -11328,22 +11332,22 @@
         <v>44155</v>
       </c>
       <c r="B265">
-        <v>16799</v>
+        <v>16801</v>
       </c>
       <c r="C265">
-        <v>16614</v>
+        <v>16637</v>
       </c>
       <c r="D265">
-        <v>16988</v>
+        <v>16994</v>
       </c>
       <c r="E265">
-        <v>18035</v>
+        <v>18032</v>
       </c>
       <c r="F265">
-        <v>17855</v>
+        <v>17841</v>
       </c>
       <c r="G265">
-        <v>18225</v>
+        <v>18223</v>
       </c>
       <c r="H265">
         <v>1.01</v>
@@ -11369,22 +11373,22 @@
         <v>44156</v>
       </c>
       <c r="B266">
-        <v>14469</v>
+        <v>14472</v>
       </c>
       <c r="C266">
-        <v>14289</v>
+        <v>14288</v>
       </c>
       <c r="D266">
-        <v>14648</v>
+        <v>14632</v>
       </c>
       <c r="E266">
-        <v>16791</v>
+        <v>16790</v>
       </c>
       <c r="F266">
-        <v>16612</v>
+        <v>16610</v>
       </c>
       <c r="G266">
-        <v>16983</v>
+        <v>16980</v>
       </c>
       <c r="H266">
         <v>0.92</v>
@@ -11410,28 +11414,28 @@
         <v>44157</v>
       </c>
       <c r="B267">
-        <v>14531</v>
+        <v>14526</v>
       </c>
       <c r="C267">
-        <v>14398</v>
+        <v>14334</v>
       </c>
       <c r="D267">
-        <v>14737</v>
+        <v>14724</v>
       </c>
       <c r="E267">
-        <v>15771</v>
+        <v>15770</v>
       </c>
       <c r="F267">
-        <v>15602</v>
+        <v>15588</v>
       </c>
       <c r="G267">
-        <v>15964</v>
+        <v>15958</v>
       </c>
       <c r="H267">
         <v>0.84</v>
       </c>
       <c r="I267">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="J267">
         <v>0.85</v>
@@ -11451,22 +11455,22 @@
         <v>44158</v>
       </c>
       <c r="B268">
-        <v>18507</v>
+        <v>18502</v>
       </c>
       <c r="C268">
-        <v>18320</v>
+        <v>18335</v>
       </c>
       <c r="D268">
-        <v>18684</v>
+        <v>18667</v>
       </c>
       <c r="E268">
-        <v>16077</v>
+        <v>16075</v>
       </c>
       <c r="F268">
-        <v>15905</v>
+        <v>15898</v>
       </c>
       <c r="G268">
-        <v>16264</v>
+        <v>16254</v>
       </c>
       <c r="H268">
         <v>0.85</v>
@@ -11475,13 +11479,13 @@
         <v>0.84</v>
       </c>
       <c r="J268">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
       <c r="K268">
         <v>0.94</v>
       </c>
       <c r="L268">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="M268">
         <v>0.94</v>
@@ -11492,28 +11496,28 @@
         <v>44159</v>
       </c>
       <c r="B269">
-        <v>17480</v>
+        <v>17487</v>
       </c>
       <c r="C269">
-        <v>17331</v>
+        <v>17319</v>
       </c>
       <c r="D269">
-        <v>17685</v>
+        <v>17646</v>
       </c>
       <c r="E269">
         <v>16247</v>
       </c>
       <c r="F269">
-        <v>16084</v>
+        <v>16069</v>
       </c>
       <c r="G269">
-        <v>16438</v>
+        <v>16417</v>
       </c>
       <c r="H269">
         <v>0.9</v>
       </c>
       <c r="I269">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="J269">
         <v>0.91</v>
@@ -11533,22 +11537,22 @@
         <v>44160</v>
       </c>
       <c r="B270">
-        <v>16979</v>
+        <v>16967</v>
       </c>
       <c r="C270">
-        <v>16788</v>
+        <v>16810</v>
       </c>
       <c r="D270">
-        <v>17179</v>
+        <v>17148</v>
       </c>
       <c r="E270">
-        <v>16874</v>
+        <v>16871</v>
       </c>
       <c r="F270">
-        <v>16709</v>
+        <v>16699</v>
       </c>
       <c r="G270">
-        <v>17071</v>
+        <v>17046</v>
       </c>
       <c r="H270">
         <v>1</v>
@@ -11574,22 +11578,22 @@
         <v>44161</v>
       </c>
       <c r="B271">
-        <v>16100</v>
+        <v>16080</v>
       </c>
       <c r="C271">
-        <v>15905</v>
+        <v>15896</v>
       </c>
       <c r="D271">
-        <v>16309</v>
+        <v>16254</v>
       </c>
       <c r="E271">
-        <v>17266</v>
+        <v>17259</v>
       </c>
       <c r="F271">
-        <v>17086</v>
+        <v>17090</v>
       </c>
       <c r="G271">
-        <v>17464</v>
+        <v>17429</v>
       </c>
       <c r="H271">
         <v>1.0900000000000001</v>
@@ -11615,22 +11619,22 @@
         <v>44162</v>
       </c>
       <c r="B272">
-        <v>16514</v>
+        <v>16515</v>
       </c>
       <c r="C272">
-        <v>16352</v>
+        <v>16332</v>
       </c>
       <c r="D272">
-        <v>16681</v>
+        <v>16680</v>
       </c>
       <c r="E272">
-        <v>16768</v>
+        <v>16762</v>
       </c>
       <c r="F272">
-        <v>16594</v>
+        <v>16589</v>
       </c>
       <c r="G272">
-        <v>16963</v>
+        <v>16932</v>
       </c>
       <c r="H272">
         <v>1.04</v>
@@ -11656,34 +11660,34 @@
         <v>44163</v>
       </c>
       <c r="B273">
-        <v>15602</v>
+        <v>15591</v>
       </c>
       <c r="C273">
-        <v>15414</v>
+        <v>15448</v>
       </c>
       <c r="D273">
-        <v>15786</v>
+        <v>15776</v>
       </c>
       <c r="E273">
-        <v>16299</v>
+        <v>16288</v>
       </c>
       <c r="F273">
-        <v>16115</v>
+        <v>16122</v>
       </c>
       <c r="G273">
-        <v>16489</v>
+        <v>16464</v>
       </c>
       <c r="H273">
         <v>1</v>
       </c>
       <c r="I273">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="J273">
         <v>1.01</v>
       </c>
       <c r="K273">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="L273">
         <v>1</v>
@@ -11697,22 +11701,22 @@
         <v>44164</v>
       </c>
       <c r="B274">
-        <v>15479</v>
+        <v>15471</v>
       </c>
       <c r="C274">
-        <v>15305</v>
+        <v>15281</v>
       </c>
       <c r="D274">
-        <v>15645</v>
+        <v>15649</v>
       </c>
       <c r="E274">
-        <v>15924</v>
+        <v>15914</v>
       </c>
       <c r="F274">
-        <v>15744</v>
+        <v>15739</v>
       </c>
       <c r="G274">
-        <v>16105</v>
+        <v>16090</v>
       </c>
       <c r="H274">
         <v>0.94</v>
@@ -11738,22 +11742,22 @@
         <v>44165</v>
       </c>
       <c r="B275">
-        <v>20888</v>
+        <v>20875</v>
       </c>
       <c r="C275">
-        <v>20661</v>
+        <v>20686</v>
       </c>
       <c r="D275">
-        <v>21090</v>
+        <v>21063</v>
       </c>
       <c r="E275">
-        <v>17121</v>
+        <v>17113</v>
       </c>
       <c r="F275">
-        <v>16933</v>
+        <v>16937</v>
       </c>
       <c r="G275">
-        <v>17301</v>
+        <v>17292</v>
       </c>
       <c r="H275">
         <v>0.99</v>
@@ -11779,22 +11783,22 @@
         <v>44166</v>
       </c>
       <c r="B276">
-        <v>20893</v>
+        <v>20885</v>
       </c>
       <c r="C276">
-        <v>20558</v>
+        <v>20694</v>
       </c>
       <c r="D276">
-        <v>21267</v>
+        <v>21090</v>
       </c>
       <c r="E276">
-        <v>18216</v>
+        <v>18205</v>
       </c>
       <c r="F276">
-        <v>17984</v>
+        <v>18027</v>
       </c>
       <c r="G276">
-        <v>18447</v>
+        <v>18395</v>
       </c>
       <c r="H276">
         <v>1.0900000000000001</v>
@@ -11803,7 +11807,7 @@
         <v>1.08</v>
       </c>
       <c r="J276">
-        <v>1.1000000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="K276">
         <v>1.0900000000000001</v>
@@ -11820,28 +11824,28 @@
         <v>44167</v>
       </c>
       <c r="B277">
-        <v>20741</v>
+        <v>20734</v>
       </c>
       <c r="C277">
-        <v>20351</v>
+        <v>20525</v>
       </c>
       <c r="D277">
-        <v>21088</v>
+        <v>20956</v>
       </c>
       <c r="E277">
-        <v>19500</v>
+        <v>19491</v>
       </c>
       <c r="F277">
-        <v>19219</v>
+        <v>19296</v>
       </c>
       <c r="G277">
-        <v>19773</v>
+        <v>19690</v>
       </c>
       <c r="H277">
         <v>1.2</v>
       </c>
       <c r="I277">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="J277">
         <v>1.21</v>
@@ -11861,22 +11865,22 @@
         <v>44168</v>
       </c>
       <c r="B278">
-        <v>21126</v>
+        <v>21065</v>
       </c>
       <c r="C278">
-        <v>20638</v>
+        <v>20728</v>
       </c>
       <c r="D278">
-        <v>21556</v>
+        <v>21429</v>
       </c>
       <c r="E278">
-        <v>20912</v>
+        <v>20890</v>
       </c>
       <c r="F278">
-        <v>20552</v>
+        <v>20658</v>
       </c>
       <c r="G278">
-        <v>21250</v>
+        <v>21135</v>
       </c>
       <c r="H278">
         <v>1.31</v>
@@ -11885,7 +11889,7 @@
         <v>1.3</v>
       </c>
       <c r="J278">
-        <v>1.33</v>
+        <v>1.32</v>
       </c>
       <c r="K278">
         <v>1.1499999999999999</v>
@@ -11902,22 +11906,22 @@
         <v>44169</v>
       </c>
       <c r="B279">
-        <v>21756</v>
+        <v>21728</v>
       </c>
       <c r="C279">
-        <v>21360</v>
+        <v>21309</v>
       </c>
       <c r="D279">
-        <v>22214</v>
+        <v>22063</v>
       </c>
       <c r="E279">
-        <v>21129</v>
+        <v>21103</v>
       </c>
       <c r="F279">
-        <v>20727</v>
+        <v>20814</v>
       </c>
       <c r="G279">
-        <v>21531</v>
+        <v>21385</v>
       </c>
       <c r="H279">
         <v>1.23</v>
@@ -11926,7 +11930,7 @@
         <v>1.22</v>
       </c>
       <c r="J279">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="K279">
         <v>1.1599999999999999</v>
@@ -11943,22 +11947,22 @@
         <v>44170</v>
       </c>
       <c r="B280">
-        <v>20775</v>
+        <v>20734</v>
       </c>
       <c r="C280">
-        <v>20394</v>
+        <v>20254</v>
       </c>
       <c r="D280">
-        <v>21126</v>
+        <v>21247</v>
       </c>
       <c r="E280">
-        <v>21099</v>
+        <v>21065</v>
       </c>
       <c r="F280">
-        <v>20686</v>
+        <v>20704</v>
       </c>
       <c r="G280">
-        <v>21496</v>
+        <v>21424</v>
       </c>
       <c r="H280">
         <v>1.1599999999999999</v>
@@ -11976,7 +11980,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="M280">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="281" spans="1:13">
@@ -11984,22 +11988,22 @@
         <v>44171</v>
       </c>
       <c r="B281">
-        <v>21126</v>
+        <v>21085</v>
       </c>
       <c r="C281">
-        <v>20615</v>
+        <v>20684</v>
       </c>
       <c r="D281">
-        <v>21696</v>
+        <v>21423</v>
       </c>
       <c r="E281">
-        <v>21196</v>
+        <v>21153</v>
       </c>
       <c r="F281">
-        <v>20752</v>
+        <v>20744</v>
       </c>
       <c r="G281">
-        <v>21648</v>
+        <v>21541</v>
       </c>
       <c r="H281">
         <v>1.0900000000000001</v>
@@ -12014,7 +12018,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="L281">
-        <v>1.1599999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="M281">
         <v>1.17</v>
@@ -12025,22 +12029,22 @@
         <v>44172</v>
       </c>
       <c r="B282">
-        <v>26221</v>
+        <v>26218</v>
       </c>
       <c r="C282">
-        <v>25420</v>
+        <v>25737</v>
       </c>
       <c r="D282">
-        <v>27034</v>
+        <v>26670</v>
       </c>
       <c r="E282">
-        <v>22469</v>
+        <v>22441</v>
       </c>
       <c r="F282">
-        <v>21947</v>
+        <v>21996</v>
       </c>
       <c r="G282">
-        <v>23017</v>
+        <v>22851</v>
       </c>
       <c r="H282">
         <v>1.07</v>
@@ -12058,7 +12062,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="M282">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="283" spans="1:13">
@@ -12066,22 +12070,22 @@
         <v>44173</v>
       </c>
       <c r="B283">
-        <v>26102</v>
+        <v>26018</v>
       </c>
       <c r="C283">
-        <v>25321</v>
+        <v>25385</v>
       </c>
       <c r="D283">
-        <v>26905</v>
+        <v>26715</v>
       </c>
       <c r="E283">
-        <v>23556</v>
+        <v>23514</v>
       </c>
       <c r="F283">
-        <v>22938</v>
+        <v>23015</v>
       </c>
       <c r="G283">
-        <v>24190</v>
+        <v>24014</v>
       </c>
       <c r="H283">
         <v>1.1100000000000001</v>
@@ -12093,13 +12097,13 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="K283">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="L283">
         <v>1.1399999999999999</v>
       </c>
       <c r="M283">
-        <v>1.1599999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="284" spans="1:13">
@@ -12107,22 +12111,22 @@
         <v>44174</v>
       </c>
       <c r="B284">
-        <v>25218</v>
+        <v>25048</v>
       </c>
       <c r="C284">
-        <v>24360</v>
+        <v>24335</v>
       </c>
       <c r="D284">
-        <v>26114</v>
+        <v>25887</v>
       </c>
       <c r="E284">
-        <v>24667</v>
+        <v>24592</v>
       </c>
       <c r="F284">
-        <v>23929</v>
+        <v>24035</v>
       </c>
       <c r="G284">
-        <v>25437</v>
+        <v>25174</v>
       </c>
       <c r="H284">
         <v>1.17</v>
@@ -12131,16 +12135,16 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="J284">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="K284">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L284">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="M284">
         <v>1.1299999999999999</v>
-      </c>
-      <c r="L284">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="M284">
-        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="285" spans="1:13">
@@ -12148,40 +12152,40 @@
         <v>44175</v>
       </c>
       <c r="B285">
-        <v>24602</v>
+        <v>24630</v>
       </c>
       <c r="C285">
-        <v>23815</v>
+        <v>23765</v>
       </c>
       <c r="D285">
-        <v>25424</v>
+        <v>25338</v>
       </c>
       <c r="E285">
-        <v>25536</v>
+        <v>25478</v>
       </c>
       <c r="F285">
-        <v>24729</v>
+        <v>24805</v>
       </c>
       <c r="G285">
-        <v>26369</v>
+        <v>26152</v>
       </c>
       <c r="H285">
         <v>1.2</v>
       </c>
       <c r="I285">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="J285">
-        <v>1.23</v>
+        <v>1.22</v>
       </c>
       <c r="K285">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L285">
         <v>1.0900000000000001</v>
       </c>
       <c r="M285">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
     </row>
     <row r="286" spans="1:13">
@@ -12189,22 +12193,22 @@
         <v>44176</v>
       </c>
       <c r="B286">
-        <v>24785</v>
+        <v>24618</v>
       </c>
       <c r="C286">
-        <v>24022</v>
+        <v>23859</v>
       </c>
       <c r="D286">
-        <v>25961</v>
+        <v>25316</v>
       </c>
       <c r="E286">
-        <v>25177</v>
+        <v>25078</v>
       </c>
       <c r="F286">
-        <v>24379</v>
+        <v>24336</v>
       </c>
       <c r="G286">
-        <v>26101</v>
+        <v>25814</v>
       </c>
       <c r="H286">
         <v>1.1200000000000001</v>
@@ -12216,13 +12220,13 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="K286">
-        <v>1.0900000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="L286">
         <v>1.07</v>
       </c>
       <c r="M286">
-        <v>1.1000000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="287" spans="1:13">
@@ -12230,28 +12234,28 @@
         <v>44177</v>
       </c>
       <c r="B287">
-        <v>23241</v>
+        <v>23141</v>
       </c>
       <c r="C287">
-        <v>22300</v>
+        <v>22413</v>
       </c>
       <c r="D287">
-        <v>24137</v>
+        <v>24035</v>
       </c>
       <c r="E287">
-        <v>24462</v>
+        <v>24359</v>
       </c>
       <c r="F287">
-        <v>23624</v>
+        <v>23593</v>
       </c>
       <c r="G287">
-        <v>25409</v>
+        <v>25144</v>
       </c>
       <c r="H287">
         <v>1.04</v>
       </c>
       <c r="I287">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="J287">
         <v>1.06</v>
@@ -12263,7 +12267,7 @@
         <v>1.05</v>
       </c>
       <c r="M287">
-        <v>1.08</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="288" spans="1:13">
@@ -12271,25 +12275,25 @@
         <v>44178</v>
       </c>
       <c r="B288">
-        <v>22635</v>
+        <v>22507</v>
       </c>
       <c r="C288">
-        <v>21634</v>
+        <v>21851</v>
       </c>
       <c r="D288">
-        <v>23635</v>
+        <v>23140</v>
       </c>
       <c r="E288">
-        <v>23816</v>
+        <v>23724</v>
       </c>
       <c r="F288">
-        <v>22943</v>
+        <v>22972</v>
       </c>
       <c r="G288">
-        <v>24789</v>
+        <v>24457</v>
       </c>
       <c r="H288">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="I288">
         <v>0.94</v>
@@ -12312,25 +12316,25 @@
         <v>44179</v>
       </c>
       <c r="B289">
-        <v>28270</v>
+        <v>28057</v>
       </c>
       <c r="C289">
-        <v>26764</v>
+        <v>26750</v>
       </c>
       <c r="D289">
-        <v>29660</v>
+        <v>29207</v>
       </c>
       <c r="E289">
-        <v>24733</v>
+        <v>24581</v>
       </c>
       <c r="F289">
-        <v>23680</v>
+        <v>23718</v>
       </c>
       <c r="G289">
-        <v>25848</v>
+        <v>25424</v>
       </c>
       <c r="H289">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="I289">
         <v>0.94</v>
@@ -12342,10 +12346,10 @@
         <v>1.04</v>
       </c>
       <c r="L289">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="M289">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="290" spans="1:13">
@@ -12353,28 +12357,28 @@
         <v>44180</v>
       </c>
       <c r="B290">
-        <v>26939</v>
+        <v>26794</v>
       </c>
       <c r="C290">
-        <v>25795</v>
+        <v>25707</v>
       </c>
       <c r="D290">
-        <v>28250</v>
+        <v>27651</v>
       </c>
       <c r="E290">
-        <v>25271</v>
+        <v>25125</v>
       </c>
       <c r="F290">
-        <v>24123</v>
+        <v>24180</v>
       </c>
       <c r="G290">
-        <v>26421</v>
+        <v>26008</v>
       </c>
       <c r="H290">
         <v>1</v>
       </c>
       <c r="I290">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="J290">
         <v>1.03</v>
@@ -12386,7 +12390,7 @@
         <v>1.01</v>
       </c>
       <c r="M290">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="291" spans="1:13">
@@ -12394,22 +12398,22 @@
         <v>44181</v>
       </c>
       <c r="B291">
-        <v>25644</v>
+        <v>25541</v>
       </c>
       <c r="C291">
-        <v>24219</v>
+        <v>24355</v>
       </c>
       <c r="D291">
-        <v>27158</v>
+        <v>26651</v>
       </c>
       <c r="E291">
-        <v>25872</v>
+        <v>25725</v>
       </c>
       <c r="F291">
-        <v>24603</v>
+        <v>24666</v>
       </c>
       <c r="G291">
-        <v>27176</v>
+        <v>26662</v>
       </c>
       <c r="H291">
         <v>1.06</v>
@@ -12418,16 +12422,16 @@
         <v>1.03</v>
       </c>
       <c r="J291">
-        <v>1.1000000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="K291">
         <v>1.01</v>
       </c>
       <c r="L291">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="M291">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="292" spans="1:13">
@@ -12435,37 +12439,37 @@
         <v>44182</v>
       </c>
       <c r="B292">
-        <v>23562</v>
+        <v>23572</v>
       </c>
       <c r="C292">
-        <v>21987</v>
+        <v>22304</v>
       </c>
       <c r="D292">
-        <v>24939</v>
+        <v>24820</v>
       </c>
       <c r="E292">
-        <v>26104</v>
+        <v>25991</v>
       </c>
       <c r="F292">
-        <v>24691</v>
+        <v>24779</v>
       </c>
       <c r="G292">
-        <v>27502</v>
+        <v>27082</v>
       </c>
       <c r="H292">
         <v>1.1000000000000001</v>
       </c>
       <c r="I292">
-        <v>1.06</v>
+        <v>1.07</v>
       </c>
       <c r="J292">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="K292">
         <v>0.99</v>
       </c>
       <c r="L292">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="M292">
         <v>1.01</v>
@@ -12476,22 +12480,22 @@
         <v>44183</v>
       </c>
       <c r="B293">
-        <v>23045</v>
+        <v>22765</v>
       </c>
       <c r="C293">
-        <v>21667</v>
+        <v>21035</v>
       </c>
       <c r="D293">
-        <v>24706</v>
+        <v>23949</v>
       </c>
       <c r="E293">
-        <v>24797</v>
+        <v>24668</v>
       </c>
       <c r="F293">
-        <v>23417</v>
+        <v>23350</v>
       </c>
       <c r="G293">
-        <v>26263</v>
+        <v>25768</v>
       </c>
       <c r="H293">
         <v>1</v>
@@ -12500,7 +12504,7 @@
         <v>0.97</v>
       </c>
       <c r="J293">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="K293">
         <v>0.97</v>
@@ -12509,7 +12513,7 @@
         <v>0.96</v>
       </c>
       <c r="M293">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="294" spans="1:13">
@@ -12517,37 +12521,37 @@
         <v>44184</v>
       </c>
       <c r="B294">
-        <v>21009</v>
+        <v>20877</v>
       </c>
       <c r="C294">
-        <v>19654</v>
+        <v>19679</v>
       </c>
       <c r="D294">
-        <v>22412</v>
+        <v>22315</v>
       </c>
       <c r="E294">
-        <v>23315</v>
+        <v>23189</v>
       </c>
       <c r="F294">
-        <v>21881</v>
+        <v>21843</v>
       </c>
       <c r="G294">
-        <v>24804</v>
+        <v>24434</v>
       </c>
       <c r="H294">
         <v>0.92</v>
       </c>
       <c r="I294">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="J294">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="K294">
         <v>0.96</v>
       </c>
       <c r="L294">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="M294">
         <v>0.98</v>
@@ -12558,40 +12562,40 @@
         <v>44185</v>
       </c>
       <c r="B295">
-        <v>19807</v>
+        <v>20070</v>
       </c>
       <c r="C295">
-        <v>17941</v>
+        <v>18729</v>
       </c>
       <c r="D295">
-        <v>21653</v>
+        <v>21497</v>
       </c>
       <c r="E295">
-        <v>21856</v>
+        <v>21821</v>
       </c>
       <c r="F295">
-        <v>20312</v>
+        <v>20437</v>
       </c>
       <c r="G295">
-        <v>23428</v>
+        <v>23145</v>
       </c>
       <c r="H295">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="I295">
-        <v>0.8</v>
+        <v>0.82</v>
       </c>
       <c r="J295">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="K295">
         <v>0.93</v>
       </c>
       <c r="L295">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="M295">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="296" spans="1:13">
@@ -12599,22 +12603,22 @@
         <v>44186</v>
       </c>
       <c r="B296">
-        <v>22734</v>
+        <v>22585</v>
       </c>
       <c r="C296">
-        <v>20564</v>
+        <v>20777</v>
       </c>
       <c r="D296">
-        <v>25004</v>
+        <v>24003</v>
       </c>
       <c r="E296">
-        <v>21649</v>
+        <v>21574</v>
       </c>
       <c r="F296">
-        <v>19956</v>
+        <v>20055</v>
       </c>
       <c r="G296">
-        <v>23444</v>
+        <v>22941</v>
       </c>
       <c r="H296">
         <v>0.83</v>
@@ -12623,13 +12627,13 @@
         <v>0.79</v>
       </c>
       <c r="J296">
-        <v>0.88</v>
+        <v>0.86</v>
       </c>
       <c r="K296">
         <v>0.9</v>
       </c>
       <c r="L296">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="M296">
         <v>0.93</v>
@@ -12640,37 +12644,37 @@
         <v>44187</v>
       </c>
       <c r="B297">
-        <v>19827</v>
+        <v>20185</v>
       </c>
       <c r="C297">
-        <v>17743</v>
+        <v>18269</v>
       </c>
       <c r="D297">
-        <v>22542</v>
+        <v>22118</v>
       </c>
       <c r="E297">
-        <v>20844</v>
+        <v>20929</v>
       </c>
       <c r="F297">
-        <v>18975</v>
+        <v>19363</v>
       </c>
       <c r="G297">
-        <v>22903</v>
+        <v>22483</v>
       </c>
       <c r="H297">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="I297">
-        <v>0.79</v>
+        <v>0.81</v>
       </c>
       <c r="J297">
         <v>0.88</v>
       </c>
       <c r="K297">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
       <c r="L297">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
       <c r="M297">
         <v>0.89</v>
@@ -12681,40 +12685,40 @@
         <v>44188</v>
       </c>
       <c r="B298">
-        <v>16555</v>
+        <v>17570</v>
       </c>
       <c r="C298">
-        <v>14113</v>
+        <v>15663</v>
       </c>
       <c r="D298">
-        <v>19609</v>
+        <v>19498</v>
       </c>
       <c r="E298">
-        <v>19731</v>
+        <v>20102</v>
       </c>
       <c r="F298">
-        <v>17590</v>
+        <v>18360</v>
       </c>
       <c r="G298">
-        <v>22202</v>
+        <v>21779</v>
       </c>
       <c r="H298">
-        <v>0.85</v>
+        <v>0.87</v>
       </c>
       <c r="I298">
-        <v>0.79</v>
+        <v>0.82</v>
       </c>
       <c r="J298">
         <v>0.91</v>
       </c>
       <c r="K298">
+        <v>0.83</v>
+      </c>
+      <c r="L298">
         <v>0.81</v>
       </c>
-      <c r="L298">
-        <v>0.78</v>
-      </c>
       <c r="M298">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="299" spans="1:13">
@@ -12722,40 +12726,40 @@
         <v>44189</v>
       </c>
       <c r="B299">
-        <v>13682</v>
+        <v>15150</v>
       </c>
       <c r="C299">
-        <v>10673</v>
+        <v>13521</v>
       </c>
       <c r="D299">
-        <v>17235</v>
+        <v>16911</v>
       </c>
       <c r="E299">
-        <v>18199</v>
+        <v>18872</v>
       </c>
       <c r="F299">
-        <v>15773</v>
+        <v>17058</v>
       </c>
       <c r="G299">
-        <v>21097</v>
+        <v>20632</v>
       </c>
       <c r="H299">
-        <v>0.83</v>
+        <v>0.87</v>
       </c>
       <c r="I299">
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
       <c r="J299">
         <v>0.91</v>
       </c>
       <c r="K299">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="L299">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="M299">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="300" spans="1:13">
@@ -12763,234 +12767,309 @@
         <v>44190</v>
       </c>
       <c r="B300">
-        <v>12026</v>
+        <v>13879</v>
       </c>
       <c r="C300">
-        <v>8604</v>
+        <v>11028</v>
       </c>
       <c r="D300">
-        <v>14874</v>
+        <v>16152</v>
       </c>
       <c r="E300">
-        <v>15522</v>
+        <v>16696</v>
       </c>
       <c r="F300">
-        <v>12783</v>
+        <v>14620</v>
       </c>
       <c r="G300">
-        <v>18565</v>
+        <v>18670</v>
       </c>
       <c r="H300">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="I300">
-        <v>0.65</v>
+        <v>0.71</v>
       </c>
       <c r="J300">
+        <v>0.84</v>
+      </c>
+      <c r="K300">
         <v>0.8</v>
       </c>
-      <c r="K300">
-        <v>0.76</v>
-      </c>
       <c r="L300">
-        <v>0.72</v>
+        <v>0.77</v>
       </c>
       <c r="M300">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13">
+      <c r="A301" s="4">
+        <v>44191</v>
+      </c>
+      <c r="B301">
+        <v>15495</v>
+      </c>
+      <c r="C301">
+        <v>12043</v>
+      </c>
+      <c r="D301">
+        <v>18643</v>
+      </c>
+      <c r="E301">
+        <v>15523</v>
+      </c>
+      <c r="F301">
+        <v>13064</v>
+      </c>
+      <c r="G301">
+        <v>17801</v>
+      </c>
+      <c r="H301">
+        <v>0.74</v>
+      </c>
+      <c r="I301">
+        <v>0.66</v>
+      </c>
+      <c r="J301">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="301" spans="1:13">
-      <c r="A301" s="3">
-        <v>44191</v>
-      </c>
-      <c r="B301">
-        <v>14402</v>
-      </c>
-      <c r="C301">
-        <v>9566</v>
-      </c>
-      <c r="D301">
-        <v>18805</v>
-      </c>
-      <c r="E301">
-        <v>14166</v>
-      </c>
-      <c r="F301">
-        <v>10739</v>
-      </c>
-      <c r="G301">
-        <v>17631</v>
-      </c>
-      <c r="H301">
+      <c r="K301">
+        <v>0.83</v>
+      </c>
+      <c r="L301">
+        <v>0.79</v>
+      </c>
+      <c r="M301">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13">
+      <c r="A302" s="4">
+        <v>44192</v>
+      </c>
+      <c r="B302">
+        <v>18095</v>
+      </c>
+      <c r="C302">
+        <v>13111</v>
+      </c>
+      <c r="D302">
+        <v>22209</v>
+      </c>
+      <c r="E302">
+        <v>15655</v>
+      </c>
+      <c r="F302">
+        <v>12426</v>
+      </c>
+      <c r="G302">
+        <v>18479</v>
+      </c>
+      <c r="H302">
+        <v>0.78</v>
+      </c>
+      <c r="I302">
         <v>0.68</v>
       </c>
-      <c r="I301">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="J301">
-        <v>0.77</v>
-      </c>
-      <c r="K301">
+      <c r="J302">
+        <v>0.87</v>
+      </c>
+      <c r="K302">
+        <v>0.89</v>
+      </c>
+      <c r="L302">
+        <v>0.81</v>
+      </c>
+      <c r="M302">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13">
+      <c r="A303" s="4">
+        <v>44193</v>
+      </c>
+      <c r="B303">
+        <v>23531</v>
+      </c>
+      <c r="C303">
+        <v>18459</v>
+      </c>
+      <c r="D303">
+        <v>29811</v>
+      </c>
+      <c r="E303">
+        <v>17750</v>
+      </c>
+      <c r="F303">
+        <v>13660</v>
+      </c>
+      <c r="G303">
+        <v>21703</v>
+      </c>
+      <c r="H303">
+        <v>0.94</v>
+      </c>
+      <c r="I303">
         <v>0.8</v>
       </c>
-      <c r="L301">
-        <v>0.73</v>
-      </c>
-      <c r="M301">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="302" spans="1:13">
-      <c r="A302" s="3">
-        <v>44192</v>
-      </c>
-      <c r="B302">
-        <v>17840</v>
-      </c>
-      <c r="C302">
-        <v>11509</v>
-      </c>
-      <c r="D302">
-        <v>23598</v>
-      </c>
-      <c r="E302">
-        <v>14487</v>
-      </c>
-      <c r="F302">
-        <v>10088</v>
-      </c>
-      <c r="G302">
-        <v>18628</v>
-      </c>
-      <c r="H302">
-        <v>0.74</v>
-      </c>
-      <c r="I302">
-        <v>0.61</v>
-      </c>
-      <c r="J302">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="303" spans="1:13">
-      <c r="A303" s="3"/>
+      <c r="J303">
+        <v>1.05</v>
+      </c>
+      <c r="K303">
+        <v>0.95</v>
+      </c>
+      <c r="L303">
+        <v>0.84</v>
+      </c>
+      <c r="M303">
+        <v>1.05</v>
+      </c>
     </row>
     <row r="304" spans="1:13">
-      <c r="A304" s="3"/>
+      <c r="A304" s="4">
+        <v>44194</v>
+      </c>
+      <c r="B304">
+        <v>19890</v>
+      </c>
+      <c r="C304">
+        <v>13210</v>
+      </c>
+      <c r="D304">
+        <v>27730</v>
+      </c>
+      <c r="E304">
+        <v>19253</v>
+      </c>
+      <c r="F304">
+        <v>14206</v>
+      </c>
+      <c r="G304">
+        <v>24598</v>
+      </c>
+      <c r="H304">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I304">
+        <v>0.96</v>
+      </c>
+      <c r="J304">
+        <v>1.38</v>
+      </c>
     </row>
     <row r="305" spans="1:1">
-      <c r="A305" s="3"/>
+      <c r="A305" s="4"/>
     </row>
     <row r="306" spans="1:1">
-      <c r="A306" s="3"/>
+      <c r="A306" s="4"/>
     </row>
     <row r="307" spans="1:1">
-      <c r="A307" s="3"/>
+      <c r="A307" s="4"/>
     </row>
     <row r="308" spans="1:1">
-      <c r="A308" s="3"/>
+      <c r="A308" s="4"/>
     </row>
     <row r="309" spans="1:1">
-      <c r="A309" s="3"/>
+      <c r="A309" s="4"/>
     </row>
     <row r="310" spans="1:1">
-      <c r="A310" s="3"/>
+      <c r="A310" s="4"/>
     </row>
     <row r="311" spans="1:1">
-      <c r="A311" s="3"/>
+      <c r="A311" s="4"/>
     </row>
     <row r="312" spans="1:1">
-      <c r="A312" s="3"/>
+      <c r="A312" s="4"/>
     </row>
     <row r="313" spans="1:1">
-      <c r="A313" s="3"/>
+      <c r="A313" s="4"/>
     </row>
     <row r="314" spans="1:1">
-      <c r="A314" s="3"/>
+      <c r="A314" s="4"/>
     </row>
     <row r="315" spans="1:1">
-      <c r="A315" s="3"/>
+      <c r="A315" s="4"/>
     </row>
     <row r="316" spans="1:1">
-      <c r="A316" s="3"/>
+      <c r="A316" s="4"/>
     </row>
     <row r="317" spans="1:1">
-      <c r="A317" s="3"/>
+      <c r="A317" s="4"/>
     </row>
     <row r="318" spans="1:1">
-      <c r="A318" s="3"/>
+      <c r="A318" s="4"/>
     </row>
     <row r="319" spans="1:1">
-      <c r="A319" s="3"/>
+      <c r="A319" s="4"/>
     </row>
     <row r="320" spans="1:1">
-      <c r="A320" s="3"/>
+      <c r="A320" s="4"/>
     </row>
     <row r="321" spans="1:1">
-      <c r="A321" s="3"/>
+      <c r="A321" s="4"/>
     </row>
     <row r="322" spans="1:1">
-      <c r="A322" s="3"/>
+      <c r="A322" s="4"/>
     </row>
     <row r="323" spans="1:1">
-      <c r="A323" s="3"/>
+      <c r="A323" s="4"/>
     </row>
     <row r="324" spans="1:1">
-      <c r="A324" s="3"/>
+      <c r="A324" s="4"/>
     </row>
     <row r="325" spans="1:1">
-      <c r="A325" s="3"/>
+      <c r="A325" s="4"/>
     </row>
     <row r="326" spans="1:1">
-      <c r="A326" s="3"/>
+      <c r="A326" s="4"/>
     </row>
     <row r="327" spans="1:1">
-      <c r="A327" s="3"/>
+      <c r="A327" s="4"/>
     </row>
     <row r="328" spans="1:1">
-      <c r="A328" s="3"/>
+      <c r="A328" s="4"/>
     </row>
     <row r="329" spans="1:1">
-      <c r="A329" s="3"/>
+      <c r="A329" s="4"/>
     </row>
     <row r="330" spans="1:1">
-      <c r="A330" s="3"/>
+      <c r="A330" s="4"/>
     </row>
     <row r="331" spans="1:1">
-      <c r="A331" s="3"/>
+      <c r="A331" s="4"/>
     </row>
     <row r="332" spans="1:1">
-      <c r="A332" s="3"/>
+      <c r="A332" s="4"/>
     </row>
     <row r="333" spans="1:1">
-      <c r="A333" s="3"/>
+      <c r="A333" s="4"/>
     </row>
     <row r="334" spans="1:1">
-      <c r="A334" s="3"/>
+      <c r="A334" s="4"/>
     </row>
     <row r="335" spans="1:1">
-      <c r="A335" s="3"/>
+      <c r="A335" s="4"/>
     </row>
     <row r="336" spans="1:1">
-      <c r="A336" s="3"/>
+      <c r="A336" s="4"/>
     </row>
     <row r="337" spans="1:1">
-      <c r="A337" s="3"/>
+      <c r="A337" s="4"/>
     </row>
     <row r="338" spans="1:1">
-      <c r="A338" s="3"/>
+      <c r="A338" s="4"/>
     </row>
     <row r="339" spans="1:1">
-      <c r="A339" s="3"/>
+      <c r="A339" s="4"/>
     </row>
     <row r="340" spans="1:1">
-      <c r="A340" s="3"/>
+      <c r="A340" s="4"/>
     </row>
     <row r="341" spans="1:1">
-      <c r="A341" s="3"/>
+      <c r="A341" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add RKI data downloaded 2021-01-04--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Nowcasting_Zahlen.xlsx
+++ b/rki-data/RKI-Nowcasting_Zahlen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-01-02\Nowcast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\3.7.Lageberichte\2021-01-03\Nowcast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87A9A508-C702-48DD-9C53-0F20F7B4F28F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92D76137-24E4-4D67-A551-F9449F96E6CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24420" windowHeight="11565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25410" windowHeight="11565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <t>Ergebnisse des Nowcastings und der Schätzung der Reproduktionszahl R</t>
   </si>
   <si>
-    <t>Datenstand: 02.01.2021, 00:00 Uhr</t>
+    <t>Datenstand: 03.01.2021, 00:00 Uhr</t>
   </si>
   <si>
     <t>Die Ergebnisse des Nowcastings, also die Schätzung der Anzahl von COVID-19 Neuerkrankungen wird dargestellt mit einem gleitenden 4-Tages-Mittelwert.</t>
@@ -41,7 +41,7 @@
     <t>Dabei wird jeder Wert mit den Werten der 3 vorhergehenden Tage gemittelt.</t>
   </si>
   <si>
-    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 02.01.2021 dargestellten Nowcasting-Kurve.</t>
+    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 03.01.2021 dargestellten Nowcasting-Kurve.</t>
   </si>
   <si>
     <t>Der letzte Schätzwert der Reproduktionszahl R wird ebenfalls im gleichen Lagebericht erwähnt.</t>
@@ -566,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -10433,10 +10433,10 @@
         <v>16811</v>
       </c>
       <c r="C243">
-        <v>16595</v>
+        <v>16594</v>
       </c>
       <c r="D243">
-        <v>16994</v>
+        <v>16992</v>
       </c>
       <c r="E243">
         <v>18130</v>
@@ -10474,10 +10474,10 @@
         <v>17247</v>
       </c>
       <c r="C244">
-        <v>17091</v>
+        <v>17094</v>
       </c>
       <c r="D244">
-        <v>17386</v>
+        <v>17387</v>
       </c>
       <c r="E244">
         <v>17641</v>
@@ -10512,22 +10512,22 @@
         <v>44135</v>
       </c>
       <c r="B245">
-        <v>15613</v>
+        <v>15614</v>
       </c>
       <c r="C245">
-        <v>15410</v>
+        <v>15413</v>
       </c>
       <c r="D245">
-        <v>15779</v>
+        <v>15776</v>
       </c>
       <c r="E245">
         <v>16940</v>
       </c>
       <c r="F245">
-        <v>16746</v>
+        <v>16747</v>
       </c>
       <c r="G245">
-        <v>17108</v>
+        <v>17107</v>
       </c>
       <c r="H245">
         <v>0.99</v>
@@ -10556,19 +10556,19 @@
         <v>16655</v>
       </c>
       <c r="C246">
-        <v>16493</v>
+        <v>16491</v>
       </c>
       <c r="D246">
-        <v>16837</v>
+        <v>16830</v>
       </c>
       <c r="E246">
         <v>16582</v>
       </c>
       <c r="F246">
-        <v>16397</v>
+        <v>16398</v>
       </c>
       <c r="G246">
-        <v>16749</v>
+        <v>16746</v>
       </c>
       <c r="H246">
         <v>0.93</v>
@@ -10594,22 +10594,22 @@
         <v>44137</v>
       </c>
       <c r="B247">
-        <v>20967</v>
+        <v>20970</v>
       </c>
       <c r="C247">
-        <v>20782</v>
+        <v>20787</v>
       </c>
       <c r="D247">
-        <v>21166</v>
+        <v>21168</v>
       </c>
       <c r="E247">
         <v>17621</v>
       </c>
       <c r="F247">
-        <v>17444</v>
+        <v>17446</v>
       </c>
       <c r="G247">
-        <v>17792</v>
+        <v>17790</v>
       </c>
       <c r="H247">
         <v>0.97</v>
@@ -10635,22 +10635,22 @@
         <v>44138</v>
       </c>
       <c r="B248">
-        <v>19018</v>
+        <v>19020</v>
       </c>
       <c r="C248">
-        <v>18842</v>
+        <v>18835</v>
       </c>
       <c r="D248">
-        <v>19200</v>
+        <v>19202</v>
       </c>
       <c r="E248">
-        <v>18063</v>
+        <v>18065</v>
       </c>
       <c r="F248">
-        <v>17882</v>
+        <v>17881</v>
       </c>
       <c r="G248">
-        <v>18245</v>
+        <v>18244</v>
       </c>
       <c r="H248">
         <v>1.02</v>
@@ -10676,22 +10676,22 @@
         <v>44139</v>
       </c>
       <c r="B249">
-        <v>18021</v>
+        <v>18020</v>
       </c>
       <c r="C249">
-        <v>17853</v>
+        <v>17857</v>
       </c>
       <c r="D249">
-        <v>18173</v>
+        <v>18172</v>
       </c>
       <c r="E249">
-        <v>18665</v>
+        <v>18666</v>
       </c>
       <c r="F249">
-        <v>18493</v>
+        <v>18492</v>
       </c>
       <c r="G249">
-        <v>18844</v>
+        <v>18843</v>
       </c>
       <c r="H249">
         <v>1.1000000000000001</v>
@@ -10720,16 +10720,16 @@
         <v>16539</v>
       </c>
       <c r="C250">
-        <v>16371</v>
+        <v>16364</v>
       </c>
       <c r="D250">
-        <v>16729</v>
+        <v>16727</v>
       </c>
       <c r="E250">
-        <v>18636</v>
+        <v>18637</v>
       </c>
       <c r="F250">
-        <v>18462</v>
+        <v>18461</v>
       </c>
       <c r="G250">
         <v>18817</v>
@@ -10758,13 +10758,13 @@
         <v>44141</v>
       </c>
       <c r="B251">
-        <v>16124</v>
+        <v>16123</v>
       </c>
       <c r="C251">
-        <v>15971</v>
+        <v>15979</v>
       </c>
       <c r="D251">
-        <v>16312</v>
+        <v>16309</v>
       </c>
       <c r="E251">
         <v>17425</v>
@@ -10773,7 +10773,7 @@
         <v>17259</v>
       </c>
       <c r="G251">
-        <v>17603</v>
+        <v>17602</v>
       </c>
       <c r="H251">
         <v>0.99</v>
@@ -10799,19 +10799,19 @@
         <v>44142</v>
       </c>
       <c r="B252">
-        <v>15049</v>
+        <v>15048</v>
       </c>
       <c r="C252">
-        <v>14901</v>
+        <v>14905</v>
       </c>
       <c r="D252">
-        <v>15204</v>
+        <v>15208</v>
       </c>
       <c r="E252">
         <v>16433</v>
       </c>
       <c r="F252">
-        <v>16274</v>
+        <v>16276</v>
       </c>
       <c r="G252">
         <v>16604</v>
@@ -10840,22 +10840,22 @@
         <v>44143</v>
       </c>
       <c r="B253">
-        <v>15143</v>
+        <v>15142</v>
       </c>
       <c r="C253">
-        <v>14942</v>
+        <v>14954</v>
       </c>
       <c r="D253">
-        <v>15322</v>
+        <v>15312</v>
       </c>
       <c r="E253">
-        <v>15714</v>
+        <v>15713</v>
       </c>
       <c r="F253">
-        <v>15546</v>
+        <v>15550</v>
       </c>
       <c r="G253">
-        <v>15892</v>
+        <v>15889</v>
       </c>
       <c r="H253">
         <v>0.84</v>
@@ -10881,22 +10881,22 @@
         <v>44144</v>
       </c>
       <c r="B254">
-        <v>19037</v>
+        <v>19036</v>
       </c>
       <c r="C254">
-        <v>18852</v>
+        <v>18842</v>
       </c>
       <c r="D254">
-        <v>19282</v>
+        <v>19272</v>
       </c>
       <c r="E254">
-        <v>16338</v>
+        <v>16337</v>
       </c>
       <c r="F254">
-        <v>16166</v>
+        <v>16170</v>
       </c>
       <c r="G254">
-        <v>16530</v>
+        <v>16525</v>
       </c>
       <c r="H254">
         <v>0.88</v>
@@ -10925,19 +10925,19 @@
         <v>18431</v>
       </c>
       <c r="C255">
-        <v>18229</v>
+        <v>18221</v>
       </c>
       <c r="D255">
-        <v>18606</v>
+        <v>18609</v>
       </c>
       <c r="E255">
-        <v>16915</v>
+        <v>16914</v>
       </c>
       <c r="F255">
-        <v>16731</v>
+        <v>16730</v>
       </c>
       <c r="G255">
-        <v>17103</v>
+        <v>17100</v>
       </c>
       <c r="H255">
         <v>0.97</v>
@@ -10963,22 +10963,22 @@
         <v>44146</v>
       </c>
       <c r="B256">
-        <v>17922</v>
+        <v>17924</v>
       </c>
       <c r="C256">
-        <v>17725</v>
+        <v>17723</v>
       </c>
       <c r="D256">
-        <v>18099</v>
+        <v>18093</v>
       </c>
       <c r="E256">
         <v>17633</v>
       </c>
       <c r="F256">
-        <v>17437</v>
+        <v>17435</v>
       </c>
       <c r="G256">
-        <v>17827</v>
+        <v>17821</v>
       </c>
       <c r="H256">
         <v>1.07</v>
@@ -11004,22 +11004,22 @@
         <v>44147</v>
       </c>
       <c r="B257">
-        <v>17651</v>
+        <v>17649</v>
       </c>
       <c r="C257">
-        <v>17473</v>
+        <v>17475</v>
       </c>
       <c r="D257">
-        <v>17848</v>
+        <v>17835</v>
       </c>
       <c r="E257">
-        <v>18261</v>
+        <v>18260</v>
       </c>
       <c r="F257">
-        <v>18070</v>
+        <v>18065</v>
       </c>
       <c r="G257">
-        <v>18459</v>
+        <v>18452</v>
       </c>
       <c r="H257">
         <v>1.1599999999999999</v>
@@ -11045,13 +11045,13 @@
         <v>44148</v>
       </c>
       <c r="B258">
-        <v>18350</v>
+        <v>18352</v>
       </c>
       <c r="C258">
-        <v>18178</v>
+        <v>18184</v>
       </c>
       <c r="D258">
-        <v>18539</v>
+        <v>18546</v>
       </c>
       <c r="E258">
         <v>18089</v>
@@ -11060,7 +11060,7 @@
         <v>17901</v>
       </c>
       <c r="G258">
-        <v>18273</v>
+        <v>18271</v>
       </c>
       <c r="H258">
         <v>1.1100000000000001</v>
@@ -11069,7 +11069,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="J258">
-        <v>1.1100000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="K258">
         <v>1.04</v>
@@ -11086,19 +11086,19 @@
         <v>44149</v>
       </c>
       <c r="B259">
-        <v>16316</v>
+        <v>16314</v>
       </c>
       <c r="C259">
-        <v>16162</v>
+        <v>16151</v>
       </c>
       <c r="D259">
-        <v>16501</v>
+        <v>16511</v>
       </c>
       <c r="E259">
         <v>17560</v>
       </c>
       <c r="F259">
-        <v>17384</v>
+        <v>17383</v>
       </c>
       <c r="G259">
         <v>17746</v>
@@ -11127,22 +11127,22 @@
         <v>44150</v>
       </c>
       <c r="B260">
-        <v>16488</v>
+        <v>16493</v>
       </c>
       <c r="C260">
-        <v>16319</v>
+        <v>16317</v>
       </c>
       <c r="D260">
-        <v>16672</v>
+        <v>16704</v>
       </c>
       <c r="E260">
-        <v>17201</v>
+        <v>17202</v>
       </c>
       <c r="F260">
-        <v>17033</v>
+        <v>17032</v>
       </c>
       <c r="G260">
-        <v>17390</v>
+        <v>17399</v>
       </c>
       <c r="H260">
         <v>0.98</v>
@@ -11168,22 +11168,22 @@
         <v>44151</v>
       </c>
       <c r="B261">
-        <v>20459</v>
+        <v>20449</v>
       </c>
       <c r="C261">
-        <v>20268</v>
+        <v>20246</v>
       </c>
       <c r="D261">
-        <v>20646</v>
+        <v>20645</v>
       </c>
       <c r="E261">
-        <v>17903</v>
+        <v>17902</v>
       </c>
       <c r="F261">
-        <v>17732</v>
+        <v>17724</v>
       </c>
       <c r="G261">
-        <v>18089</v>
+        <v>18101</v>
       </c>
       <c r="H261">
         <v>0.98</v>
@@ -11209,22 +11209,22 @@
         <v>44152</v>
       </c>
       <c r="B262">
-        <v>19440</v>
+        <v>19436</v>
       </c>
       <c r="C262">
-        <v>19214</v>
+        <v>19250</v>
       </c>
       <c r="D262">
-        <v>19603</v>
+        <v>19595</v>
       </c>
       <c r="E262">
-        <v>18176</v>
+        <v>18173</v>
       </c>
       <c r="F262">
         <v>17991</v>
       </c>
       <c r="G262">
-        <v>18355</v>
+        <v>18364</v>
       </c>
       <c r="H262">
         <v>1</v>
@@ -11250,22 +11250,22 @@
         <v>44153</v>
       </c>
       <c r="B263">
-        <v>18606</v>
+        <v>18599</v>
       </c>
       <c r="C263">
-        <v>18423</v>
+        <v>18390</v>
       </c>
       <c r="D263">
-        <v>18811</v>
+        <v>18797</v>
       </c>
       <c r="E263">
-        <v>18748</v>
+        <v>18744</v>
       </c>
       <c r="F263">
-        <v>18556</v>
+        <v>18551</v>
       </c>
       <c r="G263">
-        <v>18933</v>
+        <v>18935</v>
       </c>
       <c r="H263">
         <v>1.07</v>
@@ -11291,22 +11291,22 @@
         <v>44154</v>
       </c>
       <c r="B264">
-        <v>17282</v>
+        <v>17276</v>
       </c>
       <c r="C264">
-        <v>17092</v>
+        <v>17100</v>
       </c>
       <c r="D264">
-        <v>17484</v>
+        <v>17495</v>
       </c>
       <c r="E264">
-        <v>18947</v>
+        <v>18940</v>
       </c>
       <c r="F264">
-        <v>18749</v>
+        <v>18746</v>
       </c>
       <c r="G264">
-        <v>19136</v>
+        <v>19133</v>
       </c>
       <c r="H264">
         <v>1.1000000000000001</v>
@@ -11332,22 +11332,22 @@
         <v>44155</v>
       </c>
       <c r="B265">
-        <v>16801</v>
+        <v>16798</v>
       </c>
       <c r="C265">
-        <v>16637</v>
+        <v>16594</v>
       </c>
       <c r="D265">
-        <v>16994</v>
+        <v>16988</v>
       </c>
       <c r="E265">
-        <v>18032</v>
+        <v>18027</v>
       </c>
       <c r="F265">
-        <v>17841</v>
+        <v>17833</v>
       </c>
       <c r="G265">
-        <v>18223</v>
+        <v>18219</v>
       </c>
       <c r="H265">
         <v>1.01</v>
@@ -11373,22 +11373,22 @@
         <v>44156</v>
       </c>
       <c r="B266">
-        <v>14472</v>
+        <v>14473</v>
       </c>
       <c r="C266">
-        <v>14288</v>
+        <v>14299</v>
       </c>
       <c r="D266">
-        <v>14632</v>
+        <v>14616</v>
       </c>
       <c r="E266">
-        <v>16790</v>
+        <v>16787</v>
       </c>
       <c r="F266">
-        <v>16610</v>
+        <v>16595</v>
       </c>
       <c r="G266">
-        <v>16980</v>
+        <v>16974</v>
       </c>
       <c r="H266">
         <v>0.92</v>
@@ -11400,7 +11400,7 @@
         <v>0.93</v>
       </c>
       <c r="K266">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="L266">
         <v>0.95</v>
@@ -11414,22 +11414,22 @@
         <v>44157</v>
       </c>
       <c r="B267">
-        <v>14526</v>
+        <v>14525</v>
       </c>
       <c r="C267">
-        <v>14334</v>
+        <v>14365</v>
       </c>
       <c r="D267">
-        <v>14724</v>
+        <v>14676</v>
       </c>
       <c r="E267">
-        <v>15770</v>
+        <v>15768</v>
       </c>
       <c r="F267">
-        <v>15588</v>
+        <v>15589</v>
       </c>
       <c r="G267">
-        <v>15958</v>
+        <v>15944</v>
       </c>
       <c r="H267">
         <v>0.84</v>
@@ -11455,22 +11455,22 @@
         <v>44158</v>
       </c>
       <c r="B268">
-        <v>18502</v>
+        <v>18509</v>
       </c>
       <c r="C268">
-        <v>18335</v>
+        <v>18350</v>
       </c>
       <c r="D268">
         <v>18667</v>
       </c>
       <c r="E268">
-        <v>16075</v>
+        <v>16076</v>
       </c>
       <c r="F268">
-        <v>15898</v>
+        <v>15902</v>
       </c>
       <c r="G268">
-        <v>16254</v>
+        <v>16237</v>
       </c>
       <c r="H268">
         <v>0.85</v>
@@ -11479,13 +11479,13 @@
         <v>0.84</v>
       </c>
       <c r="J268">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
       <c r="K268">
         <v>0.94</v>
       </c>
       <c r="L268">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="M268">
         <v>0.94</v>
@@ -11496,22 +11496,22 @@
         <v>44159</v>
       </c>
       <c r="B269">
-        <v>17487</v>
+        <v>17480</v>
       </c>
       <c r="C269">
-        <v>17319</v>
+        <v>17314</v>
       </c>
       <c r="D269">
-        <v>17646</v>
+        <v>17624</v>
       </c>
       <c r="E269">
         <v>16247</v>
       </c>
       <c r="F269">
-        <v>16069</v>
+        <v>16082</v>
       </c>
       <c r="G269">
-        <v>16417</v>
+        <v>16396</v>
       </c>
       <c r="H269">
         <v>0.9</v>
@@ -11537,22 +11537,22 @@
         <v>44160</v>
       </c>
       <c r="B270">
-        <v>16967</v>
+        <v>16937</v>
       </c>
       <c r="C270">
-        <v>16810</v>
+        <v>16739</v>
       </c>
       <c r="D270">
-        <v>17148</v>
+        <v>17168</v>
       </c>
       <c r="E270">
-        <v>16871</v>
+        <v>16863</v>
       </c>
       <c r="F270">
-        <v>16699</v>
+        <v>16692</v>
       </c>
       <c r="G270">
-        <v>17046</v>
+        <v>17033</v>
       </c>
       <c r="H270">
         <v>1</v>
@@ -11578,22 +11578,22 @@
         <v>44161</v>
       </c>
       <c r="B271">
-        <v>16080</v>
+        <v>16092</v>
       </c>
       <c r="C271">
-        <v>15896</v>
+        <v>15910</v>
       </c>
       <c r="D271">
-        <v>16254</v>
+        <v>16289</v>
       </c>
       <c r="E271">
-        <v>17259</v>
+        <v>17254</v>
       </c>
       <c r="F271">
-        <v>17090</v>
+        <v>17078</v>
       </c>
       <c r="G271">
-        <v>17429</v>
+        <v>17437</v>
       </c>
       <c r="H271">
         <v>1.0900000000000001</v>
@@ -11619,28 +11619,28 @@
         <v>44162</v>
       </c>
       <c r="B272">
-        <v>16515</v>
+        <v>16527</v>
       </c>
       <c r="C272">
-        <v>16332</v>
+        <v>16370</v>
       </c>
       <c r="D272">
-        <v>16680</v>
+        <v>16719</v>
       </c>
       <c r="E272">
-        <v>16762</v>
+        <v>16759</v>
       </c>
       <c r="F272">
-        <v>16589</v>
+        <v>16583</v>
       </c>
       <c r="G272">
-        <v>16932</v>
+        <v>16950</v>
       </c>
       <c r="H272">
         <v>1.04</v>
       </c>
       <c r="I272">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="J272">
         <v>1.05</v>
@@ -11660,34 +11660,34 @@
         <v>44163</v>
       </c>
       <c r="B273">
-        <v>15591</v>
+        <v>15595</v>
       </c>
       <c r="C273">
-        <v>15448</v>
+        <v>15359</v>
       </c>
       <c r="D273">
-        <v>15776</v>
+        <v>15771</v>
       </c>
       <c r="E273">
         <v>16288</v>
       </c>
       <c r="F273">
-        <v>16122</v>
+        <v>16094</v>
       </c>
       <c r="G273">
-        <v>16464</v>
+        <v>16486</v>
       </c>
       <c r="H273">
         <v>1</v>
       </c>
       <c r="I273">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="J273">
         <v>1.01</v>
       </c>
       <c r="K273">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="L273">
         <v>1</v>
@@ -11701,22 +11701,22 @@
         <v>44164</v>
       </c>
       <c r="B274">
-        <v>15471</v>
+        <v>15490</v>
       </c>
       <c r="C274">
-        <v>15281</v>
+        <v>15324</v>
       </c>
       <c r="D274">
-        <v>15649</v>
+        <v>15679</v>
       </c>
       <c r="E274">
-        <v>15914</v>
+        <v>15926</v>
       </c>
       <c r="F274">
-        <v>15739</v>
+        <v>15741</v>
       </c>
       <c r="G274">
-        <v>16090</v>
+        <v>16114</v>
       </c>
       <c r="H274">
         <v>0.94</v>
@@ -11742,28 +11742,28 @@
         <v>44165</v>
       </c>
       <c r="B275">
-        <v>20875</v>
+        <v>20879</v>
       </c>
       <c r="C275">
-        <v>20686</v>
+        <v>20669</v>
       </c>
       <c r="D275">
-        <v>21063</v>
+        <v>21085</v>
       </c>
       <c r="E275">
-        <v>17113</v>
+        <v>17123</v>
       </c>
       <c r="F275">
-        <v>16937</v>
+        <v>16930</v>
       </c>
       <c r="G275">
-        <v>17292</v>
+        <v>17313</v>
       </c>
       <c r="H275">
         <v>0.99</v>
       </c>
       <c r="I275">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="J275">
         <v>1</v>
@@ -11783,22 +11783,22 @@
         <v>44166</v>
       </c>
       <c r="B276">
-        <v>20885</v>
+        <v>20869</v>
       </c>
       <c r="C276">
-        <v>20694</v>
+        <v>20663</v>
       </c>
       <c r="D276">
-        <v>21090</v>
+        <v>21067</v>
       </c>
       <c r="E276">
-        <v>18205</v>
+        <v>18208</v>
       </c>
       <c r="F276">
-        <v>18027</v>
+        <v>18004</v>
       </c>
       <c r="G276">
-        <v>18395</v>
+        <v>18400</v>
       </c>
       <c r="H276">
         <v>1.0900000000000001</v>
@@ -11824,22 +11824,22 @@
         <v>44167</v>
       </c>
       <c r="B277">
-        <v>20734</v>
+        <v>20721</v>
       </c>
       <c r="C277">
-        <v>20525</v>
+        <v>20519</v>
       </c>
       <c r="D277">
-        <v>20956</v>
+        <v>20940</v>
       </c>
       <c r="E277">
-        <v>19491</v>
+        <v>19490</v>
       </c>
       <c r="F277">
-        <v>19296</v>
+        <v>19294</v>
       </c>
       <c r="G277">
-        <v>19690</v>
+        <v>19693</v>
       </c>
       <c r="H277">
         <v>1.2</v>
@@ -11865,22 +11865,22 @@
         <v>44168</v>
       </c>
       <c r="B278">
-        <v>21065</v>
+        <v>21062</v>
       </c>
       <c r="C278">
-        <v>20728</v>
+        <v>20881</v>
       </c>
       <c r="D278">
-        <v>21429</v>
+        <v>21265</v>
       </c>
       <c r="E278">
-        <v>20890</v>
+        <v>20883</v>
       </c>
       <c r="F278">
-        <v>20658</v>
+        <v>20683</v>
       </c>
       <c r="G278">
-        <v>21135</v>
+        <v>21089</v>
       </c>
       <c r="H278">
         <v>1.31</v>
@@ -11906,22 +11906,22 @@
         <v>44169</v>
       </c>
       <c r="B279">
-        <v>21728</v>
+        <v>21741</v>
       </c>
       <c r="C279">
-        <v>21309</v>
+        <v>21372</v>
       </c>
       <c r="D279">
-        <v>22063</v>
+        <v>22111</v>
       </c>
       <c r="E279">
-        <v>21103</v>
+        <v>21098</v>
       </c>
       <c r="F279">
-        <v>20814</v>
+        <v>20859</v>
       </c>
       <c r="G279">
-        <v>21385</v>
+        <v>21346</v>
       </c>
       <c r="H279">
         <v>1.23</v>
@@ -11947,22 +11947,22 @@
         <v>44170</v>
       </c>
       <c r="B280">
-        <v>20734</v>
+        <v>20708</v>
       </c>
       <c r="C280">
-        <v>20254</v>
+        <v>20277</v>
       </c>
       <c r="D280">
-        <v>21247</v>
+        <v>21088</v>
       </c>
       <c r="E280">
-        <v>21065</v>
+        <v>21058</v>
       </c>
       <c r="F280">
-        <v>20704</v>
+        <v>20762</v>
       </c>
       <c r="G280">
-        <v>21424</v>
+        <v>21351</v>
       </c>
       <c r="H280">
         <v>1.1599999999999999</v>
@@ -11988,37 +11988,37 @@
         <v>44171</v>
       </c>
       <c r="B281">
-        <v>21085</v>
+        <v>21044</v>
       </c>
       <c r="C281">
-        <v>20684</v>
+        <v>20718</v>
       </c>
       <c r="D281">
-        <v>21423</v>
+        <v>21433</v>
       </c>
       <c r="E281">
-        <v>21153</v>
+        <v>21139</v>
       </c>
       <c r="F281">
-        <v>20744</v>
+        <v>20812</v>
       </c>
       <c r="G281">
-        <v>21541</v>
+        <v>21474</v>
       </c>
       <c r="H281">
-        <v>1.0900000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="I281">
         <v>1.07</v>
       </c>
       <c r="J281">
-        <v>1.1000000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="K281">
         <v>1.1599999999999999</v>
       </c>
       <c r="L281">
-        <v>1.1499999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="M281">
         <v>1.17</v>
@@ -12029,22 +12029,22 @@
         <v>44172</v>
       </c>
       <c r="B282">
-        <v>26218</v>
+        <v>26222</v>
       </c>
       <c r="C282">
-        <v>25737</v>
+        <v>25598</v>
       </c>
       <c r="D282">
-        <v>26670</v>
+        <v>26678</v>
       </c>
       <c r="E282">
-        <v>22441</v>
+        <v>22429</v>
       </c>
       <c r="F282">
-        <v>21996</v>
+        <v>21991</v>
       </c>
       <c r="G282">
-        <v>22851</v>
+        <v>22827</v>
       </c>
       <c r="H282">
         <v>1.07</v>
@@ -12056,7 +12056,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="K282">
-        <v>1.1599999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="L282">
         <v>1.1499999999999999</v>
@@ -12070,22 +12070,22 @@
         <v>44173</v>
       </c>
       <c r="B283">
-        <v>26018</v>
+        <v>25960</v>
       </c>
       <c r="C283">
-        <v>25385</v>
+        <v>25411</v>
       </c>
       <c r="D283">
-        <v>26715</v>
+        <v>26560</v>
       </c>
       <c r="E283">
-        <v>23514</v>
+        <v>23483</v>
       </c>
       <c r="F283">
-        <v>23015</v>
+        <v>23001</v>
       </c>
       <c r="G283">
-        <v>24014</v>
+        <v>23940</v>
       </c>
       <c r="H283">
         <v>1.1100000000000001</v>
@@ -12111,22 +12111,22 @@
         <v>44174</v>
       </c>
       <c r="B284">
-        <v>25048</v>
+        <v>25000</v>
       </c>
       <c r="C284">
-        <v>24335</v>
+        <v>24385</v>
       </c>
       <c r="D284">
-        <v>25887</v>
+        <v>25581</v>
       </c>
       <c r="E284">
-        <v>24592</v>
+        <v>24557</v>
       </c>
       <c r="F284">
-        <v>24035</v>
+        <v>24028</v>
       </c>
       <c r="G284">
-        <v>25174</v>
+        <v>25063</v>
       </c>
       <c r="H284">
         <v>1.17</v>
@@ -12141,7 +12141,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="L284">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="M284">
         <v>1.1299999999999999</v>
@@ -12152,22 +12152,22 @@
         <v>44175</v>
       </c>
       <c r="B285">
-        <v>24630</v>
+        <v>24576</v>
       </c>
       <c r="C285">
-        <v>23765</v>
+        <v>23866</v>
       </c>
       <c r="D285">
-        <v>25338</v>
+        <v>25285</v>
       </c>
       <c r="E285">
-        <v>25478</v>
+        <v>25439</v>
       </c>
       <c r="F285">
-        <v>24805</v>
+        <v>24815</v>
       </c>
       <c r="G285">
-        <v>26152</v>
+        <v>26026</v>
       </c>
       <c r="H285">
         <v>1.2</v>
@@ -12193,31 +12193,31 @@
         <v>44176</v>
       </c>
       <c r="B286">
-        <v>24618</v>
+        <v>24621</v>
       </c>
       <c r="C286">
-        <v>23859</v>
+        <v>23727</v>
       </c>
       <c r="D286">
-        <v>25316</v>
+        <v>25498</v>
       </c>
       <c r="E286">
-        <v>25078</v>
+        <v>25039</v>
       </c>
       <c r="F286">
-        <v>24336</v>
+        <v>24347</v>
       </c>
       <c r="G286">
-        <v>25814</v>
+        <v>25731</v>
       </c>
       <c r="H286">
         <v>1.1200000000000001</v>
       </c>
       <c r="I286">
-        <v>1.1000000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="J286">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="K286">
         <v>1.08</v>
@@ -12234,22 +12234,22 @@
         <v>44177</v>
       </c>
       <c r="B287">
-        <v>23141</v>
+        <v>23082</v>
       </c>
       <c r="C287">
-        <v>22413</v>
+        <v>22416</v>
       </c>
       <c r="D287">
-        <v>24035</v>
+        <v>23830</v>
       </c>
       <c r="E287">
-        <v>24359</v>
+        <v>24320</v>
       </c>
       <c r="F287">
-        <v>23593</v>
+        <v>23598</v>
       </c>
       <c r="G287">
-        <v>25144</v>
+        <v>25049</v>
       </c>
       <c r="H287">
         <v>1.04</v>
@@ -12258,7 +12258,7 @@
         <v>1.02</v>
       </c>
       <c r="J287">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="K287">
         <v>1.06</v>
@@ -12275,28 +12275,28 @@
         <v>44178</v>
       </c>
       <c r="B288">
-        <v>22507</v>
+        <v>22439</v>
       </c>
       <c r="C288">
-        <v>21851</v>
+        <v>21608</v>
       </c>
       <c r="D288">
-        <v>23140</v>
+        <v>23064</v>
       </c>
       <c r="E288">
-        <v>23724</v>
+        <v>23679</v>
       </c>
       <c r="F288">
-        <v>22972</v>
+        <v>22904</v>
       </c>
       <c r="G288">
-        <v>24457</v>
+        <v>24419</v>
       </c>
       <c r="H288">
         <v>0.96</v>
       </c>
       <c r="I288">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="J288">
         <v>0.98</v>
@@ -12308,7 +12308,7 @@
         <v>1.04</v>
       </c>
       <c r="M288">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="289" spans="1:13">
@@ -12316,37 +12316,37 @@
         <v>44179</v>
       </c>
       <c r="B289">
-        <v>28057</v>
+        <v>28027</v>
       </c>
       <c r="C289">
-        <v>26750</v>
+        <v>27238</v>
       </c>
       <c r="D289">
-        <v>29207</v>
+        <v>28967</v>
       </c>
       <c r="E289">
-        <v>24581</v>
+        <v>24542</v>
       </c>
       <c r="F289">
-        <v>23718</v>
+        <v>23747</v>
       </c>
       <c r="G289">
-        <v>25424</v>
+        <v>25340</v>
       </c>
       <c r="H289">
         <v>0.96</v>
       </c>
       <c r="I289">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="J289">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="K289">
         <v>1.04</v>
       </c>
       <c r="L289">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="M289">
         <v>1.05</v>
@@ -12357,22 +12357,22 @@
         <v>44180</v>
       </c>
       <c r="B290">
-        <v>26794</v>
+        <v>26700</v>
       </c>
       <c r="C290">
-        <v>25707</v>
+        <v>25446</v>
       </c>
       <c r="D290">
-        <v>27651</v>
+        <v>27793</v>
       </c>
       <c r="E290">
-        <v>25125</v>
+        <v>25062</v>
       </c>
       <c r="F290">
-        <v>24180</v>
+        <v>24177</v>
       </c>
       <c r="G290">
-        <v>26008</v>
+        <v>25914</v>
       </c>
       <c r="H290">
         <v>1</v>
@@ -12381,7 +12381,7 @@
         <v>0.98</v>
       </c>
       <c r="J290">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="K290">
         <v>1.03</v>
@@ -12398,22 +12398,22 @@
         <v>44181</v>
       </c>
       <c r="B291">
-        <v>25541</v>
+        <v>25467</v>
       </c>
       <c r="C291">
-        <v>24355</v>
+        <v>24372</v>
       </c>
       <c r="D291">
-        <v>26651</v>
+        <v>26526</v>
       </c>
       <c r="E291">
-        <v>25725</v>
+        <v>25658</v>
       </c>
       <c r="F291">
         <v>24666</v>
       </c>
       <c r="G291">
-        <v>26662</v>
+        <v>26587</v>
       </c>
       <c r="H291">
         <v>1.06</v>
@@ -12439,31 +12439,31 @@
         <v>44182</v>
       </c>
       <c r="B292">
-        <v>23572</v>
+        <v>23438</v>
       </c>
       <c r="C292">
-        <v>22304</v>
+        <v>22259</v>
       </c>
       <c r="D292">
-        <v>24820</v>
+        <v>24410</v>
       </c>
       <c r="E292">
-        <v>25991</v>
+        <v>25908</v>
       </c>
       <c r="F292">
-        <v>24779</v>
+        <v>24829</v>
       </c>
       <c r="G292">
-        <v>27082</v>
+        <v>26924</v>
       </c>
       <c r="H292">
-        <v>1.1000000000000001</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I292">
         <v>1.07</v>
       </c>
       <c r="J292">
-        <v>1.1299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="K292">
         <v>0.99</v>
@@ -12472,7 +12472,7 @@
         <v>0.98</v>
       </c>
       <c r="M292">
-        <v>1.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="293" spans="1:13">
@@ -12480,28 +12480,28 @@
         <v>44183</v>
       </c>
       <c r="B293">
-        <v>22765</v>
+        <v>22716</v>
       </c>
       <c r="C293">
-        <v>21035</v>
+        <v>21366</v>
       </c>
       <c r="D293">
-        <v>23949</v>
+        <v>23716</v>
       </c>
       <c r="E293">
-        <v>24668</v>
+        <v>24580</v>
       </c>
       <c r="F293">
-        <v>23350</v>
+        <v>23361</v>
       </c>
       <c r="G293">
-        <v>25768</v>
+        <v>25611</v>
       </c>
       <c r="H293">
         <v>1</v>
       </c>
       <c r="I293">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="J293">
         <v>1.03</v>
@@ -12510,7 +12510,7 @@
         <v>0.97</v>
       </c>
       <c r="L293">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="M293">
         <v>0.99</v>
@@ -12521,31 +12521,31 @@
         <v>44184</v>
       </c>
       <c r="B294">
-        <v>20877</v>
+        <v>20909</v>
       </c>
       <c r="C294">
-        <v>19679</v>
+        <v>19814</v>
       </c>
       <c r="D294">
-        <v>22315</v>
+        <v>21957</v>
       </c>
       <c r="E294">
-        <v>23189</v>
+        <v>23133</v>
       </c>
       <c r="F294">
-        <v>21843</v>
+        <v>21953</v>
       </c>
       <c r="G294">
-        <v>24434</v>
+        <v>24152</v>
       </c>
       <c r="H294">
         <v>0.92</v>
       </c>
       <c r="I294">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="J294">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="K294">
         <v>0.96</v>
@@ -12554,7 +12554,7 @@
         <v>0.94</v>
       </c>
       <c r="M294">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="295" spans="1:13">
@@ -12562,22 +12562,22 @@
         <v>44185</v>
       </c>
       <c r="B295">
-        <v>20070</v>
+        <v>20009</v>
       </c>
       <c r="C295">
-        <v>18729</v>
+        <v>18835</v>
       </c>
       <c r="D295">
-        <v>21497</v>
+        <v>21364</v>
       </c>
       <c r="E295">
-        <v>21821</v>
+        <v>21768</v>
       </c>
       <c r="F295">
-        <v>20437</v>
+        <v>20569</v>
       </c>
       <c r="G295">
-        <v>23145</v>
+        <v>22862</v>
       </c>
       <c r="H295">
         <v>0.85</v>
@@ -12592,7 +12592,7 @@
         <v>0.93</v>
       </c>
       <c r="L295">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="M295">
         <v>0.95</v>
@@ -12603,28 +12603,28 @@
         <v>44186</v>
       </c>
       <c r="B296">
-        <v>22585</v>
+        <v>22621</v>
       </c>
       <c r="C296">
-        <v>20777</v>
+        <v>21157</v>
       </c>
       <c r="D296">
-        <v>24003</v>
+        <v>24076</v>
       </c>
       <c r="E296">
-        <v>21574</v>
+        <v>21564</v>
       </c>
       <c r="F296">
-        <v>20055</v>
+        <v>20293</v>
       </c>
       <c r="G296">
-        <v>22941</v>
+        <v>22778</v>
       </c>
       <c r="H296">
         <v>0.83</v>
       </c>
       <c r="I296">
-        <v>0.79</v>
+        <v>0.81</v>
       </c>
       <c r="J296">
         <v>0.86</v>
@@ -12636,7 +12636,7 @@
         <v>0.88</v>
       </c>
       <c r="M296">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="297" spans="1:13">
@@ -12644,28 +12644,28 @@
         <v>44187</v>
       </c>
       <c r="B297">
-        <v>20185</v>
+        <v>20179</v>
       </c>
       <c r="C297">
-        <v>18269</v>
+        <v>18371</v>
       </c>
       <c r="D297">
-        <v>22118</v>
+        <v>21737</v>
       </c>
       <c r="E297">
         <v>20929</v>
       </c>
       <c r="F297">
-        <v>19363</v>
+        <v>19544</v>
       </c>
       <c r="G297">
-        <v>22483</v>
+        <v>22283</v>
       </c>
       <c r="H297">
         <v>0.85</v>
       </c>
       <c r="I297">
-        <v>0.81</v>
+        <v>0.82</v>
       </c>
       <c r="J297">
         <v>0.88</v>
@@ -12674,7 +12674,7 @@
         <v>0.87</v>
       </c>
       <c r="L297">
-        <v>0.84</v>
+        <v>0.85</v>
       </c>
       <c r="M297">
         <v>0.89</v>
@@ -12685,22 +12685,22 @@
         <v>44188</v>
       </c>
       <c r="B298">
-        <v>17570</v>
+        <v>17542</v>
       </c>
       <c r="C298">
-        <v>15663</v>
+        <v>15986</v>
       </c>
       <c r="D298">
-        <v>19498</v>
+        <v>19496</v>
       </c>
       <c r="E298">
-        <v>20102</v>
+        <v>20088</v>
       </c>
       <c r="F298">
-        <v>18360</v>
+        <v>18587</v>
       </c>
       <c r="G298">
-        <v>21779</v>
+        <v>21668</v>
       </c>
       <c r="H298">
         <v>0.87</v>
@@ -12718,7 +12718,7 @@
         <v>0.81</v>
       </c>
       <c r="M298">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="299" spans="1:13">
@@ -12726,34 +12726,34 @@
         <v>44189</v>
       </c>
       <c r="B299">
-        <v>15150</v>
+        <v>15287</v>
       </c>
       <c r="C299">
-        <v>13521</v>
+        <v>13540</v>
       </c>
       <c r="D299">
-        <v>16911</v>
+        <v>16913</v>
       </c>
       <c r="E299">
-        <v>18872</v>
+        <v>18907</v>
       </c>
       <c r="F299">
-        <v>17058</v>
+        <v>17263</v>
       </c>
       <c r="G299">
-        <v>20632</v>
+        <v>20555</v>
       </c>
       <c r="H299">
         <v>0.87</v>
       </c>
       <c r="I299">
-        <v>0.82</v>
+        <v>0.81</v>
       </c>
       <c r="J299">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="K299">
-        <v>0.8</v>
+        <v>0.81</v>
       </c>
       <c r="L299">
         <v>0.78</v>
@@ -12767,31 +12767,31 @@
         <v>44190</v>
       </c>
       <c r="B300">
-        <v>13879</v>
+        <v>13840</v>
       </c>
       <c r="C300">
-        <v>11028</v>
+        <v>11803</v>
       </c>
       <c r="D300">
-        <v>16152</v>
+        <v>15822</v>
       </c>
       <c r="E300">
-        <v>16696</v>
+        <v>16712</v>
       </c>
       <c r="F300">
-        <v>14620</v>
+        <v>14925</v>
       </c>
       <c r="G300">
-        <v>18670</v>
+        <v>18492</v>
       </c>
       <c r="H300">
-        <v>0.77</v>
+        <v>0.78</v>
       </c>
       <c r="I300">
-        <v>0.71</v>
+        <v>0.73</v>
       </c>
       <c r="J300">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="K300">
         <v>0.8</v>
@@ -12808,40 +12808,40 @@
         <v>44191</v>
       </c>
       <c r="B301">
-        <v>15495</v>
+        <v>15037</v>
       </c>
       <c r="C301">
-        <v>12043</v>
+        <v>12614</v>
       </c>
       <c r="D301">
-        <v>18643</v>
+        <v>17881</v>
       </c>
       <c r="E301">
-        <v>15523</v>
+        <v>15427</v>
       </c>
       <c r="F301">
-        <v>13064</v>
+        <v>13486</v>
       </c>
       <c r="G301">
-        <v>17801</v>
+        <v>17528</v>
       </c>
       <c r="H301">
         <v>0.74</v>
       </c>
       <c r="I301">
-        <v>0.66</v>
+        <v>0.69</v>
       </c>
       <c r="J301">
-        <v>0.81</v>
+        <v>0.79</v>
       </c>
       <c r="K301">
         <v>0.83</v>
       </c>
       <c r="L301">
-        <v>0.79</v>
+        <v>0.78</v>
       </c>
       <c r="M301">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="302" spans="1:13">
@@ -12849,40 +12849,40 @@
         <v>44192</v>
       </c>
       <c r="B302">
-        <v>18095</v>
+        <v>17324</v>
       </c>
       <c r="C302">
-        <v>13111</v>
+        <v>12856</v>
       </c>
       <c r="D302">
-        <v>22209</v>
+        <v>21003</v>
       </c>
       <c r="E302">
-        <v>15655</v>
+        <v>15372</v>
       </c>
       <c r="F302">
-        <v>12426</v>
+        <v>12703</v>
       </c>
       <c r="G302">
-        <v>18479</v>
+        <v>17905</v>
       </c>
       <c r="H302">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="I302">
         <v>0.68</v>
       </c>
       <c r="J302">
+        <v>0.83</v>
+      </c>
+      <c r="K302">
         <v>0.87</v>
-      </c>
-      <c r="K302">
-        <v>0.89</v>
       </c>
       <c r="L302">
         <v>0.81</v>
       </c>
       <c r="M302">
-        <v>0.96</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="303" spans="1:13">
@@ -12890,40 +12890,40 @@
         <v>44193</v>
       </c>
       <c r="B303">
-        <v>23531</v>
+        <v>21419</v>
       </c>
       <c r="C303">
-        <v>18459</v>
+        <v>15246</v>
       </c>
       <c r="D303">
-        <v>29811</v>
+        <v>27147</v>
       </c>
       <c r="E303">
-        <v>17750</v>
+        <v>16905</v>
       </c>
       <c r="F303">
-        <v>13660</v>
+        <v>13130</v>
       </c>
       <c r="G303">
-        <v>21703</v>
+        <v>20463</v>
       </c>
       <c r="H303">
-        <v>0.94</v>
+        <v>0.89</v>
       </c>
       <c r="I303">
-        <v>0.8</v>
+        <v>0.79</v>
       </c>
       <c r="J303">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="K303">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="L303">
         <v>0.84</v>
       </c>
       <c r="M303">
-        <v>1.05</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="304" spans="1:13">
@@ -12931,79 +12931,117 @@
         <v>44194</v>
       </c>
       <c r="B304">
-        <v>19890</v>
+        <v>17483</v>
       </c>
       <c r="C304">
-        <v>13210</v>
+        <v>11104</v>
       </c>
       <c r="D304">
-        <v>27730</v>
+        <v>23567</v>
       </c>
       <c r="E304">
-        <v>19253</v>
+        <v>17816</v>
       </c>
       <c r="F304">
-        <v>14206</v>
+        <v>12955</v>
       </c>
       <c r="G304">
-        <v>24598</v>
+        <v>22399</v>
       </c>
       <c r="H304">
-        <v>1.1499999999999999</v>
+        <v>1.07</v>
       </c>
       <c r="I304">
-        <v>0.96</v>
+        <v>0.93</v>
       </c>
       <c r="J304">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="305" spans="1:1">
-      <c r="A305" s="4"/>
-    </row>
-    <row r="306" spans="1:1">
+        <v>1.21</v>
+      </c>
+      <c r="K304">
+        <v>0.91</v>
+      </c>
+      <c r="L304">
+        <v>0.82</v>
+      </c>
+      <c r="M304">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10">
+      <c r="A305" s="4">
+        <v>44195</v>
+      </c>
+      <c r="B305">
+        <v>12399</v>
+      </c>
+      <c r="C305">
+        <v>7142</v>
+      </c>
+      <c r="D305">
+        <v>16576</v>
+      </c>
+      <c r="E305">
+        <v>17156</v>
+      </c>
+      <c r="F305">
+        <v>11587</v>
+      </c>
+      <c r="G305">
+        <v>22073</v>
+      </c>
+      <c r="H305">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I305">
+        <v>0.93</v>
+      </c>
+      <c r="J305">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10">
       <c r="A306" s="4"/>
     </row>
-    <row r="307" spans="1:1">
+    <row r="307" spans="1:10">
       <c r="A307" s="4"/>
     </row>
-    <row r="308" spans="1:1">
+    <row r="308" spans="1:10">
       <c r="A308" s="4"/>
     </row>
-    <row r="309" spans="1:1">
+    <row r="309" spans="1:10">
       <c r="A309" s="4"/>
     </row>
-    <row r="310" spans="1:1">
+    <row r="310" spans="1:10">
       <c r="A310" s="4"/>
     </row>
-    <row r="311" spans="1:1">
+    <row r="311" spans="1:10">
       <c r="A311" s="4"/>
     </row>
-    <row r="312" spans="1:1">
+    <row r="312" spans="1:10">
       <c r="A312" s="4"/>
     </row>
-    <row r="313" spans="1:1">
+    <row r="313" spans="1:10">
       <c r="A313" s="4"/>
     </row>
-    <row r="314" spans="1:1">
+    <row r="314" spans="1:10">
       <c r="A314" s="4"/>
     </row>
-    <row r="315" spans="1:1">
+    <row r="315" spans="1:10">
       <c r="A315" s="4"/>
     </row>
-    <row r="316" spans="1:1">
+    <row r="316" spans="1:10">
       <c r="A316" s="4"/>
     </row>
-    <row r="317" spans="1:1">
+    <row r="317" spans="1:10">
       <c r="A317" s="4"/>
     </row>
-    <row r="318" spans="1:1">
+    <row r="318" spans="1:10">
       <c r="A318" s="4"/>
     </row>
-    <row r="319" spans="1:1">
+    <row r="319" spans="1:10">
       <c r="A319" s="4"/>
     </row>
-    <row r="320" spans="1:1">
+    <row r="320" spans="1:10">
       <c r="A320" s="4"/>
     </row>
     <row r="321" spans="1:1">

</xml_diff>

<commit_message>
add RKI data downloaded 2021-01-30--13-35-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Nowcasting_Zahlen.xlsx
+++ b/rki-data/RKI-Nowcasting_Zahlen.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7124447C-A9CD-416E-8E48-78AD46BC7109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5523C0-C789-4CCF-A19F-56CE9F515543}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <t>Ergebnisse des Nowcastings und der Schätzung der Reproduktionszahl R</t>
   </si>
   <si>
-    <t>Datenstand: 2021-01-27, 00:00 Uhr</t>
+    <t>Datenstand: 2021-01-29, 00:00 Uhr</t>
   </si>
   <si>
     <t>Die Ergebnisse des Nowcastings, also die Schätzung der Anzahl von COVID-19 Neuerkrankungen wird dargestellt mit einem gleitenden 4-Tages-Mittelwert.</t>
@@ -36,7 +36,7 @@
     <t>Dabei wird jeder Wert mit den Werten der 3 vorhergehenden Tage gemittelt.</t>
   </si>
   <si>
-    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-01-27 dargestellten Nowcasting-Kurve.</t>
+    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-01-29 dargestellten Nowcasting-Kurve.</t>
   </si>
   <si>
     <t>Der letzte Schätzwert der Reproduktionszahl R wird ebenfalls im gleichen Lagebericht erwähnt.</t>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Punktschätzer der Anzahl Neuerkrankungen (ohne Glättung)</t>
+  </si>
+  <si>
+    <t>Untere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen (ohne Glä</t>
+  </si>
+  <si>
+    <t>Obere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen (ohne Glät</t>
   </si>
   <si>
     <t>Punktschätzer der Anzahl Neuerkrankungen</t>
@@ -83,26 +89,15 @@
   <si>
     <t>Obere Grenze des 95%-Prädiktionsintervalls des 7-Tage-R Wertes</t>
   </si>
-  <si>
-    <t>Untere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen (ohne Glättung)</t>
-  </si>
-  <si>
-    <t>Obere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen (ohne Glättung)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,16 +127,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -560,56 +548,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M329"/>
+  <dimension ref="A1:M331"/>
   <sheetViews>
-    <sheetView topLeftCell="A319" workbookViewId="0">
-      <selection activeCell="A329" sqref="A329"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="13" width="19.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="90">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="M1" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -11454,16 +11437,16 @@
         <v>18471</v>
       </c>
       <c r="C268">
-        <v>18287</v>
+        <v>18284</v>
       </c>
       <c r="D268">
-        <v>18642</v>
+        <v>18641</v>
       </c>
       <c r="E268">
         <v>16052</v>
       </c>
       <c r="F268">
-        <v>15867</v>
+        <v>15866</v>
       </c>
       <c r="G268">
         <v>16226</v>
@@ -11498,16 +11481,16 @@
         <v>17251</v>
       </c>
       <c r="D269">
-        <v>17600</v>
+        <v>17592</v>
       </c>
       <c r="E269">
         <v>16212</v>
       </c>
       <c r="F269">
-        <v>16036</v>
+        <v>16035</v>
       </c>
       <c r="G269">
-        <v>16383</v>
+        <v>16381</v>
       </c>
       <c r="H269">
         <v>0.9</v>
@@ -11533,22 +11516,22 @@
         <v>44160</v>
       </c>
       <c r="B270">
-        <v>16896</v>
+        <v>16895</v>
       </c>
       <c r="C270">
-        <v>16666</v>
+        <v>16661</v>
       </c>
       <c r="D270">
-        <v>17076</v>
+        <v>17077</v>
       </c>
       <c r="E270">
         <v>16824</v>
       </c>
       <c r="F270">
-        <v>16630</v>
+        <v>16628</v>
       </c>
       <c r="G270">
-        <v>17003</v>
+        <v>17001</v>
       </c>
       <c r="H270">
         <v>1</v>
@@ -11574,22 +11557,22 @@
         <v>44161</v>
       </c>
       <c r="B271">
-        <v>16013</v>
+        <v>16012</v>
       </c>
       <c r="C271">
-        <v>15836</v>
+        <v>15835</v>
       </c>
       <c r="D271">
-        <v>16183</v>
+        <v>16185</v>
       </c>
       <c r="E271">
         <v>17201</v>
       </c>
       <c r="F271">
-        <v>17010</v>
+        <v>17008</v>
       </c>
       <c r="G271">
-        <v>17375</v>
+        <v>17374</v>
       </c>
       <c r="H271">
         <v>1.0900000000000001</v>
@@ -11615,22 +11598,22 @@
         <v>44162</v>
       </c>
       <c r="B272">
-        <v>16413</v>
+        <v>16412</v>
       </c>
       <c r="C272">
-        <v>16243</v>
+        <v>16242</v>
       </c>
       <c r="D272">
-        <v>16585</v>
+        <v>16582</v>
       </c>
       <c r="E272">
-        <v>16687</v>
+        <v>16686</v>
       </c>
       <c r="F272">
-        <v>16499</v>
+        <v>16497</v>
       </c>
       <c r="G272">
-        <v>16861</v>
+        <v>16859</v>
       </c>
       <c r="H272">
         <v>1.04</v>
@@ -11656,19 +11639,19 @@
         <v>44163</v>
       </c>
       <c r="B273">
-        <v>15493</v>
+        <v>15492</v>
       </c>
       <c r="C273">
-        <v>15321</v>
+        <v>15325</v>
       </c>
       <c r="D273">
         <v>15676</v>
       </c>
       <c r="E273">
-        <v>16204</v>
+        <v>16203</v>
       </c>
       <c r="F273">
-        <v>16016</v>
+        <v>16015</v>
       </c>
       <c r="G273">
         <v>16380</v>
@@ -11700,19 +11683,19 @@
         <v>15344</v>
       </c>
       <c r="C274">
-        <v>15161</v>
+        <v>15154</v>
       </c>
       <c r="D274">
-        <v>15493</v>
+        <v>15486</v>
       </c>
       <c r="E274">
-        <v>15816</v>
+        <v>15815</v>
       </c>
       <c r="F274">
-        <v>15640</v>
+        <v>15639</v>
       </c>
       <c r="G274">
-        <v>15984</v>
+        <v>15982</v>
       </c>
       <c r="H274">
         <v>0.94</v>
@@ -11738,22 +11721,22 @@
         <v>44165</v>
       </c>
       <c r="B275">
-        <v>20712</v>
+        <v>20713</v>
       </c>
       <c r="C275">
-        <v>20460</v>
+        <v>20471</v>
       </c>
       <c r="D275">
-        <v>20897</v>
+        <v>20895</v>
       </c>
       <c r="E275">
         <v>16990</v>
       </c>
       <c r="F275">
-        <v>16796</v>
+        <v>16798</v>
       </c>
       <c r="G275">
-        <v>17163</v>
+        <v>17160</v>
       </c>
       <c r="H275">
         <v>0.99</v>
@@ -11779,22 +11762,22 @@
         <v>44166</v>
       </c>
       <c r="B276">
-        <v>20738</v>
+        <v>20741</v>
       </c>
       <c r="C276">
-        <v>20523</v>
+        <v>20532</v>
       </c>
       <c r="D276">
-        <v>20950</v>
+        <v>20947</v>
       </c>
       <c r="E276">
         <v>18072</v>
       </c>
       <c r="F276">
-        <v>17866</v>
+        <v>17870</v>
       </c>
       <c r="G276">
-        <v>18254</v>
+        <v>18251</v>
       </c>
       <c r="H276">
         <v>1.08</v>
@@ -11820,22 +11803,22 @@
         <v>44167</v>
       </c>
       <c r="B277">
-        <v>20603</v>
+        <v>20605</v>
       </c>
       <c r="C277">
-        <v>20393</v>
+        <v>20390</v>
       </c>
       <c r="D277">
-        <v>20824</v>
+        <v>20834</v>
       </c>
       <c r="E277">
-        <v>19349</v>
+        <v>19351</v>
       </c>
       <c r="F277">
-        <v>19134</v>
+        <v>19136</v>
       </c>
       <c r="G277">
-        <v>19541</v>
+        <v>19540</v>
       </c>
       <c r="H277">
         <v>1.19</v>
@@ -11861,22 +11844,22 @@
         <v>44168</v>
       </c>
       <c r="B278">
-        <v>20872</v>
+        <v>20868</v>
       </c>
       <c r="C278">
-        <v>20664</v>
+        <v>20652</v>
       </c>
       <c r="D278">
-        <v>21058</v>
+        <v>21040</v>
       </c>
       <c r="E278">
-        <v>20731</v>
+        <v>20732</v>
       </c>
       <c r="F278">
-        <v>20510</v>
+        <v>20511</v>
       </c>
       <c r="G278">
-        <v>20932</v>
+        <v>20929</v>
       </c>
       <c r="H278">
         <v>1.31</v>
@@ -11902,22 +11885,22 @@
         <v>44169</v>
       </c>
       <c r="B279">
-        <v>21547</v>
+        <v>21543</v>
       </c>
       <c r="C279">
-        <v>21339</v>
+        <v>21350</v>
       </c>
       <c r="D279">
-        <v>21739</v>
+        <v>21744</v>
       </c>
       <c r="E279">
-        <v>20940</v>
+        <v>20939</v>
       </c>
       <c r="F279">
-        <v>20730</v>
+        <v>20731</v>
       </c>
       <c r="G279">
-        <v>21143</v>
+        <v>21141</v>
       </c>
       <c r="H279">
         <v>1.23</v>
@@ -11943,22 +11926,22 @@
         <v>44170</v>
       </c>
       <c r="B280">
-        <v>20439</v>
+        <v>20434</v>
       </c>
       <c r="C280">
-        <v>20255</v>
+        <v>20266</v>
       </c>
       <c r="D280">
+        <v>20658</v>
+      </c>
+      <c r="E280">
+        <v>20863</v>
+      </c>
+      <c r="F280">
         <v>20664</v>
       </c>
-      <c r="E280">
-        <v>20865</v>
-      </c>
-      <c r="F280">
-        <v>20663</v>
-      </c>
       <c r="G280">
-        <v>21071</v>
+        <v>21069</v>
       </c>
       <c r="H280">
         <v>1.1499999999999999</v>
@@ -11984,22 +11967,22 @@
         <v>44171</v>
       </c>
       <c r="B281">
-        <v>20804</v>
+        <v>20796</v>
       </c>
       <c r="C281">
-        <v>20624</v>
+        <v>20627</v>
       </c>
       <c r="D281">
-        <v>20990</v>
+        <v>20973</v>
       </c>
       <c r="E281">
-        <v>20915</v>
+        <v>20910</v>
       </c>
       <c r="F281">
-        <v>20720</v>
+        <v>20724</v>
       </c>
       <c r="G281">
-        <v>21113</v>
+        <v>21104</v>
       </c>
       <c r="H281">
         <v>1.08</v>
@@ -12025,22 +12008,22 @@
         <v>44172</v>
       </c>
       <c r="B282">
-        <v>26086</v>
+        <v>26080</v>
       </c>
       <c r="C282">
-        <v>25877</v>
+        <v>25854</v>
       </c>
       <c r="D282">
-        <v>26296</v>
+        <v>26295</v>
       </c>
       <c r="E282">
-        <v>22219</v>
+        <v>22213</v>
       </c>
       <c r="F282">
         <v>22024</v>
       </c>
       <c r="G282">
-        <v>22422</v>
+        <v>22418</v>
       </c>
       <c r="H282">
         <v>1.07</v>
@@ -12066,22 +12049,22 @@
         <v>44173</v>
       </c>
       <c r="B283">
-        <v>25870</v>
+        <v>25869</v>
       </c>
       <c r="C283">
-        <v>25637</v>
+        <v>25649</v>
       </c>
       <c r="D283">
-        <v>26085</v>
+        <v>26086</v>
       </c>
       <c r="E283">
-        <v>23300</v>
+        <v>23295</v>
       </c>
       <c r="F283">
-        <v>23098</v>
+        <v>23099</v>
       </c>
       <c r="G283">
-        <v>23509</v>
+        <v>23503</v>
       </c>
       <c r="H283">
         <v>1.1100000000000001</v>
@@ -12107,22 +12090,22 @@
         <v>44174</v>
       </c>
       <c r="B284">
-        <v>25184</v>
+        <v>25177</v>
       </c>
       <c r="C284">
-        <v>24989</v>
+        <v>24974</v>
       </c>
       <c r="D284">
-        <v>25394</v>
+        <v>25373</v>
       </c>
       <c r="E284">
-        <v>24486</v>
+        <v>24481</v>
       </c>
       <c r="F284">
-        <v>24282</v>
+        <v>24276</v>
       </c>
       <c r="G284">
-        <v>24691</v>
+        <v>24682</v>
       </c>
       <c r="H284">
         <v>1.17</v>
@@ -12148,22 +12131,22 @@
         <v>44175</v>
       </c>
       <c r="B285">
-        <v>24667</v>
+        <v>24663</v>
       </c>
       <c r="C285">
-        <v>24448</v>
+        <v>24428</v>
       </c>
       <c r="D285">
-        <v>24887</v>
+        <v>24879</v>
       </c>
       <c r="E285">
-        <v>25452</v>
+        <v>25447</v>
       </c>
       <c r="F285">
-        <v>25238</v>
+        <v>25226</v>
       </c>
       <c r="G285">
-        <v>25665</v>
+        <v>25658</v>
       </c>
       <c r="H285">
         <v>1.22</v>
@@ -12178,7 +12161,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="L285">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M285">
         <v>1.1100000000000001</v>
@@ -12189,22 +12172,22 @@
         <v>44176</v>
       </c>
       <c r="B286">
-        <v>24487</v>
+        <v>24479</v>
       </c>
       <c r="C286">
-        <v>24275</v>
+        <v>24284</v>
       </c>
       <c r="D286">
-        <v>24686</v>
+        <v>24705</v>
       </c>
       <c r="E286">
-        <v>25052</v>
+        <v>25047</v>
       </c>
       <c r="F286">
-        <v>24837</v>
+        <v>24834</v>
       </c>
       <c r="G286">
-        <v>25263</v>
+        <v>25260</v>
       </c>
       <c r="H286">
         <v>1.1299999999999999</v>
@@ -12213,13 +12196,13 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="J286">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="K286">
         <v>1.0900000000000001</v>
       </c>
       <c r="L286">
-        <v>1.08</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="M286">
         <v>1.0900000000000001</v>
@@ -12230,22 +12213,22 @@
         <v>44177</v>
       </c>
       <c r="B287">
-        <v>23024</v>
+        <v>23013</v>
       </c>
       <c r="C287">
-        <v>22847</v>
+        <v>22844</v>
       </c>
       <c r="D287">
-        <v>23252</v>
+        <v>23233</v>
       </c>
       <c r="E287">
-        <v>24340</v>
+        <v>24333</v>
       </c>
       <c r="F287">
-        <v>24140</v>
+        <v>24132</v>
       </c>
       <c r="G287">
-        <v>24555</v>
+        <v>24547</v>
       </c>
       <c r="H287">
         <v>1.04</v>
@@ -12271,22 +12254,22 @@
         <v>44178</v>
       </c>
       <c r="B288">
-        <v>22284</v>
+        <v>22273</v>
       </c>
       <c r="C288">
-        <v>22022</v>
+        <v>22026</v>
       </c>
       <c r="D288">
         <v>22501</v>
       </c>
       <c r="E288">
-        <v>23615</v>
+        <v>23607</v>
       </c>
       <c r="F288">
-        <v>23398</v>
+        <v>23395</v>
       </c>
       <c r="G288">
-        <v>23831</v>
+        <v>23829</v>
       </c>
       <c r="H288">
         <v>0.96</v>
@@ -12312,22 +12295,22 @@
         <v>44179</v>
       </c>
       <c r="B289">
-        <v>28056</v>
+        <v>28045</v>
       </c>
       <c r="C289">
-        <v>27781</v>
+        <v>27793</v>
       </c>
       <c r="D289">
-        <v>28274</v>
+        <v>28268</v>
       </c>
       <c r="E289">
-        <v>24463</v>
+        <v>24453</v>
       </c>
       <c r="F289">
-        <v>24231</v>
+        <v>24237</v>
       </c>
       <c r="G289">
-        <v>24678</v>
+        <v>24677</v>
       </c>
       <c r="H289">
         <v>0.96</v>
@@ -12353,22 +12336,22 @@
         <v>44180</v>
       </c>
       <c r="B290">
-        <v>26574</v>
+        <v>26559</v>
       </c>
       <c r="C290">
-        <v>26345</v>
+        <v>26351</v>
       </c>
       <c r="D290">
-        <v>26835</v>
+        <v>26816</v>
       </c>
       <c r="E290">
-        <v>24985</v>
+        <v>24973</v>
       </c>
       <c r="F290">
-        <v>24749</v>
+        <v>24753</v>
       </c>
       <c r="G290">
-        <v>25215</v>
+        <v>25204</v>
       </c>
       <c r="H290">
         <v>1</v>
@@ -12394,28 +12377,28 @@
         <v>44181</v>
       </c>
       <c r="B291">
-        <v>25498</v>
+        <v>25477</v>
       </c>
       <c r="C291">
-        <v>25244</v>
+        <v>25218</v>
       </c>
       <c r="D291">
-        <v>25711</v>
+        <v>25662</v>
       </c>
       <c r="E291">
-        <v>25603</v>
+        <v>25588</v>
       </c>
       <c r="F291">
-        <v>25348</v>
+        <v>25347</v>
       </c>
       <c r="G291">
-        <v>25830</v>
+        <v>25812</v>
       </c>
       <c r="H291">
         <v>1.05</v>
       </c>
       <c r="I291">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
       <c r="J291">
         <v>1.06</v>
@@ -12435,22 +12418,22 @@
         <v>44182</v>
       </c>
       <c r="B292">
-        <v>23803</v>
+        <v>23780</v>
       </c>
       <c r="C292">
-        <v>23598</v>
+        <v>23568</v>
       </c>
       <c r="D292">
-        <v>23980</v>
+        <v>23955</v>
       </c>
       <c r="E292">
-        <v>25983</v>
+        <v>25965</v>
       </c>
       <c r="F292">
-        <v>25742</v>
+        <v>25732</v>
       </c>
       <c r="G292">
-        <v>26200</v>
+        <v>26175</v>
       </c>
       <c r="H292">
         <v>1.1000000000000001</v>
@@ -12476,22 +12459,22 @@
         <v>44183</v>
       </c>
       <c r="B293">
-        <v>23186</v>
+        <v>23164</v>
       </c>
       <c r="C293">
-        <v>22975</v>
+        <v>22956</v>
       </c>
       <c r="D293">
-        <v>23403</v>
+        <v>23368</v>
       </c>
       <c r="E293">
-        <v>24766</v>
+        <v>24745</v>
       </c>
       <c r="F293">
-        <v>24540</v>
+        <v>24523</v>
       </c>
       <c r="G293">
-        <v>24982</v>
+        <v>24950</v>
       </c>
       <c r="H293">
         <v>1.01</v>
@@ -12517,22 +12500,22 @@
         <v>44184</v>
       </c>
       <c r="B294">
-        <v>20684</v>
+        <v>20660</v>
       </c>
       <c r="C294">
-        <v>20494</v>
+        <v>20464</v>
       </c>
       <c r="D294">
-        <v>20889</v>
+        <v>20879</v>
       </c>
       <c r="E294">
-        <v>23293</v>
+        <v>23270</v>
       </c>
       <c r="F294">
-        <v>23078</v>
+        <v>23051</v>
       </c>
       <c r="G294">
-        <v>23495</v>
+        <v>23466</v>
       </c>
       <c r="H294">
         <v>0.93</v>
@@ -12550,7 +12533,7 @@
         <v>0.96</v>
       </c>
       <c r="M294">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="295" spans="1:13">
@@ -12558,22 +12541,22 @@
         <v>44185</v>
       </c>
       <c r="B295">
-        <v>20044</v>
+        <v>20038</v>
       </c>
       <c r="C295">
-        <v>19841</v>
+        <v>19858</v>
       </c>
       <c r="D295">
-        <v>20277</v>
+        <v>20239</v>
       </c>
       <c r="E295">
-        <v>21929</v>
+        <v>21911</v>
       </c>
       <c r="F295">
-        <v>21727</v>
+        <v>21711</v>
       </c>
       <c r="G295">
-        <v>22137</v>
+        <v>22110</v>
       </c>
       <c r="H295">
         <v>0.86</v>
@@ -12599,22 +12582,22 @@
         <v>44186</v>
       </c>
       <c r="B296">
-        <v>23136</v>
+        <v>23078</v>
       </c>
       <c r="C296">
-        <v>22928</v>
+        <v>22884</v>
       </c>
       <c r="D296">
-        <v>23344</v>
+        <v>23267</v>
       </c>
       <c r="E296">
-        <v>21763</v>
+        <v>21735</v>
       </c>
       <c r="F296">
-        <v>21559</v>
+        <v>21540</v>
       </c>
       <c r="G296">
-        <v>21978</v>
+        <v>21938</v>
       </c>
       <c r="H296">
         <v>0.84</v>
@@ -12640,22 +12623,22 @@
         <v>44187</v>
       </c>
       <c r="B297">
-        <v>20601</v>
+        <v>20596</v>
       </c>
       <c r="C297">
-        <v>20344</v>
+        <v>20392</v>
       </c>
       <c r="D297">
-        <v>20789</v>
+        <v>20809</v>
       </c>
       <c r="E297">
-        <v>21116</v>
+        <v>21093</v>
       </c>
       <c r="F297">
-        <v>20901</v>
+        <v>20900</v>
       </c>
       <c r="G297">
-        <v>21325</v>
+        <v>21298</v>
       </c>
       <c r="H297">
         <v>0.85</v>
@@ -12681,22 +12664,22 @@
         <v>44188</v>
       </c>
       <c r="B298">
-        <v>18569</v>
+        <v>18592</v>
       </c>
       <c r="C298">
-        <v>18404</v>
+        <v>18399</v>
       </c>
       <c r="D298">
-        <v>18732</v>
+        <v>18783</v>
       </c>
       <c r="E298">
-        <v>20587</v>
+        <v>20576</v>
       </c>
       <c r="F298">
-        <v>20379</v>
+        <v>20383</v>
       </c>
       <c r="G298">
-        <v>20785</v>
+        <v>20774</v>
       </c>
       <c r="H298">
         <v>0.88</v>
@@ -12722,22 +12705,22 @@
         <v>44189</v>
       </c>
       <c r="B299">
-        <v>16535</v>
+        <v>16540</v>
       </c>
       <c r="C299">
-        <v>16346</v>
+        <v>16395</v>
       </c>
       <c r="D299">
-        <v>16718</v>
+        <v>16680</v>
       </c>
       <c r="E299">
-        <v>19710</v>
+        <v>19701</v>
       </c>
       <c r="F299">
-        <v>19505</v>
+        <v>19517</v>
       </c>
       <c r="G299">
-        <v>19896</v>
+        <v>19884</v>
       </c>
       <c r="H299">
         <v>0.9</v>
@@ -12746,7 +12729,7 @@
         <v>0.89</v>
       </c>
       <c r="J299">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="K299">
         <v>0.83</v>
@@ -12763,22 +12746,22 @@
         <v>44190</v>
       </c>
       <c r="B300">
-        <v>15007</v>
+        <v>14984</v>
       </c>
       <c r="C300">
-        <v>14844</v>
+        <v>14780</v>
       </c>
       <c r="D300">
-        <v>15173</v>
+        <v>15159</v>
       </c>
       <c r="E300">
         <v>17678</v>
       </c>
       <c r="F300">
-        <v>17484</v>
+        <v>17491</v>
       </c>
       <c r="G300">
-        <v>17853</v>
+        <v>17857</v>
       </c>
       <c r="H300">
         <v>0.81</v>
@@ -12804,22 +12787,22 @@
         <v>44191</v>
       </c>
       <c r="B301">
-        <v>16379</v>
+        <v>16328</v>
       </c>
       <c r="C301">
-        <v>16211</v>
+        <v>16148</v>
       </c>
       <c r="D301">
-        <v>16543</v>
+        <v>16493</v>
       </c>
       <c r="E301">
-        <v>16622</v>
+        <v>16611</v>
       </c>
       <c r="F301">
-        <v>16451</v>
+        <v>16430</v>
       </c>
       <c r="G301">
-        <v>16791</v>
+        <v>16778</v>
       </c>
       <c r="H301">
         <v>0.79</v>
@@ -12845,22 +12828,22 @@
         <v>44192</v>
       </c>
       <c r="B302">
-        <v>18241</v>
+        <v>18186</v>
       </c>
       <c r="C302">
-        <v>18036</v>
+        <v>17982</v>
       </c>
       <c r="D302">
-        <v>18442</v>
+        <v>18381</v>
       </c>
       <c r="E302">
-        <v>16540</v>
+        <v>16509</v>
       </c>
       <c r="F302">
-        <v>16359</v>
+        <v>16326</v>
       </c>
       <c r="G302">
-        <v>16719</v>
+        <v>16678</v>
       </c>
       <c r="H302">
         <v>0.8</v>
@@ -12886,22 +12869,22 @@
         <v>44193</v>
       </c>
       <c r="B303">
-        <v>22370</v>
+        <v>22342</v>
       </c>
       <c r="C303">
-        <v>21976</v>
+        <v>22145</v>
       </c>
       <c r="D303">
-        <v>22851</v>
+        <v>22517</v>
       </c>
       <c r="E303">
-        <v>17999</v>
+        <v>17960</v>
       </c>
       <c r="F303">
-        <v>17766</v>
+        <v>17764</v>
       </c>
       <c r="G303">
-        <v>18252</v>
+        <v>18137</v>
       </c>
       <c r="H303">
         <v>0.91</v>
@@ -12927,22 +12910,22 @@
         <v>44194</v>
       </c>
       <c r="B304">
-        <v>18580</v>
+        <v>18634</v>
       </c>
       <c r="C304">
-        <v>18239</v>
+        <v>18472</v>
       </c>
       <c r="D304">
-        <v>18926</v>
+        <v>18803</v>
       </c>
       <c r="E304">
-        <v>18893</v>
+        <v>18872</v>
       </c>
       <c r="F304">
-        <v>18615</v>
+        <v>18687</v>
       </c>
       <c r="G304">
-        <v>19190</v>
+        <v>19048</v>
       </c>
       <c r="H304">
         <v>1.07</v>
@@ -12968,31 +12951,31 @@
         <v>44195</v>
       </c>
       <c r="B305">
-        <v>16289</v>
+        <v>16261</v>
       </c>
       <c r="C305">
-        <v>15887</v>
+        <v>15935</v>
       </c>
       <c r="D305">
-        <v>16612</v>
+        <v>16577</v>
       </c>
       <c r="E305">
-        <v>18870</v>
+        <v>18856</v>
       </c>
       <c r="F305">
-        <v>18534</v>
+        <v>18633</v>
       </c>
       <c r="G305">
-        <v>19208</v>
+        <v>19069</v>
       </c>
       <c r="H305">
         <v>1.1399999999999999</v>
       </c>
       <c r="I305">
-        <v>1.1200000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J305">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="K305">
         <v>0.95</v>
@@ -13009,22 +12992,22 @@
         <v>44196</v>
       </c>
       <c r="B306">
-        <v>14682</v>
+        <v>14647</v>
       </c>
       <c r="C306">
-        <v>14299</v>
+        <v>14359</v>
       </c>
       <c r="D306">
-        <v>15044</v>
+        <v>14859</v>
       </c>
       <c r="E306">
-        <v>17980</v>
+        <v>17971</v>
       </c>
       <c r="F306">
-        <v>17600</v>
+        <v>17727</v>
       </c>
       <c r="G306">
-        <v>18358</v>
+        <v>18189</v>
       </c>
       <c r="H306">
         <v>1.0900000000000001</v>
@@ -13050,22 +13033,22 @@
         <v>44197</v>
       </c>
       <c r="B307">
-        <v>15142</v>
+        <v>15124</v>
       </c>
       <c r="C307">
-        <v>14783</v>
+        <v>14773</v>
       </c>
       <c r="D307">
-        <v>15526</v>
+        <v>15462</v>
       </c>
       <c r="E307">
-        <v>16173</v>
+        <v>16166</v>
       </c>
       <c r="F307">
-        <v>15802</v>
+        <v>15885</v>
       </c>
       <c r="G307">
-        <v>16527</v>
+        <v>16425</v>
       </c>
       <c r="H307">
         <v>0.9</v>
@@ -13091,31 +13074,31 @@
         <v>44198</v>
       </c>
       <c r="B308">
-        <v>16215</v>
+        <v>16260</v>
       </c>
       <c r="C308">
-        <v>15855</v>
+        <v>15848</v>
       </c>
       <c r="D308">
-        <v>16606</v>
+        <v>16602</v>
       </c>
       <c r="E308">
-        <v>15582</v>
+        <v>15573</v>
       </c>
       <c r="F308">
-        <v>15206</v>
+        <v>15229</v>
       </c>
       <c r="G308">
-        <v>15947</v>
+        <v>15875</v>
       </c>
       <c r="H308">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="I308">
         <v>0.81</v>
       </c>
       <c r="J308">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="K308">
         <v>0.98</v>
@@ -13132,22 +13115,22 @@
         <v>44199</v>
       </c>
       <c r="B309">
-        <v>17783</v>
+        <v>17761</v>
       </c>
       <c r="C309">
-        <v>17366</v>
+        <v>17352</v>
       </c>
       <c r="D309">
-        <v>18150</v>
+        <v>18153</v>
       </c>
       <c r="E309">
-        <v>15956</v>
+        <v>15948</v>
       </c>
       <c r="F309">
-        <v>15576</v>
+        <v>15583</v>
       </c>
       <c r="G309">
-        <v>16331</v>
+        <v>16269</v>
       </c>
       <c r="H309">
         <v>0.85</v>
@@ -13173,22 +13156,22 @@
         <v>44200</v>
       </c>
       <c r="B310">
-        <v>21456</v>
+        <v>21331</v>
       </c>
       <c r="C310">
-        <v>20905</v>
+        <v>20886</v>
       </c>
       <c r="D310">
-        <v>21938</v>
+        <v>21757</v>
       </c>
       <c r="E310">
-        <v>17649</v>
+        <v>17619</v>
       </c>
       <c r="F310">
-        <v>17228</v>
+        <v>17215</v>
       </c>
       <c r="G310">
-        <v>18055</v>
+        <v>17993</v>
       </c>
       <c r="H310">
         <v>0.98</v>
@@ -13197,7 +13180,7 @@
         <v>0.97</v>
       </c>
       <c r="J310">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="K310">
         <v>0.99</v>
@@ -13214,31 +13197,31 @@
         <v>44201</v>
       </c>
       <c r="B311">
-        <v>19307</v>
+        <v>19280</v>
       </c>
       <c r="C311">
-        <v>18920</v>
+        <v>18765</v>
       </c>
       <c r="D311">
-        <v>19728</v>
+        <v>19744</v>
       </c>
       <c r="E311">
-        <v>18690</v>
+        <v>18658</v>
       </c>
       <c r="F311">
-        <v>18262</v>
+        <v>18212</v>
       </c>
       <c r="G311">
-        <v>19105</v>
+        <v>19064</v>
       </c>
       <c r="H311">
-        <v>1.1599999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="I311">
         <v>1.1399999999999999</v>
       </c>
       <c r="J311">
-        <v>1.18</v>
+        <v>1.17</v>
       </c>
       <c r="K311">
         <v>1</v>
@@ -13255,28 +13238,28 @@
         <v>44202</v>
       </c>
       <c r="B312">
-        <v>17151</v>
+        <v>17124</v>
       </c>
       <c r="C312">
-        <v>16557</v>
+        <v>16736</v>
       </c>
       <c r="D312">
-        <v>17711</v>
+        <v>17442</v>
       </c>
       <c r="E312">
-        <v>18924</v>
+        <v>18874</v>
       </c>
       <c r="F312">
-        <v>18437</v>
+        <v>18435</v>
       </c>
       <c r="G312">
-        <v>19382</v>
+        <v>19274</v>
       </c>
       <c r="H312">
         <v>1.21</v>
       </c>
       <c r="I312">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="J312">
         <v>1.23</v>
@@ -13296,22 +13279,22 @@
         <v>44203</v>
       </c>
       <c r="B313">
-        <v>15729</v>
+        <v>15715</v>
       </c>
       <c r="C313">
-        <v>15291</v>
+        <v>15388</v>
       </c>
       <c r="D313">
-        <v>16204</v>
+        <v>16144</v>
       </c>
       <c r="E313">
-        <v>18411</v>
+        <v>18362</v>
       </c>
       <c r="F313">
-        <v>17918</v>
+        <v>17944</v>
       </c>
       <c r="G313">
-        <v>18895</v>
+        <v>18772</v>
       </c>
       <c r="H313">
         <v>1.1499999999999999</v>
@@ -13323,13 +13306,13 @@
         <v>1.17</v>
       </c>
       <c r="K313">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="L313">
         <v>1.02</v>
       </c>
       <c r="M313">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="314" spans="1:13">
@@ -13337,22 +13320,22 @@
         <v>44204</v>
       </c>
       <c r="B314">
-        <v>15591</v>
+        <v>15522</v>
       </c>
       <c r="C314">
-        <v>15182</v>
+        <v>15014</v>
       </c>
       <c r="D314">
-        <v>16084</v>
+        <v>16074</v>
       </c>
       <c r="E314">
-        <v>16945</v>
+        <v>16910</v>
       </c>
       <c r="F314">
-        <v>16488</v>
+        <v>16476</v>
       </c>
       <c r="G314">
-        <v>17432</v>
+        <v>17351</v>
       </c>
       <c r="H314">
         <v>0.96</v>
@@ -13378,22 +13361,22 @@
         <v>44205</v>
       </c>
       <c r="B315">
-        <v>13735</v>
+        <v>13623</v>
       </c>
       <c r="C315">
-        <v>13245</v>
+        <v>13238</v>
       </c>
       <c r="D315">
-        <v>14173</v>
+        <v>14010</v>
       </c>
       <c r="E315">
-        <v>15552</v>
+        <v>15496</v>
       </c>
       <c r="F315">
-        <v>15069</v>
+        <v>15094</v>
       </c>
       <c r="G315">
-        <v>16043</v>
+        <v>15918</v>
       </c>
       <c r="H315">
         <v>0.83</v>
@@ -13402,7 +13385,7 @@
         <v>0.82</v>
       </c>
       <c r="J315">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="K315">
         <v>0.96</v>
@@ -13411,7 +13394,7 @@
         <v>0.95</v>
       </c>
       <c r="M315">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="316" spans="1:13">
@@ -13419,22 +13402,22 @@
         <v>44206</v>
       </c>
       <c r="B316">
-        <v>14231</v>
+        <v>14199</v>
       </c>
       <c r="C316">
-        <v>13734</v>
+        <v>13758</v>
       </c>
       <c r="D316">
-        <v>14724</v>
+        <v>14598</v>
       </c>
       <c r="E316">
-        <v>14821</v>
+        <v>14765</v>
       </c>
       <c r="F316">
-        <v>14363</v>
+        <v>14350</v>
       </c>
       <c r="G316">
-        <v>15296</v>
+        <v>15206</v>
       </c>
       <c r="H316">
         <v>0.78</v>
@@ -13449,10 +13432,10 @@
         <v>0.92</v>
       </c>
       <c r="L316">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="M316">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="317" spans="1:13">
@@ -13460,22 +13443,22 @@
         <v>44207</v>
       </c>
       <c r="B317">
-        <v>16704</v>
+        <v>16758</v>
       </c>
       <c r="C317">
-        <v>16117</v>
+        <v>16203</v>
       </c>
       <c r="D317">
-        <v>17178</v>
+        <v>17316</v>
       </c>
       <c r="E317">
-        <v>15065</v>
+        <v>15025</v>
       </c>
       <c r="F317">
-        <v>14570</v>
+        <v>14553</v>
       </c>
       <c r="G317">
-        <v>15540</v>
+        <v>15499</v>
       </c>
       <c r="H317">
         <v>0.82</v>
@@ -13484,7 +13467,7 @@
         <v>0.8</v>
       </c>
       <c r="J317">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="K317">
         <v>0.88</v>
@@ -13501,28 +13484,28 @@
         <v>44208</v>
       </c>
       <c r="B318">
-        <v>15333</v>
+        <v>15311</v>
       </c>
       <c r="C318">
-        <v>14714</v>
+        <v>14775</v>
       </c>
       <c r="D318">
-        <v>16056</v>
+        <v>15794</v>
       </c>
       <c r="E318">
-        <v>15001</v>
+        <v>14973</v>
       </c>
       <c r="F318">
-        <v>14453</v>
+        <v>14494</v>
       </c>
       <c r="G318">
-        <v>15533</v>
+        <v>15429</v>
       </c>
       <c r="H318">
         <v>0.89</v>
       </c>
       <c r="I318">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
       <c r="J318">
         <v>0.91</v>
@@ -13542,37 +13525,37 @@
         <v>44209</v>
       </c>
       <c r="B319">
-        <v>14564</v>
+        <v>14608</v>
       </c>
       <c r="C319">
-        <v>13767</v>
+        <v>14121</v>
       </c>
       <c r="D319">
-        <v>15148</v>
+        <v>15147</v>
       </c>
       <c r="E319">
-        <v>15208</v>
+        <v>15219</v>
       </c>
       <c r="F319">
-        <v>14583</v>
+        <v>14714</v>
       </c>
       <c r="G319">
-        <v>15777</v>
+        <v>15714</v>
       </c>
       <c r="H319">
         <v>0.98</v>
       </c>
       <c r="I319">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="J319">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="K319">
+        <v>0.89</v>
+      </c>
+      <c r="L319">
         <v>0.88</v>
-      </c>
-      <c r="L319">
-        <v>0.87</v>
       </c>
       <c r="M319">
         <v>0.9</v>
@@ -13583,25 +13566,25 @@
         <v>44210</v>
       </c>
       <c r="B320">
-        <v>13542</v>
+        <v>13568</v>
       </c>
       <c r="C320">
-        <v>12814</v>
+        <v>13000</v>
       </c>
       <c r="D320">
-        <v>14396</v>
+        <v>14161</v>
       </c>
       <c r="E320">
-        <v>15036</v>
+        <v>15061</v>
       </c>
       <c r="F320">
-        <v>14353</v>
+        <v>14525</v>
       </c>
       <c r="G320">
-        <v>15695</v>
+        <v>15604</v>
       </c>
       <c r="H320">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="I320">
         <v>0.99</v>
@@ -13610,7 +13593,7 @@
         <v>1.05</v>
       </c>
       <c r="K320">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="L320">
         <v>0.89</v>
@@ -13624,34 +13607,34 @@
         <v>44211</v>
       </c>
       <c r="B321">
-        <v>13626</v>
+        <v>13514</v>
       </c>
       <c r="C321">
-        <v>12788</v>
+        <v>12887</v>
       </c>
       <c r="D321">
-        <v>14514</v>
+        <v>14085</v>
       </c>
       <c r="E321">
-        <v>14266</v>
+        <v>14250</v>
       </c>
       <c r="F321">
-        <v>13521</v>
+        <v>13696</v>
       </c>
       <c r="G321">
-        <v>15028</v>
+        <v>14797</v>
       </c>
       <c r="H321">
         <v>0.95</v>
       </c>
       <c r="I321">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="J321">
         <v>0.97</v>
       </c>
       <c r="K321">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="L321">
         <v>0.91</v>
@@ -13665,40 +13648,40 @@
         <v>44212</v>
       </c>
       <c r="B322">
-        <v>12170</v>
+        <v>12200</v>
       </c>
       <c r="C322">
-        <v>11192</v>
+        <v>11601</v>
       </c>
       <c r="D322">
-        <v>13063</v>
+        <v>12870</v>
       </c>
       <c r="E322">
-        <v>13476</v>
+        <v>13472</v>
       </c>
       <c r="F322">
-        <v>12640</v>
+        <v>12902</v>
       </c>
       <c r="G322">
-        <v>14280</v>
+        <v>14066</v>
       </c>
       <c r="H322">
         <v>0.9</v>
       </c>
       <c r="I322">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="J322">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="K322">
         <v>0.93</v>
       </c>
       <c r="L322">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="M322">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="323" spans="1:13">
@@ -13706,22 +13689,22 @@
         <v>44213</v>
       </c>
       <c r="B323">
-        <v>12451</v>
+        <v>12522</v>
       </c>
       <c r="C323">
-        <v>11432</v>
+        <v>11865</v>
       </c>
       <c r="D323">
-        <v>13515</v>
+        <v>13197</v>
       </c>
       <c r="E323">
-        <v>12947</v>
+        <v>12951</v>
       </c>
       <c r="F323">
-        <v>12056</v>
+        <v>12338</v>
       </c>
       <c r="G323">
-        <v>13872</v>
+        <v>13578</v>
       </c>
       <c r="H323">
         <v>0.85</v>
@@ -13730,16 +13713,16 @@
         <v>0.82</v>
       </c>
       <c r="J323">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="K323">
         <v>0.94</v>
       </c>
       <c r="L323">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="M323">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="324" spans="1:13">
@@ -13747,40 +13730,40 @@
         <v>44214</v>
       </c>
       <c r="B324">
-        <v>15639</v>
+        <v>15457</v>
       </c>
       <c r="C324">
-        <v>14050</v>
+        <v>14314</v>
       </c>
       <c r="D324">
-        <v>17200</v>
+        <v>16561</v>
       </c>
       <c r="E324">
-        <v>13472</v>
+        <v>13423</v>
       </c>
       <c r="F324">
-        <v>12365</v>
+        <v>12667</v>
       </c>
       <c r="G324">
-        <v>14573</v>
+        <v>14178</v>
       </c>
       <c r="H324">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="I324">
         <v>0.85</v>
       </c>
       <c r="J324">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="K324">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="L324">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="M324">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="325" spans="1:13">
@@ -13788,40 +13771,40 @@
         <v>44215</v>
       </c>
       <c r="B325">
-        <v>14239</v>
+        <v>14082</v>
       </c>
       <c r="C325">
-        <v>12525</v>
+        <v>13000</v>
       </c>
       <c r="D325">
-        <v>15817</v>
+        <v>15339</v>
       </c>
       <c r="E325">
-        <v>13625</v>
+        <v>13565</v>
       </c>
       <c r="F325">
-        <v>12300</v>
+        <v>12695</v>
       </c>
       <c r="G325">
-        <v>14899</v>
+        <v>14492</v>
       </c>
       <c r="H325">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="I325">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="J325">
-        <v>1.01</v>
+        <v>0.99</v>
       </c>
       <c r="K325">
         <v>0.95</v>
       </c>
       <c r="L325">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="M325">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="326" spans="1:13">
@@ -13829,40 +13812,40 @@
         <v>44216</v>
       </c>
       <c r="B326">
-        <v>13039</v>
+        <v>13423</v>
       </c>
       <c r="C326">
-        <v>11074</v>
+        <v>12130</v>
       </c>
       <c r="D326">
-        <v>14710</v>
+        <v>14701</v>
       </c>
       <c r="E326">
-        <v>13842</v>
+        <v>13871</v>
       </c>
       <c r="F326">
-        <v>12270</v>
+        <v>12827</v>
       </c>
       <c r="G326">
-        <v>15310</v>
+        <v>14950</v>
       </c>
       <c r="H326">
         <v>1.03</v>
       </c>
       <c r="I326">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
       <c r="J326">
-        <v>1.1000000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="K326">
         <v>0.94</v>
       </c>
       <c r="L326">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="M326">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="327" spans="1:13">
@@ -13870,40 +13853,40 @@
         <v>44217</v>
       </c>
       <c r="B327">
-        <v>11039</v>
+        <v>11692</v>
       </c>
       <c r="C327">
-        <v>8948</v>
+        <v>10252</v>
       </c>
       <c r="D327">
-        <v>13286</v>
+        <v>12890</v>
       </c>
       <c r="E327">
-        <v>13489</v>
+        <v>13663</v>
       </c>
       <c r="F327">
-        <v>11649</v>
+        <v>12424</v>
       </c>
       <c r="G327">
-        <v>15253</v>
+        <v>14873</v>
       </c>
       <c r="H327">
-        <v>1.04</v>
+        <v>1.06</v>
       </c>
       <c r="I327">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="J327">
-        <v>1.1299999999999999</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K327">
-        <v>0.91</v>
+        <v>0.94</v>
       </c>
       <c r="L327">
-        <v>0.86</v>
+        <v>0.9</v>
       </c>
       <c r="M327">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="328" spans="1:13">
@@ -13911,72 +13894,154 @@
         <v>44218</v>
       </c>
       <c r="B328">
-        <v>9564</v>
+        <v>11651</v>
       </c>
       <c r="C328">
-        <v>6856</v>
+        <v>9798</v>
       </c>
       <c r="D328">
-        <v>12370</v>
+        <v>13200</v>
       </c>
       <c r="E328">
-        <v>11970</v>
+        <v>12712</v>
       </c>
       <c r="F328">
-        <v>9851</v>
+        <v>11295</v>
       </c>
       <c r="G328">
-        <v>14045</v>
+        <v>14033</v>
       </c>
       <c r="H328">
+        <v>0.95</v>
+      </c>
+      <c r="I328">
+        <v>0.88</v>
+      </c>
+      <c r="J328">
+        <v>1.02</v>
+      </c>
+      <c r="K328">
+        <v>0.93</v>
+      </c>
+      <c r="L328">
+        <v>0.9</v>
+      </c>
+      <c r="M328">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="329" spans="1:13">
+      <c r="A329" s="1">
+        <v>44219</v>
+      </c>
+      <c r="B329">
+        <v>10555</v>
+      </c>
+      <c r="C329">
+        <v>8652</v>
+      </c>
+      <c r="D329">
+        <v>12708</v>
+      </c>
+      <c r="E329">
+        <v>11830</v>
+      </c>
+      <c r="F329">
+        <v>10208</v>
+      </c>
+      <c r="G329">
+        <v>13375</v>
+      </c>
+      <c r="H329">
+        <v>0.87</v>
+      </c>
+      <c r="I329">
+        <v>0.81</v>
+      </c>
+      <c r="J329">
+        <v>0.94</v>
+      </c>
+      <c r="K329">
+        <v>0.93</v>
+      </c>
+      <c r="L329">
+        <v>0.88</v>
+      </c>
+      <c r="M329">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="330" spans="1:13">
+      <c r="A330" s="1">
+        <v>44220</v>
+      </c>
+      <c r="B330">
+        <v>10801</v>
+      </c>
+      <c r="C330">
+        <v>7754</v>
+      </c>
+      <c r="D330">
+        <v>13975</v>
+      </c>
+      <c r="E330">
+        <v>11175</v>
+      </c>
+      <c r="F330">
+        <v>9114</v>
+      </c>
+      <c r="G330">
+        <v>13193</v>
+      </c>
+      <c r="H330">
+        <v>0.81</v>
+      </c>
+      <c r="I330">
+        <v>0.73</v>
+      </c>
+      <c r="J330">
         <v>0.89</v>
       </c>
-      <c r="I328">
-        <v>0.81</v>
-      </c>
-      <c r="J328">
-        <v>0.98</v>
-      </c>
-      <c r="K328">
-        <v>0.87</v>
-      </c>
-      <c r="L328">
-        <v>0.82</v>
-      </c>
-      <c r="M328">
+      <c r="K330">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="329" spans="1:13">
-      <c r="A329" s="4">
-        <v>44219</v>
-      </c>
-      <c r="B329">
-        <v>7679</v>
-      </c>
-      <c r="C329">
-        <v>4350</v>
-      </c>
-      <c r="D329">
-        <v>10590</v>
-      </c>
-      <c r="E329">
-        <v>10330</v>
-      </c>
-      <c r="F329">
-        <v>7807</v>
-      </c>
-      <c r="G329">
-        <v>12739</v>
-      </c>
-      <c r="H329">
-        <v>0.76</v>
-      </c>
-      <c r="I329">
-        <v>0.67</v>
-      </c>
-      <c r="J329">
+      <c r="L330">
         <v>0.84</v>
+      </c>
+      <c r="M330">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="331" spans="1:13">
+      <c r="A331" s="1">
+        <v>44221</v>
+      </c>
+      <c r="B331">
+        <v>13547</v>
+      </c>
+      <c r="C331">
+        <v>7803</v>
+      </c>
+      <c r="D331">
+        <v>18671</v>
+      </c>
+      <c r="E331">
+        <v>11638</v>
+      </c>
+      <c r="F331">
+        <v>8502</v>
+      </c>
+      <c r="G331">
+        <v>14638</v>
+      </c>
+      <c r="H331">
+        <v>0.85</v>
+      </c>
+      <c r="I331">
+        <v>0.72</v>
+      </c>
+      <c r="J331">
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add RKI data downloaded 2021-03-26--19-15-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Nowcasting_Zahlen.xlsx
+++ b/rki-data/RKI-Nowcasting_Zahlen.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF60395-2DB3-4D11-894E-78E8EAFA7414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A85AB7E-556C-4AD5-B460-7A09A0930139}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13845" windowHeight="13965" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7515" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="1" r:id="rId1"/>
     <sheet name="Nowcast_R" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="411">
   <si>
     <t>Erläuterung</t>
   </si>
@@ -27,7 +27,7 @@
     <t>Ergebnisse des Nowcastings und der Schätzung der Reproduktionszahl R</t>
   </si>
   <si>
-    <t>Datenstand: 2021-03-25, 00:00 Uhr</t>
+    <t>Datenstand: 2021-03-26, 00:00 Uhr</t>
   </si>
   <si>
     <t>Die Ergebnisse des Nowcastings, also die Schätzung der Anzahl von COVID-19 Neuerkrankungen wird dargestellt mit einem gleitenden 4-Tages-Mittelwert.</t>
@@ -36,7 +36,7 @@
     <t>Dabei wird jeder Wert mit den Werten der 3 vorhergehenden Tage gemittelt.</t>
   </si>
   <si>
-    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-03-25 dargestellten Nowcasting-Kurve.</t>
+    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-03-26 dargestellten Nowcasting-Kurve.</t>
   </si>
   <si>
     <t>Der letzte Schätzwert der Reproduktionszahl R wird ebenfalls im gleichen Lagebericht erwähnt.</t>
@@ -1207,6 +1207,9 @@
   </si>
   <si>
     <t>21.03.2021</t>
+  </si>
+  <si>
+    <t>22.03.2021</t>
   </si>
   <si>
     <t>Punktschätzer der Anzahl Neuerkrankungen (ohne Glättung)</t>
@@ -1281,7 +1284,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1601,9 +1604,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1703,15 +1708,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M386"/>
+  <dimension ref="A1:M387"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:M386"/>
+      <selection activeCell="H6" sqref="H6:M387"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="13" width="19.7109375" customWidth="1"/>
+    <col min="1" max="13" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="90">
@@ -1719,40 +1724,40 @@
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>408</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1778,22 +1783,22 @@
         <v>238</v>
       </c>
       <c r="H2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1819,22 +1824,22 @@
         <v>276</v>
       </c>
       <c r="H3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1860,22 +1865,22 @@
         <v>342</v>
       </c>
       <c r="H4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M4" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1901,22 +1906,22 @@
         <v>412</v>
       </c>
       <c r="H5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="K5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="L5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M5" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -15009,7 +15014,7 @@
         <v>13668</v>
       </c>
       <c r="D325" s="2">
-        <v>13965</v>
+        <v>13966</v>
       </c>
       <c r="E325" s="2">
         <v>13274</v>
@@ -15047,10 +15052,10 @@
         <v>13187</v>
       </c>
       <c r="C326" s="2">
-        <v>13043</v>
+        <v>13041</v>
       </c>
       <c r="D326" s="2">
-        <v>13348</v>
+        <v>13347</v>
       </c>
       <c r="E326" s="2">
         <v>13576</v>
@@ -15088,16 +15093,16 @@
         <v>11600</v>
       </c>
       <c r="C327" s="2">
-        <v>11432</v>
+        <v>11431</v>
       </c>
       <c r="D327" s="2">
-        <v>11742</v>
+        <v>11741</v>
       </c>
       <c r="E327" s="2">
         <v>13475</v>
       </c>
       <c r="F327" s="2">
-        <v>13313</v>
+        <v>13312</v>
       </c>
       <c r="G327" s="2">
         <v>13620</v>
@@ -15129,7 +15134,7 @@
         <v>11472</v>
       </c>
       <c r="C328" s="2">
-        <v>11329</v>
+        <v>11327</v>
       </c>
       <c r="D328" s="2">
         <v>11597</v>
@@ -15138,10 +15143,10 @@
         <v>12521</v>
       </c>
       <c r="F328" s="2">
-        <v>12368</v>
+        <v>12367</v>
       </c>
       <c r="G328" s="2">
-        <v>12663</v>
+        <v>12662</v>
       </c>
       <c r="H328" s="3">
         <v>0.95</v>
@@ -15173,16 +15178,16 @@
         <v>10122</v>
       </c>
       <c r="D329" s="2">
-        <v>10400</v>
+        <v>10399</v>
       </c>
       <c r="E329" s="2">
         <v>11631</v>
       </c>
       <c r="F329" s="2">
-        <v>11481</v>
+        <v>11480</v>
       </c>
       <c r="G329" s="2">
-        <v>11772</v>
+        <v>11771</v>
       </c>
       <c r="H329" s="3">
         <v>0.88</v>
@@ -15208,22 +15213,22 @@
         <v>340</v>
       </c>
       <c r="B330" s="2">
-        <v>9925</v>
+        <v>9924</v>
       </c>
       <c r="C330" s="2">
-        <v>9797</v>
+        <v>9796</v>
       </c>
       <c r="D330" s="2">
-        <v>10049</v>
+        <v>10050</v>
       </c>
       <c r="E330" s="2">
         <v>10815</v>
       </c>
       <c r="F330" s="2">
-        <v>10670</v>
+        <v>10669</v>
       </c>
       <c r="G330" s="2">
-        <v>10947</v>
+        <v>10946</v>
       </c>
       <c r="H330" s="3">
         <v>0.8</v>
@@ -15252,16 +15257,16 @@
         <v>12463</v>
       </c>
       <c r="C331" s="2">
-        <v>12338</v>
+        <v>12337</v>
       </c>
       <c r="D331" s="2">
-        <v>12592</v>
+        <v>12589</v>
       </c>
       <c r="E331" s="2">
         <v>11031</v>
       </c>
       <c r="F331" s="2">
-        <v>10896</v>
+        <v>10895</v>
       </c>
       <c r="G331" s="2">
         <v>11159</v>
@@ -15296,16 +15301,16 @@
         <v>11147</v>
       </c>
       <c r="D332" s="2">
-        <v>11398</v>
+        <v>11399</v>
       </c>
       <c r="E332" s="2">
         <v>10982</v>
       </c>
       <c r="F332" s="2">
-        <v>10851</v>
+        <v>10850</v>
       </c>
       <c r="G332" s="2">
-        <v>11110</v>
+        <v>11109</v>
       </c>
       <c r="H332" s="3">
         <v>0.88</v>
@@ -15331,22 +15336,22 @@
         <v>343</v>
       </c>
       <c r="B333" s="2">
-        <v>10264</v>
+        <v>10265</v>
       </c>
       <c r="C333" s="2">
         <v>10154</v>
       </c>
       <c r="D333" s="2">
-        <v>10386</v>
+        <v>10383</v>
       </c>
       <c r="E333" s="2">
-        <v>10982</v>
+        <v>10983</v>
       </c>
       <c r="F333" s="2">
-        <v>10859</v>
+        <v>10858</v>
       </c>
       <c r="G333" s="2">
-        <v>11106</v>
+        <v>11105</v>
       </c>
       <c r="H333" s="3">
         <v>0.94</v>
@@ -15378,16 +15383,16 @@
         <v>9622</v>
       </c>
       <c r="D334" s="2">
-        <v>9882</v>
+        <v>9881</v>
       </c>
       <c r="E334" s="2">
-        <v>10939</v>
+        <v>10940</v>
       </c>
       <c r="F334" s="2">
         <v>10815</v>
       </c>
       <c r="G334" s="2">
-        <v>11064</v>
+        <v>11063</v>
       </c>
       <c r="H334" s="3">
         <v>1.01</v>
@@ -15416,19 +15421,19 @@
         <v>9360</v>
       </c>
       <c r="C335" s="2">
-        <v>9204</v>
+        <v>9203</v>
       </c>
       <c r="D335" s="2">
-        <v>9522</v>
+        <v>9521</v>
       </c>
       <c r="E335" s="2">
         <v>10164</v>
       </c>
       <c r="F335" s="2">
-        <v>10032</v>
+        <v>10031</v>
       </c>
       <c r="G335" s="2">
-        <v>10297</v>
+        <v>10296</v>
       </c>
       <c r="H335" s="3">
         <v>0.92</v>
@@ -15457,19 +15462,19 @@
         <v>8288</v>
       </c>
       <c r="C336" s="2">
-        <v>8160</v>
+        <v>8163</v>
       </c>
       <c r="D336" s="2">
-        <v>8401</v>
+        <v>8399</v>
       </c>
       <c r="E336" s="2">
         <v>9416</v>
       </c>
       <c r="F336" s="2">
-        <v>9285</v>
+        <v>9286</v>
       </c>
       <c r="G336" s="2">
-        <v>9548</v>
+        <v>9546</v>
       </c>
       <c r="H336" s="3">
         <v>0.86</v>
@@ -15495,13 +15500,13 @@
         <v>347</v>
       </c>
       <c r="B337" s="2">
-        <v>8041</v>
+        <v>8040</v>
       </c>
       <c r="C337" s="2">
-        <v>7899</v>
+        <v>7897</v>
       </c>
       <c r="D337" s="2">
-        <v>8152</v>
+        <v>8155</v>
       </c>
       <c r="E337" s="2">
         <v>8860</v>
@@ -15539,13 +15544,13 @@
         <v>10341</v>
       </c>
       <c r="C338" s="2">
-        <v>10250</v>
+        <v>10248</v>
       </c>
       <c r="D338" s="2">
         <v>10461</v>
       </c>
       <c r="E338" s="2">
-        <v>9008</v>
+        <v>9007</v>
       </c>
       <c r="F338" s="2">
         <v>8878</v>
@@ -15577,22 +15582,22 @@
         <v>349</v>
       </c>
       <c r="B339" s="2">
-        <v>9444</v>
+        <v>9442</v>
       </c>
       <c r="C339" s="2">
-        <v>9340</v>
+        <v>9337</v>
       </c>
       <c r="D339" s="2">
-        <v>9546</v>
+        <v>9540</v>
       </c>
       <c r="E339" s="2">
-        <v>9029</v>
+        <v>9028</v>
       </c>
       <c r="F339" s="2">
-        <v>8912</v>
+        <v>8911</v>
       </c>
       <c r="G339" s="2">
-        <v>9140</v>
+        <v>9138</v>
       </c>
       <c r="H339" s="3">
         <v>0.89</v>
@@ -15618,22 +15623,22 @@
         <v>350</v>
       </c>
       <c r="B340" s="2">
-        <v>8675</v>
+        <v>8673</v>
       </c>
       <c r="C340" s="2">
-        <v>8577</v>
+        <v>8573</v>
       </c>
       <c r="D340" s="2">
-        <v>8793</v>
+        <v>8789</v>
       </c>
       <c r="E340" s="2">
-        <v>9125</v>
+        <v>9124</v>
       </c>
       <c r="F340" s="2">
-        <v>9016</v>
+        <v>9014</v>
       </c>
       <c r="G340" s="2">
-        <v>9238</v>
+        <v>9236</v>
       </c>
       <c r="H340" s="3">
         <v>0.97</v>
@@ -15659,22 +15664,22 @@
         <v>351</v>
       </c>
       <c r="B341" s="2">
-        <v>7753</v>
+        <v>7752</v>
       </c>
       <c r="C341" s="2">
-        <v>7659</v>
+        <v>7662</v>
       </c>
       <c r="D341" s="2">
-        <v>7853</v>
+        <v>7847</v>
       </c>
       <c r="E341" s="2">
-        <v>9053</v>
+        <v>9052</v>
       </c>
       <c r="F341" s="2">
-        <v>8956</v>
+        <v>8955</v>
       </c>
       <c r="G341" s="2">
-        <v>9163</v>
+        <v>9159</v>
       </c>
       <c r="H341" s="3">
         <v>1.02</v>
@@ -15700,22 +15705,22 @@
         <v>352</v>
       </c>
       <c r="B342" s="2">
-        <v>7522</v>
+        <v>7524</v>
       </c>
       <c r="C342" s="2">
-        <v>7397</v>
+        <v>7392</v>
       </c>
       <c r="D342" s="2">
-        <v>7631</v>
+        <v>7637</v>
       </c>
       <c r="E342" s="2">
-        <v>8349</v>
+        <v>8348</v>
       </c>
       <c r="F342" s="2">
-        <v>8243</v>
+        <v>8241</v>
       </c>
       <c r="G342" s="2">
-        <v>8456</v>
+        <v>8453</v>
       </c>
       <c r="H342" s="3">
         <v>0.93</v>
@@ -15741,22 +15746,22 @@
         <v>353</v>
       </c>
       <c r="B343" s="2">
-        <v>6735</v>
+        <v>6736</v>
       </c>
       <c r="C343" s="2">
-        <v>6649</v>
+        <v>6644</v>
       </c>
       <c r="D343" s="2">
-        <v>6850</v>
+        <v>6842</v>
       </c>
       <c r="E343" s="2">
         <v>7671</v>
       </c>
       <c r="F343" s="2">
-        <v>7570</v>
+        <v>7567</v>
       </c>
       <c r="G343" s="2">
-        <v>7782</v>
+        <v>7778</v>
       </c>
       <c r="H343" s="3">
         <v>0.85</v>
@@ -15774,7 +15779,7 @@
         <v>0.89</v>
       </c>
       <c r="M343" s="3">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="344" spans="1:13">
@@ -15785,19 +15790,19 @@
         <v>6434</v>
       </c>
       <c r="C344" s="2">
-        <v>6342</v>
+        <v>6341</v>
       </c>
       <c r="D344" s="2">
-        <v>6527</v>
+        <v>6525</v>
       </c>
       <c r="E344" s="2">
         <v>7111</v>
       </c>
       <c r="F344" s="2">
-        <v>7012</v>
+        <v>7009</v>
       </c>
       <c r="G344" s="2">
-        <v>7215</v>
+        <v>7213</v>
       </c>
       <c r="H344" s="3">
         <v>0.78</v>
@@ -15823,22 +15828,22 @@
         <v>355</v>
       </c>
       <c r="B345" s="2">
-        <v>8133</v>
+        <v>8136</v>
       </c>
       <c r="C345" s="2">
-        <v>8008</v>
+        <v>8009</v>
       </c>
       <c r="D345" s="2">
-        <v>8250</v>
+        <v>8240</v>
       </c>
       <c r="E345" s="2">
-        <v>7206</v>
+        <v>7207</v>
       </c>
       <c r="F345" s="2">
-        <v>7099</v>
+        <v>7096</v>
       </c>
       <c r="G345" s="2">
-        <v>7314</v>
+        <v>7311</v>
       </c>
       <c r="H345" s="3">
         <v>0.8</v>
@@ -15856,7 +15861,7 @@
         <v>0.88</v>
       </c>
       <c r="M345" s="3">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="346" spans="1:13">
@@ -15864,22 +15869,22 @@
         <v>356</v>
       </c>
       <c r="B346" s="2">
-        <v>7686</v>
+        <v>7685</v>
       </c>
       <c r="C346" s="2">
-        <v>7586</v>
+        <v>7585</v>
       </c>
       <c r="D346" s="2">
-        <v>7790</v>
+        <v>7789</v>
       </c>
       <c r="E346" s="2">
-        <v>7247</v>
+        <v>7248</v>
       </c>
       <c r="F346" s="2">
-        <v>7146</v>
+        <v>7144</v>
       </c>
       <c r="G346" s="2">
-        <v>7354</v>
+        <v>7349</v>
       </c>
       <c r="H346" s="3">
         <v>0.87</v>
@@ -15905,22 +15910,22 @@
         <v>357</v>
       </c>
       <c r="B347" s="2">
-        <v>7429</v>
+        <v>7432</v>
       </c>
       <c r="C347" s="2">
-        <v>7312</v>
+        <v>7315</v>
       </c>
       <c r="D347" s="2">
-        <v>7520</v>
+        <v>7522</v>
       </c>
       <c r="E347" s="2">
-        <v>7421</v>
+        <v>7422</v>
       </c>
       <c r="F347" s="2">
         <v>7312</v>
       </c>
       <c r="G347" s="2">
-        <v>7522</v>
+        <v>7519</v>
       </c>
       <c r="H347" s="3">
         <v>0.97</v>
@@ -15935,7 +15940,7 @@
         <v>0.89</v>
       </c>
       <c r="L347" s="3">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="M347" s="3">
         <v>0.89</v>
@@ -15946,22 +15951,22 @@
         <v>358</v>
       </c>
       <c r="B348" s="2">
-        <v>6686</v>
+        <v>6690</v>
       </c>
       <c r="C348" s="2">
-        <v>6575</v>
+        <v>6600</v>
       </c>
       <c r="D348" s="2">
-        <v>6795</v>
+        <v>6789</v>
       </c>
       <c r="E348" s="2">
-        <v>7484</v>
+        <v>7486</v>
       </c>
       <c r="F348" s="2">
-        <v>7370</v>
+        <v>7377</v>
       </c>
       <c r="G348" s="2">
-        <v>7588</v>
+        <v>7585</v>
       </c>
       <c r="H348" s="3">
         <v>1.05</v>
@@ -15987,22 +15992,22 @@
         <v>359</v>
       </c>
       <c r="B349" s="2">
-        <v>6910</v>
+        <v>6912</v>
       </c>
       <c r="C349" s="2">
-        <v>6818</v>
+        <v>6819</v>
       </c>
       <c r="D349" s="2">
-        <v>7038</v>
+        <v>7030</v>
       </c>
       <c r="E349" s="2">
-        <v>7178</v>
+        <v>7180</v>
       </c>
       <c r="F349" s="2">
-        <v>7073</v>
+        <v>7079</v>
       </c>
       <c r="G349" s="2">
-        <v>7286</v>
+        <v>7282</v>
       </c>
       <c r="H349" s="3">
         <v>1</v>
@@ -16028,22 +16033,22 @@
         <v>360</v>
       </c>
       <c r="B350" s="2">
-        <v>6424</v>
+        <v>6423</v>
       </c>
       <c r="C350" s="2">
-        <v>6329</v>
+        <v>6317</v>
       </c>
       <c r="D350" s="2">
-        <v>6519</v>
+        <v>6515</v>
       </c>
       <c r="E350" s="2">
-        <v>6862</v>
+        <v>6864</v>
       </c>
       <c r="F350" s="2">
-        <v>6758</v>
+        <v>6763</v>
       </c>
       <c r="G350" s="2">
-        <v>6968</v>
+        <v>6964</v>
       </c>
       <c r="H350" s="3">
         <v>0.95</v>
@@ -16069,22 +16074,22 @@
         <v>361</v>
       </c>
       <c r="B351" s="2">
-        <v>6623</v>
+        <v>6625</v>
       </c>
       <c r="C351" s="2">
-        <v>6520</v>
+        <v>6512</v>
       </c>
       <c r="D351" s="2">
-        <v>6713</v>
+        <v>6721</v>
       </c>
       <c r="E351" s="2">
-        <v>6661</v>
+        <v>6663</v>
       </c>
       <c r="F351" s="2">
-        <v>6560</v>
+        <v>6562</v>
       </c>
       <c r="G351" s="2">
-        <v>6766</v>
+        <v>6764</v>
       </c>
       <c r="H351" s="3">
         <v>0.9</v>
@@ -16110,22 +16115,22 @@
         <v>362</v>
       </c>
       <c r="B352" s="2">
-        <v>8535</v>
+        <v>8538</v>
       </c>
       <c r="C352" s="2">
-        <v>8437</v>
+        <v>8425</v>
       </c>
       <c r="D352" s="2">
-        <v>8632</v>
+        <v>8661</v>
       </c>
       <c r="E352" s="2">
-        <v>7123</v>
+        <v>7124</v>
       </c>
       <c r="F352" s="2">
-        <v>7026</v>
+        <v>7018</v>
       </c>
       <c r="G352" s="2">
-        <v>7225</v>
+        <v>7232</v>
       </c>
       <c r="H352" s="3">
         <v>0.95</v>
@@ -16151,31 +16156,31 @@
         <v>363</v>
       </c>
       <c r="B353" s="2">
-        <v>8153</v>
+        <v>8146</v>
       </c>
       <c r="C353" s="2">
-        <v>8031</v>
+        <v>8051</v>
       </c>
       <c r="D353" s="2">
-        <v>8276</v>
+        <v>8253</v>
       </c>
       <c r="E353" s="2">
-        <v>7434</v>
+        <v>7433</v>
       </c>
       <c r="F353" s="2">
-        <v>7329</v>
+        <v>7326</v>
       </c>
       <c r="G353" s="2">
-        <v>7535</v>
+        <v>7537</v>
       </c>
       <c r="H353" s="3">
         <v>1.04</v>
       </c>
       <c r="I353" s="3">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="J353" s="3">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
       <c r="K353" s="3">
         <v>1.03</v>
@@ -16192,22 +16197,22 @@
         <v>364</v>
       </c>
       <c r="B354" s="2">
-        <v>8072</v>
+        <v>8071</v>
       </c>
       <c r="C354" s="2">
-        <v>7954</v>
+        <v>7963</v>
       </c>
       <c r="D354" s="2">
-        <v>8166</v>
+        <v>8198</v>
       </c>
       <c r="E354" s="2">
-        <v>7846</v>
+        <v>7845</v>
       </c>
       <c r="F354" s="2">
-        <v>7735</v>
+        <v>7738</v>
       </c>
       <c r="G354" s="2">
-        <v>7947</v>
+        <v>7958</v>
       </c>
       <c r="H354" s="3">
         <v>1.1399999999999999</v>
@@ -16233,28 +16238,28 @@
         <v>365</v>
       </c>
       <c r="B355" s="2">
-        <v>7729</v>
+        <v>7722</v>
       </c>
       <c r="C355" s="2">
-        <v>7620</v>
+        <v>7601</v>
       </c>
       <c r="D355" s="2">
-        <v>7844</v>
+        <v>7825</v>
       </c>
       <c r="E355" s="2">
-        <v>8122</v>
+        <v>8119</v>
       </c>
       <c r="F355" s="2">
         <v>8010</v>
       </c>
       <c r="G355" s="2">
-        <v>8229</v>
+        <v>8234</v>
       </c>
       <c r="H355" s="3">
         <v>1.22</v>
       </c>
       <c r="I355" s="3">
-        <v>1.21</v>
+        <v>1.2</v>
       </c>
       <c r="J355" s="3">
         <v>1.23</v>
@@ -16274,22 +16279,22 @@
         <v>366</v>
       </c>
       <c r="B356" s="2">
-        <v>7678</v>
+        <v>7672</v>
       </c>
       <c r="C356" s="2">
-        <v>7568</v>
+        <v>7563</v>
       </c>
       <c r="D356" s="2">
-        <v>7777</v>
+        <v>7780</v>
       </c>
       <c r="E356" s="2">
-        <v>7908</v>
+        <v>7903</v>
       </c>
       <c r="F356" s="2">
-        <v>7793</v>
+        <v>7795</v>
       </c>
       <c r="G356" s="2">
-        <v>8016</v>
+        <v>8014</v>
       </c>
       <c r="H356" s="3">
         <v>1.1100000000000001</v>
@@ -16315,22 +16320,22 @@
         <v>367</v>
       </c>
       <c r="B357" s="2">
-        <v>7360</v>
+        <v>7355</v>
       </c>
       <c r="C357" s="2">
-        <v>7238</v>
+        <v>7263</v>
       </c>
       <c r="D357" s="2">
-        <v>7449</v>
+        <v>7446</v>
       </c>
       <c r="E357" s="2">
-        <v>7710</v>
+        <v>7705</v>
       </c>
       <c r="F357" s="2">
-        <v>7595</v>
+        <v>7597</v>
       </c>
       <c r="G357" s="2">
-        <v>7809</v>
+        <v>7812</v>
       </c>
       <c r="H357" s="3">
         <v>1.04</v>
@@ -16356,22 +16361,22 @@
         <v>368</v>
       </c>
       <c r="B358" s="2">
-        <v>7135</v>
+        <v>7129</v>
       </c>
       <c r="C358" s="2">
-        <v>7045</v>
+        <v>7023</v>
       </c>
       <c r="D358" s="2">
-        <v>7246</v>
+        <v>7235</v>
       </c>
       <c r="E358" s="2">
-        <v>7475</v>
+        <v>7470</v>
       </c>
       <c r="F358" s="2">
-        <v>7368</v>
+        <v>7362</v>
       </c>
       <c r="G358" s="2">
-        <v>7579</v>
+        <v>7571</v>
       </c>
       <c r="H358" s="3">
         <v>0.95</v>
@@ -16397,22 +16402,22 @@
         <v>369</v>
       </c>
       <c r="B359" s="2">
-        <v>8945</v>
+        <v>8950</v>
       </c>
       <c r="C359" s="2">
-        <v>8850</v>
+        <v>8823</v>
       </c>
       <c r="D359" s="2">
-        <v>9055</v>
+        <v>9081</v>
       </c>
       <c r="E359" s="2">
-        <v>7779</v>
+        <v>7776</v>
       </c>
       <c r="F359" s="2">
-        <v>7675</v>
+        <v>7668</v>
       </c>
       <c r="G359" s="2">
-        <v>7881</v>
+        <v>7885</v>
       </c>
       <c r="H359" s="3">
         <v>0.96</v>
@@ -16438,22 +16443,22 @@
         <v>370</v>
       </c>
       <c r="B360" s="2">
-        <v>8507</v>
+        <v>8509</v>
       </c>
       <c r="C360" s="2">
-        <v>8354</v>
+        <v>8389</v>
       </c>
       <c r="D360" s="2">
-        <v>8661</v>
+        <v>8621</v>
       </c>
       <c r="E360" s="2">
-        <v>7987</v>
+        <v>7986</v>
       </c>
       <c r="F360" s="2">
-        <v>7872</v>
+        <v>7874</v>
       </c>
       <c r="G360" s="2">
-        <v>8103</v>
+        <v>8096</v>
       </c>
       <c r="H360" s="3">
         <v>1.01</v>
@@ -16479,22 +16484,22 @@
         <v>371</v>
       </c>
       <c r="B361" s="2">
-        <v>8089</v>
+        <v>8091</v>
       </c>
       <c r="C361" s="2">
-        <v>7955</v>
+        <v>7949</v>
       </c>
       <c r="D361" s="2">
-        <v>8212</v>
+        <v>8230</v>
       </c>
       <c r="E361" s="2">
-        <v>8169</v>
+        <v>8170</v>
       </c>
       <c r="F361" s="2">
-        <v>8051</v>
+        <v>8046</v>
       </c>
       <c r="G361" s="2">
-        <v>8294</v>
+        <v>8292</v>
       </c>
       <c r="H361" s="3">
         <v>1.06</v>
@@ -16520,13 +16525,13 @@
         <v>372</v>
       </c>
       <c r="B362" s="2">
-        <v>7685</v>
+        <v>7675</v>
       </c>
       <c r="C362" s="2">
-        <v>7532</v>
+        <v>7529</v>
       </c>
       <c r="D362" s="2">
-        <v>7825</v>
+        <v>7789</v>
       </c>
       <c r="E362" s="2">
         <v>8306</v>
@@ -16535,7 +16540,7 @@
         <v>8173</v>
       </c>
       <c r="G362" s="2">
-        <v>8439</v>
+        <v>8430</v>
       </c>
       <c r="H362" s="3">
         <v>1.1100000000000001</v>
@@ -16561,22 +16566,22 @@
         <v>373</v>
       </c>
       <c r="B363" s="2">
-        <v>7973</v>
+        <v>7951</v>
       </c>
       <c r="C363" s="2">
-        <v>7864</v>
+        <v>7803</v>
       </c>
       <c r="D363" s="2">
-        <v>8119</v>
+        <v>8080</v>
       </c>
       <c r="E363" s="2">
-        <v>8063</v>
+        <v>8057</v>
       </c>
       <c r="F363" s="2">
-        <v>7926</v>
+        <v>7917</v>
       </c>
       <c r="G363" s="2">
-        <v>8205</v>
+        <v>8180</v>
       </c>
       <c r="H363" s="3">
         <v>1.04</v>
@@ -16602,22 +16607,22 @@
         <v>374</v>
       </c>
       <c r="B364" s="2">
-        <v>7205</v>
+        <v>7188</v>
       </c>
       <c r="C364" s="2">
-        <v>7072</v>
+        <v>7064</v>
       </c>
       <c r="D364" s="2">
-        <v>7333</v>
+        <v>7310</v>
       </c>
       <c r="E364" s="2">
-        <v>7738</v>
+        <v>7726</v>
       </c>
       <c r="F364" s="2">
-        <v>7606</v>
+        <v>7586</v>
       </c>
       <c r="G364" s="2">
-        <v>7872</v>
+        <v>7852</v>
       </c>
       <c r="H364" s="3">
         <v>0.97</v>
@@ -16643,28 +16648,28 @@
         <v>375</v>
       </c>
       <c r="B365" s="2">
-        <v>7380</v>
+        <v>7368</v>
       </c>
       <c r="C365" s="2">
-        <v>7244</v>
+        <v>7235</v>
       </c>
       <c r="D365" s="2">
-        <v>7522</v>
+        <v>7494</v>
       </c>
       <c r="E365" s="2">
-        <v>7561</v>
+        <v>7545</v>
       </c>
       <c r="F365" s="2">
-        <v>7428</v>
+        <v>7408</v>
       </c>
       <c r="G365" s="2">
-        <v>7700</v>
+        <v>7668</v>
       </c>
       <c r="H365" s="3">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="I365" s="3">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="J365" s="3">
         <v>0.93</v>
@@ -16684,22 +16689,22 @@
         <v>376</v>
       </c>
       <c r="B366" s="2">
-        <v>9545</v>
+        <v>9559</v>
       </c>
       <c r="C366" s="2">
-        <v>9372</v>
+        <v>9409</v>
       </c>
       <c r="D366" s="2">
-        <v>9695</v>
+        <v>9743</v>
       </c>
       <c r="E366" s="2">
-        <v>8025</v>
+        <v>8016</v>
       </c>
       <c r="F366" s="2">
-        <v>7888</v>
+        <v>7878</v>
       </c>
       <c r="G366" s="2">
-        <v>8167</v>
+        <v>8157</v>
       </c>
       <c r="H366" s="3">
         <v>0.97</v>
@@ -16725,25 +16730,25 @@
         <v>377</v>
       </c>
       <c r="B367" s="2">
-        <v>8929</v>
+        <v>8950</v>
       </c>
       <c r="C367" s="2">
-        <v>8778</v>
+        <v>8815</v>
       </c>
       <c r="D367" s="2">
-        <v>9109</v>
+        <v>9105</v>
       </c>
       <c r="E367" s="2">
-        <v>8265</v>
+        <v>8266</v>
       </c>
       <c r="F367" s="2">
-        <v>8116</v>
+        <v>8131</v>
       </c>
       <c r="G367" s="2">
-        <v>8415</v>
+        <v>8413</v>
       </c>
       <c r="H367" s="3">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="I367" s="3">
         <v>1.01</v>
@@ -16758,7 +16763,7 @@
         <v>1.03</v>
       </c>
       <c r="M367" s="3">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="368" spans="1:13">
@@ -16766,25 +16771,25 @@
         <v>378</v>
       </c>
       <c r="B368" s="2">
-        <v>8930</v>
+        <v>8952</v>
       </c>
       <c r="C368" s="2">
-        <v>8799</v>
+        <v>8784</v>
       </c>
       <c r="D368" s="2">
-        <v>9084</v>
+        <v>9149</v>
       </c>
       <c r="E368" s="2">
-        <v>8696</v>
+        <v>8707</v>
       </c>
       <c r="F368" s="2">
-        <v>8548</v>
+        <v>8561</v>
       </c>
       <c r="G368" s="2">
-        <v>8852</v>
+        <v>8873</v>
       </c>
       <c r="H368" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="I368" s="3">
         <v>1.1100000000000001</v>
@@ -16807,28 +16812,28 @@
         <v>379</v>
       </c>
       <c r="B369" s="2">
-        <v>8621</v>
+        <v>8656</v>
       </c>
       <c r="C369" s="2">
-        <v>8482</v>
+        <v>8512</v>
       </c>
       <c r="D369" s="2">
-        <v>8780</v>
+        <v>8827</v>
       </c>
       <c r="E369" s="2">
-        <v>9006</v>
+        <v>9029</v>
       </c>
       <c r="F369" s="2">
-        <v>8858</v>
+        <v>8880</v>
       </c>
       <c r="G369" s="2">
-        <v>9167</v>
+        <v>9206</v>
       </c>
       <c r="H369" s="3">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="I369" s="3">
-        <v>1.17</v>
+        <v>1.18</v>
       </c>
       <c r="J369" s="3">
         <v>1.21</v>
@@ -16840,7 +16845,7 @@
         <v>1.05</v>
       </c>
       <c r="M369" s="3">
-        <v>1.06</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="370" spans="1:13">
@@ -16848,28 +16853,28 @@
         <v>380</v>
       </c>
       <c r="B370" s="2">
-        <v>8994</v>
+        <v>9020</v>
       </c>
       <c r="C370" s="2">
-        <v>8796</v>
+        <v>8846</v>
       </c>
       <c r="D370" s="2">
-        <v>9149</v>
+        <v>9172</v>
       </c>
       <c r="E370" s="2">
-        <v>8868</v>
+        <v>8895</v>
       </c>
       <c r="F370" s="2">
-        <v>8714</v>
+        <v>8739</v>
       </c>
       <c r="G370" s="2">
-        <v>9030</v>
+        <v>9063</v>
       </c>
       <c r="H370" s="3">
         <v>1.1100000000000001</v>
       </c>
       <c r="I370" s="3">
-        <v>1.0900000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J370" s="3">
         <v>1.1200000000000001</v>
@@ -16889,22 +16894,22 @@
         <v>381</v>
       </c>
       <c r="B371" s="2">
-        <v>8852</v>
+        <v>8897</v>
       </c>
       <c r="C371" s="2">
-        <v>8683</v>
+        <v>8684</v>
       </c>
       <c r="D371" s="2">
-        <v>9005</v>
+        <v>9111</v>
       </c>
       <c r="E371" s="2">
-        <v>8849</v>
+        <v>8881</v>
       </c>
       <c r="F371" s="2">
-        <v>8690</v>
+        <v>8707</v>
       </c>
       <c r="G371" s="2">
-        <v>9004</v>
+        <v>9065</v>
       </c>
       <c r="H371" s="3">
         <v>1.07</v>
@@ -16913,10 +16918,10 @@
         <v>1.06</v>
       </c>
       <c r="J371" s="3">
-        <v>1.08</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="K371" s="3">
-        <v>1.0900000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L371" s="3">
         <v>1.0900000000000001</v>
@@ -16933,19 +16938,19 @@
         <v>9102</v>
       </c>
       <c r="C372" s="2">
-        <v>8904</v>
+        <v>8921</v>
       </c>
       <c r="D372" s="2">
-        <v>9296</v>
+        <v>9264</v>
       </c>
       <c r="E372" s="2">
-        <v>8892</v>
+        <v>8919</v>
       </c>
       <c r="F372" s="2">
-        <v>8716</v>
+        <v>8741</v>
       </c>
       <c r="G372" s="2">
-        <v>9057</v>
+        <v>9094</v>
       </c>
       <c r="H372" s="3">
         <v>1.02</v>
@@ -16957,10 +16962,10 @@
         <v>1.04</v>
       </c>
       <c r="K372" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="L372" s="3">
         <v>1.1100000000000001</v>
-      </c>
-      <c r="L372" s="3">
-        <v>1.1000000000000001</v>
       </c>
       <c r="M372" s="3">
         <v>1.1200000000000001</v>
@@ -16971,22 +16976,22 @@
         <v>383</v>
       </c>
       <c r="B373" s="2">
-        <v>11841</v>
+        <v>11814</v>
       </c>
       <c r="C373" s="2">
-        <v>11482</v>
+        <v>11463</v>
       </c>
       <c r="D373" s="2">
-        <v>12129</v>
+        <v>12042</v>
       </c>
       <c r="E373" s="2">
-        <v>9697</v>
+        <v>9708</v>
       </c>
       <c r="F373" s="2">
-        <v>9466</v>
+        <v>9479</v>
       </c>
       <c r="G373" s="2">
-        <v>9895</v>
+        <v>9897</v>
       </c>
       <c r="H373" s="3">
         <v>1.08</v>
@@ -17012,22 +17017,22 @@
         <v>384</v>
       </c>
       <c r="B374" s="2">
-        <v>11507</v>
+        <v>11520</v>
       </c>
       <c r="C374" s="2">
-        <v>11148</v>
+        <v>11163</v>
       </c>
       <c r="D374" s="2">
-        <v>11897</v>
+        <v>11851</v>
       </c>
       <c r="E374" s="2">
-        <v>10326</v>
+        <v>10333</v>
       </c>
       <c r="F374" s="2">
-        <v>10054</v>
+        <v>10058</v>
       </c>
       <c r="G374" s="2">
-        <v>10582</v>
+        <v>10567</v>
       </c>
       <c r="H374" s="3">
         <v>1.1599999999999999</v>
@@ -17053,25 +17058,25 @@
         <v>385</v>
       </c>
       <c r="B375" s="2">
-        <v>11627</v>
+        <v>11675</v>
       </c>
       <c r="C375" s="2">
-        <v>11270</v>
+        <v>11337</v>
       </c>
       <c r="D375" s="2">
-        <v>12010</v>
+        <v>12046</v>
       </c>
       <c r="E375" s="2">
-        <v>11019</v>
+        <v>11028</v>
       </c>
       <c r="F375" s="2">
-        <v>10701</v>
+        <v>10721</v>
       </c>
       <c r="G375" s="2">
-        <v>11333</v>
+        <v>11301</v>
       </c>
       <c r="H375" s="3">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="I375" s="3">
         <v>1.22</v>
@@ -17080,7 +17085,7 @@
         <v>1.26</v>
       </c>
       <c r="K375" s="3">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="L375" s="3">
         <v>1.1499999999999999</v>
@@ -17094,25 +17099,25 @@
         <v>386</v>
       </c>
       <c r="B376" s="2">
-        <v>11513</v>
+        <v>11503</v>
       </c>
       <c r="C376" s="2">
-        <v>11035</v>
+        <v>11163</v>
       </c>
       <c r="D376" s="2">
-        <v>11968</v>
+        <v>11946</v>
       </c>
       <c r="E376" s="2">
-        <v>11622</v>
+        <v>11628</v>
       </c>
       <c r="F376" s="2">
-        <v>11234</v>
+        <v>11281</v>
       </c>
       <c r="G376" s="2">
-        <v>12001</v>
+        <v>11971</v>
       </c>
       <c r="H376" s="3">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="I376" s="3">
         <v>1.28</v>
@@ -17124,7 +17129,7 @@
         <v>1.17</v>
       </c>
       <c r="L376" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="M376" s="3">
         <v>1.18</v>
@@ -17135,28 +17140,28 @@
         <v>387</v>
       </c>
       <c r="B377" s="2">
-        <v>11862</v>
+        <v>11935</v>
       </c>
       <c r="C377" s="2">
-        <v>11335</v>
+        <v>11483</v>
       </c>
       <c r="D377" s="2">
         <v>12446</v>
       </c>
       <c r="E377" s="2">
-        <v>11627</v>
+        <v>11658</v>
       </c>
       <c r="F377" s="2">
-        <v>11197</v>
+        <v>11287</v>
       </c>
       <c r="G377" s="2">
-        <v>12080</v>
+        <v>12072</v>
       </c>
       <c r="H377" s="3">
         <v>1.2</v>
       </c>
       <c r="I377" s="3">
-        <v>1.17</v>
+        <v>1.18</v>
       </c>
       <c r="J377" s="3">
         <v>1.22</v>
@@ -17176,28 +17181,28 @@
         <v>388</v>
       </c>
       <c r="B378" s="2">
-        <v>11775</v>
+        <v>11725</v>
       </c>
       <c r="C378" s="2">
-        <v>11150</v>
+        <v>11121</v>
       </c>
       <c r="D378" s="2">
-        <v>12294</v>
+        <v>12292</v>
       </c>
       <c r="E378" s="2">
-        <v>11694</v>
+        <v>11709</v>
       </c>
       <c r="F378" s="2">
-        <v>11198</v>
+        <v>11276</v>
       </c>
       <c r="G378" s="2">
-        <v>12179</v>
+        <v>12182</v>
       </c>
       <c r="H378" s="3">
         <v>1.1299999999999999</v>
       </c>
       <c r="I378" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J378" s="3">
         <v>1.1599999999999999</v>
@@ -17206,7 +17211,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="L378" s="3">
-        <v>1.1399999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="M378" s="3">
         <v>1.18</v>
@@ -17217,40 +17222,40 @@
         <v>389</v>
       </c>
       <c r="B379" s="2">
-        <v>11963</v>
+        <v>12091</v>
       </c>
       <c r="C379" s="2">
-        <v>11167</v>
+        <v>11379</v>
       </c>
       <c r="D379" s="2">
-        <v>12655</v>
+        <v>12595</v>
       </c>
       <c r="E379" s="2">
-        <v>11778</v>
+        <v>11814</v>
       </c>
       <c r="F379" s="2">
-        <v>11172</v>
+        <v>11286</v>
       </c>
       <c r="G379" s="2">
-        <v>12341</v>
+        <v>12320</v>
       </c>
       <c r="H379" s="3">
         <v>1.07</v>
       </c>
       <c r="I379" s="3">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="J379" s="3">
         <v>1.1000000000000001</v>
       </c>
       <c r="K379" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.17</v>
       </c>
       <c r="L379" s="3">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M379" s="3">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="380" spans="1:13">
@@ -17258,28 +17263,28 @@
         <v>390</v>
       </c>
       <c r="B380" s="2">
-        <v>15146</v>
+        <v>15272</v>
       </c>
       <c r="C380" s="2">
-        <v>13937</v>
+        <v>14440</v>
       </c>
       <c r="D380" s="2">
-        <v>16388</v>
+        <v>16224</v>
       </c>
       <c r="E380" s="2">
-        <v>12687</v>
+        <v>12756</v>
       </c>
       <c r="F380" s="2">
-        <v>11897</v>
+        <v>12106</v>
       </c>
       <c r="G380" s="2">
-        <v>13445</v>
+        <v>13389</v>
       </c>
       <c r="H380" s="3">
-        <v>1.0900000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I380" s="3">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
       <c r="J380" s="3">
         <v>1.1299999999999999</v>
@@ -17288,7 +17293,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="L380" s="3">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="M380" s="3">
         <v>1.19</v>
@@ -17299,28 +17304,28 @@
         <v>391</v>
       </c>
       <c r="B381" s="2">
-        <v>14766</v>
+        <v>14843</v>
       </c>
       <c r="C381" s="2">
-        <v>13345</v>
+        <v>13811</v>
       </c>
       <c r="D381" s="2">
-        <v>16121</v>
+        <v>16108</v>
       </c>
       <c r="E381" s="2">
-        <v>13413</v>
+        <v>13483</v>
       </c>
       <c r="F381" s="2">
-        <v>12400</v>
+        <v>12688</v>
       </c>
       <c r="G381" s="2">
-        <v>14364</v>
+        <v>14305</v>
       </c>
       <c r="H381" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="I381" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J381" s="3">
         <v>1.2</v>
@@ -17329,7 +17334,7 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="L381" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="M381" s="3">
         <v>1.19</v>
@@ -17340,40 +17345,40 @@
         <v>392</v>
       </c>
       <c r="B382" s="2">
-        <v>14601</v>
+        <v>14799</v>
       </c>
       <c r="C382" s="2">
-        <v>12758</v>
+        <v>13289</v>
       </c>
       <c r="D382" s="2">
-        <v>16672</v>
+        <v>16164</v>
       </c>
       <c r="E382" s="2">
-        <v>14119</v>
+        <v>14251</v>
       </c>
       <c r="F382" s="2">
-        <v>12802</v>
+        <v>13230</v>
       </c>
       <c r="G382" s="2">
-        <v>15459</v>
+        <v>15273</v>
       </c>
       <c r="H382" s="3">
-        <v>1.21</v>
+        <v>1.22</v>
       </c>
       <c r="I382" s="3">
+        <v>1.17</v>
+      </c>
+      <c r="J382" s="3">
+        <v>1.27</v>
+      </c>
+      <c r="K382" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="J382" s="3">
-        <v>1.26</v>
-      </c>
-      <c r="K382" s="3">
-        <v>1.1399999999999999</v>
-      </c>
       <c r="L382" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="M382" s="3">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="383" spans="1:13">
@@ -17381,40 +17386,40 @@
         <v>393</v>
       </c>
       <c r="B383" s="2">
-        <v>13531</v>
+        <v>14234</v>
       </c>
       <c r="C383" s="2">
-        <v>11467</v>
+        <v>12662</v>
       </c>
       <c r="D383" s="2">
-        <v>15406</v>
+        <v>15966</v>
       </c>
       <c r="E383" s="2">
-        <v>14511</v>
+        <v>14787</v>
       </c>
       <c r="F383" s="2">
-        <v>12877</v>
+        <v>13551</v>
       </c>
       <c r="G383" s="2">
-        <v>16146</v>
+        <v>16115</v>
       </c>
       <c r="H383" s="3">
-        <v>1.23</v>
+        <v>1.25</v>
       </c>
       <c r="I383" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.19</v>
       </c>
       <c r="J383" s="3">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
       <c r="K383" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="L383" s="3">
-        <v>1.07</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M383" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="384" spans="1:13">
@@ -17422,37 +17427,37 @@
         <v>394</v>
       </c>
       <c r="B384" s="2">
-        <v>13231</v>
+        <v>14173</v>
       </c>
       <c r="C384" s="2">
-        <v>10792</v>
+        <v>12013</v>
       </c>
       <c r="D384" s="2">
-        <v>15961</v>
+        <v>16307</v>
       </c>
       <c r="E384" s="2">
-        <v>14032</v>
+        <v>14512</v>
       </c>
       <c r="F384" s="2">
-        <v>12091</v>
+        <v>12944</v>
       </c>
       <c r="G384" s="2">
-        <v>16040</v>
+        <v>16136</v>
       </c>
       <c r="H384" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I384" s="3">
-        <v>1.02</v>
+        <v>1.07</v>
       </c>
       <c r="J384" s="3">
-        <v>1.18</v>
+        <v>1.21</v>
       </c>
       <c r="K384" s="3">
-        <v>1.0900000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="L384" s="3">
-        <v>1.04</v>
+        <v>1.07</v>
       </c>
       <c r="M384" s="3">
         <v>1.1599999999999999</v>
@@ -17463,40 +17468,40 @@
         <v>395</v>
       </c>
       <c r="B385" s="2">
-        <v>13690</v>
+        <v>14246</v>
       </c>
       <c r="C385" s="2">
-        <v>10078</v>
+        <v>11261</v>
       </c>
       <c r="D385" s="2">
-        <v>17233</v>
+        <v>17133</v>
       </c>
       <c r="E385" s="2">
-        <v>13763</v>
+        <v>14363</v>
       </c>
       <c r="F385" s="2">
-        <v>11274</v>
+        <v>12306</v>
       </c>
       <c r="G385" s="2">
-        <v>16318</v>
+        <v>16392</v>
       </c>
       <c r="H385" s="3">
-        <v>1.03</v>
+        <v>1.07</v>
       </c>
       <c r="I385" s="3">
-        <v>0.92</v>
+        <v>0.97</v>
       </c>
       <c r="J385" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K385" s="3">
         <v>1.1299999999999999</v>
       </c>
-      <c r="K385" s="3">
-        <v>1.08</v>
-      </c>
       <c r="L385" s="3">
-        <v>1</v>
+        <v>1.06</v>
       </c>
       <c r="M385" s="3">
-        <v>1.17</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="386" spans="1:13">
@@ -17504,40 +17509,81 @@
         <v>396</v>
       </c>
       <c r="B386" s="2">
-        <v>13871</v>
+        <v>16427</v>
       </c>
       <c r="C386" s="2">
-        <v>9051</v>
+        <v>12767</v>
       </c>
       <c r="D386" s="2">
-        <v>20043</v>
+        <v>20689</v>
       </c>
       <c r="E386" s="2">
-        <v>13581</v>
+        <v>14770</v>
       </c>
       <c r="F386" s="2">
-        <v>10347</v>
+        <v>12176</v>
       </c>
       <c r="G386" s="2">
-        <v>17161</v>
+        <v>17524</v>
       </c>
       <c r="H386" s="3">
-        <v>0.96</v>
+        <v>1.04</v>
       </c>
       <c r="I386" s="3">
-        <v>0.83</v>
+        <v>0.91</v>
       </c>
       <c r="J386" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="K386" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="L386" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="M386" s="3" t="s">
-        <v>402</v>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="K386" s="3">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="L386" s="3">
+        <v>1.06</v>
+      </c>
+      <c r="M386" s="3">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="387" spans="1:13">
+      <c r="A387" t="s">
+        <v>397</v>
+      </c>
+      <c r="B387" s="2">
+        <v>19522</v>
+      </c>
+      <c r="C387" s="2">
+        <v>12812</v>
+      </c>
+      <c r="D387" s="2">
+        <v>27368</v>
+      </c>
+      <c r="E387" s="2">
+        <v>16092</v>
+      </c>
+      <c r="F387" s="2">
+        <v>12213</v>
+      </c>
+      <c r="G387" s="2">
+        <v>20374</v>
+      </c>
+      <c r="H387" s="3">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="I387" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J387" s="3">
+        <v>1.23</v>
+      </c>
+      <c r="K387" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="L387" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="M387" s="3" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-04-15--05-03-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Nowcasting_Zahlen.xlsx
+++ b/rki-data/RKI-Nowcasting_Zahlen.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20371"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAAC9FD-DD11-4103-8567-FC9A3F501811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{734B81DC-68D9-452D-B243-D6C449C2E7FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="430">
   <si>
     <t>Erläuterung</t>
   </si>
@@ -27,7 +27,7 @@
     <t>Ergebnisse des Nowcastings und der Schätzung der Reproduktionszahl R</t>
   </si>
   <si>
-    <t>Datenstand: 2021-04-13, 00:00 Uhr</t>
+    <t>Datenstand: 2021-04-14, 00:00 Uhr</t>
   </si>
   <si>
     <t>Die Ergebnisse des Nowcastings, also die Schätzung der Anzahl von COVID-19 Neuerkrankungen wird dargestellt mit einem gleitenden 4-Tages-Mittelwert.</t>
@@ -36,7 +36,7 @@
     <t>Dabei wird jeder Wert mit den Werten der 3 vorhergehenden Tage gemittelt.</t>
   </si>
   <si>
-    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-04-13 dargestellten Nowcasting-Kurve.</t>
+    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-04-14 dargestellten Nowcasting-Kurve.</t>
   </si>
   <si>
     <t>Der letzte Schätzwert der Reproduktionszahl R wird ebenfalls im gleichen Lagebericht erwähnt.</t>
@@ -1266,6 +1266,9 @@
     <t>09.04.2021</t>
   </si>
   <si>
+    <t>10.04.2021</t>
+  </si>
+  <si>
     <t>Punktschätzer der Anzahl Neuerkrankungen (ohne Glättung)</t>
   </si>
   <si>
@@ -1278,9 +1281,18 @@
     <t>Obere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen</t>
   </si>
   <si>
+    <t>Punktschätzer der 4-Tage R-Wert</t>
+  </si>
+  <si>
     <t>.</t>
   </si>
   <si>
+    <t>Untere Grenze des 95%-Prädiktionsintervalls der 4-Tage R-Wert</t>
+  </si>
+  <si>
+    <t>Obere Grenze des 95%-Prädiktionsintervalls der 4-Tage R-Wert</t>
+  </si>
+  <si>
     <t>Punktschätzer des 7-Tage-R Wertes</t>
   </si>
   <si>
@@ -1293,16 +1305,7 @@
     <t>Untere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen (ohne Glättung)</t>
   </si>
   <si>
-    <t>Obere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen (ohne Glätttung)</t>
-  </si>
-  <si>
-    <t>Punktschätzer des 4-Tage R-Wertes</t>
-  </si>
-  <si>
-    <t>Untere Grenze des 95%-Prädiktionsintervalls des 4-Tage R-Wertes</t>
-  </si>
-  <si>
-    <t>Obere Grenze des 95%-Prädiktionsintervalls des 4-Tage R-Wertes</t>
+    <t>Obere Grenze des 95%-Prädiktionsintervalls der Anzahl Neuerkrankungen (ohne Glättung)</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1341,7 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1660,7 +1663,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1760,67 +1763,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M405"/>
+  <dimension ref="A1:M406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:M405"/>
+      <selection activeCell="H6" sqref="H6:M406"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="13" width="19.140625" customWidth="1"/>
+    <col min="1" max="13" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="94.5" customHeight="1">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="90">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>427</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1846,22 +1838,22 @@
         <v>238</v>
       </c>
       <c r="H2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="J2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="K2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="L2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="M2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1887,22 +1879,22 @@
         <v>276</v>
       </c>
       <c r="H3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="J3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="K3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="L3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="M3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1928,22 +1920,22 @@
         <v>342</v>
       </c>
       <c r="H4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="J4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="K4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="L4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="M4" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1969,22 +1961,22 @@
         <v>412</v>
       </c>
       <c r="H5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="J5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="K5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="L5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="M5" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -15894,10 +15886,10 @@
         <v>8136</v>
       </c>
       <c r="C345" s="2">
-        <v>8012</v>
+        <v>8011</v>
       </c>
       <c r="D345" s="2">
-        <v>8249</v>
+        <v>8246</v>
       </c>
       <c r="E345" s="2">
         <v>7208</v>
@@ -15906,7 +15898,7 @@
         <v>7098</v>
       </c>
       <c r="G345" s="2">
-        <v>7314</v>
+        <v>7313</v>
       </c>
       <c r="H345" s="3">
         <v>0.8</v>
@@ -15935,19 +15927,19 @@
         <v>7684</v>
       </c>
       <c r="C346" s="2">
-        <v>7585</v>
+        <v>7588</v>
       </c>
       <c r="D346" s="2">
-        <v>7788</v>
+        <v>7784</v>
       </c>
       <c r="E346" s="2">
         <v>7248</v>
       </c>
       <c r="F346" s="2">
-        <v>7146</v>
+        <v>7147</v>
       </c>
       <c r="G346" s="2">
-        <v>7351</v>
+        <v>7350</v>
       </c>
       <c r="H346" s="3">
         <v>0.87</v>
@@ -15976,10 +15968,10 @@
         <v>7430</v>
       </c>
       <c r="C347" s="2">
-        <v>7328</v>
+        <v>7327</v>
       </c>
       <c r="D347" s="2">
-        <v>7518</v>
+        <v>7520</v>
       </c>
       <c r="E347" s="2">
         <v>7421</v>
@@ -15988,7 +15980,7 @@
         <v>7318</v>
       </c>
       <c r="G347" s="2">
-        <v>7522</v>
+        <v>7521</v>
       </c>
       <c r="H347" s="3">
         <v>0.97</v>
@@ -16014,22 +16006,22 @@
         <v>358</v>
       </c>
       <c r="B348" s="2">
-        <v>6691</v>
+        <v>6692</v>
       </c>
       <c r="C348" s="2">
         <v>6598</v>
       </c>
       <c r="D348" s="2">
-        <v>6804</v>
+        <v>6807</v>
       </c>
       <c r="E348" s="2">
-        <v>7485</v>
+        <v>7486</v>
       </c>
       <c r="F348" s="2">
-        <v>7380</v>
+        <v>7381</v>
       </c>
       <c r="G348" s="2">
-        <v>7590</v>
+        <v>7589</v>
       </c>
       <c r="H348" s="3">
         <v>1.05</v>
@@ -16055,19 +16047,19 @@
         <v>359</v>
       </c>
       <c r="B349" s="2">
-        <v>6907</v>
+        <v>6908</v>
       </c>
       <c r="C349" s="2">
-        <v>6809</v>
+        <v>6815</v>
       </c>
       <c r="D349" s="2">
-        <v>7023</v>
+        <v>7024</v>
       </c>
       <c r="E349" s="2">
-        <v>7178</v>
+        <v>7179</v>
       </c>
       <c r="F349" s="2">
-        <v>7080</v>
+        <v>7082</v>
       </c>
       <c r="G349" s="2">
         <v>7283</v>
@@ -16099,19 +16091,19 @@
         <v>6423</v>
       </c>
       <c r="C350" s="2">
-        <v>6321</v>
+        <v>6324</v>
       </c>
       <c r="D350" s="2">
-        <v>6538</v>
+        <v>6541</v>
       </c>
       <c r="E350" s="2">
         <v>6863</v>
       </c>
       <c r="F350" s="2">
-        <v>6764</v>
+        <v>6766</v>
       </c>
       <c r="G350" s="2">
-        <v>6971</v>
+        <v>6973</v>
       </c>
       <c r="H350" s="3">
         <v>0.95</v>
@@ -16140,19 +16132,19 @@
         <v>6626</v>
       </c>
       <c r="C351" s="2">
-        <v>6543</v>
+        <v>6542</v>
       </c>
       <c r="D351" s="2">
-        <v>6735</v>
+        <v>6739</v>
       </c>
       <c r="E351" s="2">
-        <v>6661</v>
+        <v>6662</v>
       </c>
       <c r="F351" s="2">
-        <v>6567</v>
+        <v>6570</v>
       </c>
       <c r="G351" s="2">
-        <v>6775</v>
+        <v>6777</v>
       </c>
       <c r="H351" s="3">
         <v>0.9</v>
@@ -16181,19 +16173,19 @@
         <v>8545</v>
       </c>
       <c r="C352" s="2">
-        <v>8434</v>
+        <v>8437</v>
       </c>
       <c r="D352" s="2">
-        <v>8652</v>
+        <v>8653</v>
       </c>
       <c r="E352" s="2">
-        <v>7125</v>
+        <v>7126</v>
       </c>
       <c r="F352" s="2">
-        <v>7027</v>
+        <v>7029</v>
       </c>
       <c r="G352" s="2">
-        <v>7237</v>
+        <v>7239</v>
       </c>
       <c r="H352" s="3">
         <v>0.95</v>
@@ -16222,10 +16214,10 @@
         <v>8146</v>
       </c>
       <c r="C353" s="2">
-        <v>8029</v>
+        <v>8028</v>
       </c>
       <c r="D353" s="2">
-        <v>8285</v>
+        <v>8286</v>
       </c>
       <c r="E353" s="2">
         <v>7435</v>
@@ -16234,13 +16226,13 @@
         <v>7332</v>
       </c>
       <c r="G353" s="2">
-        <v>7552</v>
+        <v>7554</v>
       </c>
       <c r="H353" s="3">
         <v>1.04</v>
       </c>
       <c r="I353" s="3">
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="J353" s="3">
         <v>1.05</v>
@@ -16263,19 +16255,19 @@
         <v>8073</v>
       </c>
       <c r="C354" s="2">
-        <v>7946</v>
+        <v>7948</v>
       </c>
       <c r="D354" s="2">
-        <v>8173</v>
+        <v>8171</v>
       </c>
       <c r="E354" s="2">
         <v>7847</v>
       </c>
       <c r="F354" s="2">
-        <v>7738</v>
+        <v>7739</v>
       </c>
       <c r="G354" s="2">
-        <v>7961</v>
+        <v>7962</v>
       </c>
       <c r="H354" s="3">
         <v>1.1399999999999999</v>
@@ -16301,19 +16293,19 @@
         <v>365</v>
       </c>
       <c r="B355" s="2">
-        <v>7719</v>
+        <v>7720</v>
       </c>
       <c r="C355" s="2">
-        <v>7596</v>
+        <v>7595</v>
       </c>
       <c r="D355" s="2">
-        <v>7830</v>
+        <v>7831</v>
       </c>
       <c r="E355" s="2">
         <v>8121</v>
       </c>
       <c r="F355" s="2">
-        <v>8001</v>
+        <v>8002</v>
       </c>
       <c r="G355" s="2">
         <v>8235</v>
@@ -16345,19 +16337,19 @@
         <v>7652</v>
       </c>
       <c r="C356" s="2">
-        <v>7535</v>
+        <v>7537</v>
       </c>
       <c r="D356" s="2">
-        <v>7755</v>
+        <v>7762</v>
       </c>
       <c r="E356" s="2">
         <v>7897</v>
       </c>
       <c r="F356" s="2">
-        <v>7776</v>
+        <v>7777</v>
       </c>
       <c r="G356" s="2">
-        <v>8010</v>
+        <v>8012</v>
       </c>
       <c r="H356" s="3">
         <v>1.1100000000000001</v>
@@ -16383,13 +16375,13 @@
         <v>367</v>
       </c>
       <c r="B357" s="2">
-        <v>7382</v>
+        <v>7383</v>
       </c>
       <c r="C357" s="2">
         <v>7278</v>
       </c>
       <c r="D357" s="2">
-        <v>7490</v>
+        <v>7489</v>
       </c>
       <c r="E357" s="2">
         <v>7707</v>
@@ -16398,7 +16390,7 @@
         <v>7589</v>
       </c>
       <c r="G357" s="2">
-        <v>7812</v>
+        <v>7813</v>
       </c>
       <c r="H357" s="3">
         <v>1.04</v>
@@ -16424,22 +16416,22 @@
         <v>368</v>
       </c>
       <c r="B358" s="2">
-        <v>7126</v>
+        <v>7125</v>
       </c>
       <c r="C358" s="2">
-        <v>7027</v>
+        <v>7022</v>
       </c>
       <c r="D358" s="2">
-        <v>7233</v>
+        <v>7234</v>
       </c>
       <c r="E358" s="2">
         <v>7470</v>
       </c>
       <c r="F358" s="2">
-        <v>7359</v>
+        <v>7358</v>
       </c>
       <c r="G358" s="2">
-        <v>7577</v>
+        <v>7579</v>
       </c>
       <c r="H358" s="3">
         <v>0.95</v>
@@ -16471,13 +16463,13 @@
         <v>8829</v>
       </c>
       <c r="D359" s="2">
-        <v>9068</v>
+        <v>9059</v>
       </c>
       <c r="E359" s="2">
         <v>7779</v>
       </c>
       <c r="F359" s="2">
-        <v>7667</v>
+        <v>7666</v>
       </c>
       <c r="G359" s="2">
         <v>7886</v>
@@ -16506,22 +16498,22 @@
         <v>370</v>
       </c>
       <c r="B360" s="2">
-        <v>8499</v>
+        <v>8501</v>
       </c>
       <c r="C360" s="2">
-        <v>8392</v>
+        <v>8390</v>
       </c>
       <c r="D360" s="2">
-        <v>8604</v>
+        <v>8596</v>
       </c>
       <c r="E360" s="2">
-        <v>7991</v>
+        <v>7992</v>
       </c>
       <c r="F360" s="2">
-        <v>7881</v>
+        <v>7880</v>
       </c>
       <c r="G360" s="2">
-        <v>8098</v>
+        <v>8094</v>
       </c>
       <c r="H360" s="3">
         <v>1.01</v>
@@ -16547,13 +16539,13 @@
         <v>371</v>
       </c>
       <c r="B361" s="2">
-        <v>8089</v>
+        <v>8088</v>
       </c>
       <c r="C361" s="2">
-        <v>7984</v>
+        <v>7990</v>
       </c>
       <c r="D361" s="2">
-        <v>8205</v>
+        <v>8204</v>
       </c>
       <c r="E361" s="2">
         <v>8168</v>
@@ -16562,7 +16554,7 @@
         <v>8058</v>
       </c>
       <c r="G361" s="2">
-        <v>8277</v>
+        <v>8273</v>
       </c>
       <c r="H361" s="3">
         <v>1.06</v>
@@ -16588,10 +16580,10 @@
         <v>372</v>
       </c>
       <c r="B362" s="2">
-        <v>7658</v>
+        <v>7657</v>
       </c>
       <c r="C362" s="2">
-        <v>7546</v>
+        <v>7535</v>
       </c>
       <c r="D362" s="2">
         <v>7774</v>
@@ -16600,10 +16592,10 @@
         <v>8301</v>
       </c>
       <c r="F362" s="2">
-        <v>8188</v>
+        <v>8186</v>
       </c>
       <c r="G362" s="2">
-        <v>8412</v>
+        <v>8408</v>
       </c>
       <c r="H362" s="3">
         <v>1.1100000000000001</v>
@@ -16629,22 +16621,22 @@
         <v>373</v>
       </c>
       <c r="B363" s="2">
-        <v>7940</v>
+        <v>7939</v>
       </c>
       <c r="C363" s="2">
-        <v>7844</v>
+        <v>7836</v>
       </c>
       <c r="D363" s="2">
         <v>8050</v>
       </c>
       <c r="E363" s="2">
-        <v>8047</v>
+        <v>8046</v>
       </c>
       <c r="F363" s="2">
-        <v>7941</v>
+        <v>7938</v>
       </c>
       <c r="G363" s="2">
-        <v>8158</v>
+        <v>8156</v>
       </c>
       <c r="H363" s="3">
         <v>1.03</v>
@@ -16670,22 +16662,22 @@
         <v>374</v>
       </c>
       <c r="B364" s="2">
-        <v>7182</v>
+        <v>7185</v>
       </c>
       <c r="C364" s="2">
-        <v>7082</v>
+        <v>7083</v>
       </c>
       <c r="D364" s="2">
-        <v>7288</v>
+        <v>7282</v>
       </c>
       <c r="E364" s="2">
         <v>7717</v>
       </c>
       <c r="F364" s="2">
-        <v>7614</v>
+        <v>7611</v>
       </c>
       <c r="G364" s="2">
-        <v>7829</v>
+        <v>7827</v>
       </c>
       <c r="H364" s="3">
         <v>0.97</v>
@@ -16711,22 +16703,22 @@
         <v>375</v>
       </c>
       <c r="B365" s="2">
-        <v>7350</v>
+        <v>7351</v>
       </c>
       <c r="C365" s="2">
-        <v>7227</v>
+        <v>7234</v>
       </c>
       <c r="D365" s="2">
-        <v>7453</v>
+        <v>7444</v>
       </c>
       <c r="E365" s="2">
-        <v>7532</v>
+        <v>7533</v>
       </c>
       <c r="F365" s="2">
-        <v>7424</v>
+        <v>7422</v>
       </c>
       <c r="G365" s="2">
-        <v>7641</v>
+        <v>7637</v>
       </c>
       <c r="H365" s="3">
         <v>0.92</v>
@@ -16752,22 +16744,22 @@
         <v>376</v>
       </c>
       <c r="B366" s="2">
-        <v>9525</v>
+        <v>9526</v>
       </c>
       <c r="C366" s="2">
         <v>9416</v>
       </c>
       <c r="D366" s="2">
-        <v>9644</v>
+        <v>9631</v>
       </c>
       <c r="E366" s="2">
-        <v>7999</v>
+        <v>8000</v>
       </c>
       <c r="F366" s="2">
         <v>7892</v>
       </c>
       <c r="G366" s="2">
-        <v>8108</v>
+        <v>8102</v>
       </c>
       <c r="H366" s="3">
         <v>0.96</v>
@@ -16793,22 +16785,22 @@
         <v>377</v>
       </c>
       <c r="B367" s="2">
-        <v>8913</v>
+        <v>8911</v>
       </c>
       <c r="C367" s="2">
-        <v>8817</v>
+        <v>8794</v>
       </c>
       <c r="D367" s="2">
-        <v>9029</v>
+        <v>9038</v>
       </c>
       <c r="E367" s="2">
         <v>8243</v>
       </c>
       <c r="F367" s="2">
-        <v>8135</v>
+        <v>8132</v>
       </c>
       <c r="G367" s="2">
-        <v>8353</v>
+        <v>8349</v>
       </c>
       <c r="H367" s="3">
         <v>1.02</v>
@@ -16834,22 +16826,22 @@
         <v>378</v>
       </c>
       <c r="B368" s="2">
-        <v>9001</v>
+        <v>9000</v>
       </c>
       <c r="C368" s="2">
-        <v>8875</v>
+        <v>8860</v>
       </c>
       <c r="D368" s="2">
-        <v>9107</v>
+        <v>9086</v>
       </c>
       <c r="E368" s="2">
         <v>8697</v>
       </c>
       <c r="F368" s="2">
-        <v>8583</v>
+        <v>8576</v>
       </c>
       <c r="G368" s="2">
-        <v>8808</v>
+        <v>8800</v>
       </c>
       <c r="H368" s="3">
         <v>1.1299999999999999</v>
@@ -16875,22 +16867,22 @@
         <v>379</v>
       </c>
       <c r="B369" s="2">
-        <v>8659</v>
+        <v>8651</v>
       </c>
       <c r="C369" s="2">
-        <v>8545</v>
+        <v>8541</v>
       </c>
       <c r="D369" s="2">
-        <v>8764</v>
+        <v>8768</v>
       </c>
       <c r="E369" s="2">
-        <v>9025</v>
+        <v>9022</v>
       </c>
       <c r="F369" s="2">
-        <v>8913</v>
+        <v>8902</v>
       </c>
       <c r="G369" s="2">
-        <v>9136</v>
+        <v>9131</v>
       </c>
       <c r="H369" s="3">
         <v>1.2</v>
@@ -16919,19 +16911,19 @@
         <v>9026</v>
       </c>
       <c r="C370" s="2">
-        <v>8924</v>
+        <v>8913</v>
       </c>
       <c r="D370" s="2">
-        <v>9136</v>
+        <v>9149</v>
       </c>
       <c r="E370" s="2">
-        <v>8900</v>
+        <v>8897</v>
       </c>
       <c r="F370" s="2">
-        <v>8790</v>
+        <v>8777</v>
       </c>
       <c r="G370" s="2">
-        <v>9009</v>
+        <v>9010</v>
       </c>
       <c r="H370" s="3">
         <v>1.1100000000000001</v>
@@ -16957,22 +16949,22 @@
         <v>381</v>
       </c>
       <c r="B371" s="2">
-        <v>8901</v>
+        <v>8892</v>
       </c>
       <c r="C371" s="2">
-        <v>8776</v>
+        <v>8779</v>
       </c>
       <c r="D371" s="2">
-        <v>9024</v>
+        <v>9022</v>
       </c>
       <c r="E371" s="2">
-        <v>8897</v>
+        <v>8892</v>
       </c>
       <c r="F371" s="2">
-        <v>8780</v>
+        <v>8773</v>
       </c>
       <c r="G371" s="2">
-        <v>9008</v>
+        <v>9006</v>
       </c>
       <c r="H371" s="3">
         <v>1.08</v>
@@ -17001,19 +16993,19 @@
         <v>9037</v>
       </c>
       <c r="C372" s="2">
-        <v>8926</v>
+        <v>8903</v>
       </c>
       <c r="D372" s="2">
-        <v>9148</v>
+        <v>9163</v>
       </c>
       <c r="E372" s="2">
-        <v>8906</v>
+        <v>8902</v>
       </c>
       <c r="F372" s="2">
-        <v>8793</v>
+        <v>8784</v>
       </c>
       <c r="G372" s="2">
-        <v>9018</v>
+        <v>9025</v>
       </c>
       <c r="H372" s="3">
         <v>1.02</v>
@@ -17039,22 +17031,22 @@
         <v>383</v>
       </c>
       <c r="B373" s="2">
-        <v>11800</v>
+        <v>11781</v>
       </c>
       <c r="C373" s="2">
-        <v>11671</v>
+        <v>11636</v>
       </c>
       <c r="D373" s="2">
-        <v>11925</v>
+        <v>11935</v>
       </c>
       <c r="E373" s="2">
-        <v>9691</v>
+        <v>9684</v>
       </c>
       <c r="F373" s="2">
-        <v>9574</v>
+        <v>9558</v>
       </c>
       <c r="G373" s="2">
-        <v>9808</v>
+        <v>9817</v>
       </c>
       <c r="H373" s="3">
         <v>1.07</v>
@@ -17080,22 +17072,22 @@
         <v>384</v>
       </c>
       <c r="B374" s="2">
-        <v>11499</v>
+        <v>11500</v>
       </c>
       <c r="C374" s="2">
-        <v>11361</v>
+        <v>11350</v>
       </c>
       <c r="D374" s="2">
-        <v>11650</v>
+        <v>11668</v>
       </c>
       <c r="E374" s="2">
-        <v>10309</v>
+        <v>10303</v>
       </c>
       <c r="F374" s="2">
-        <v>10183</v>
+        <v>10167</v>
       </c>
       <c r="G374" s="2">
-        <v>10437</v>
+        <v>10447</v>
       </c>
       <c r="H374" s="3">
         <v>1.1599999999999999</v>
@@ -17121,22 +17113,22 @@
         <v>385</v>
       </c>
       <c r="B375" s="2">
-        <v>11706</v>
+        <v>11716</v>
       </c>
       <c r="C375" s="2">
-        <v>11579</v>
+        <v>11588</v>
       </c>
       <c r="D375" s="2">
-        <v>11833</v>
+        <v>11840</v>
       </c>
       <c r="E375" s="2">
-        <v>11010</v>
+        <v>11009</v>
       </c>
       <c r="F375" s="2">
-        <v>10884</v>
+        <v>10869</v>
       </c>
       <c r="G375" s="2">
-        <v>11139</v>
+        <v>11151</v>
       </c>
       <c r="H375" s="3">
         <v>1.24</v>
@@ -17162,19 +17154,19 @@
         <v>386</v>
       </c>
       <c r="B376" s="2">
-        <v>11522</v>
+        <v>11507</v>
       </c>
       <c r="C376" s="2">
-        <v>11370</v>
+        <v>11365</v>
       </c>
       <c r="D376" s="2">
-        <v>11675</v>
+        <v>11643</v>
       </c>
       <c r="E376" s="2">
-        <v>11632</v>
+        <v>11626</v>
       </c>
       <c r="F376" s="2">
-        <v>11495</v>
+        <v>11485</v>
       </c>
       <c r="G376" s="2">
         <v>11771</v>
@@ -17183,7 +17175,7 @@
         <v>1.31</v>
       </c>
       <c r="I376" s="3">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="J376" s="3">
         <v>1.32</v>
@@ -17203,22 +17195,22 @@
         <v>387</v>
       </c>
       <c r="B377" s="2">
-        <v>12062</v>
+        <v>12041</v>
       </c>
       <c r="C377" s="2">
-        <v>11923</v>
+        <v>11898</v>
       </c>
       <c r="D377" s="2">
-        <v>12176</v>
+        <v>12200</v>
       </c>
       <c r="E377" s="2">
-        <v>11697</v>
+        <v>11691</v>
       </c>
       <c r="F377" s="2">
-        <v>11558</v>
+        <v>11550</v>
       </c>
       <c r="G377" s="2">
-        <v>11833</v>
+        <v>11838</v>
       </c>
       <c r="H377" s="3">
         <v>1.21</v>
@@ -17244,22 +17236,22 @@
         <v>388</v>
       </c>
       <c r="B378" s="2">
-        <v>11835</v>
+        <v>11848</v>
       </c>
       <c r="C378" s="2">
-        <v>11707</v>
+        <v>11724</v>
       </c>
       <c r="D378" s="2">
-        <v>11960</v>
+        <v>12001</v>
       </c>
       <c r="E378" s="2">
-        <v>11781</v>
+        <v>11778</v>
       </c>
       <c r="F378" s="2">
         <v>11644</v>
       </c>
       <c r="G378" s="2">
-        <v>11911</v>
+        <v>11921</v>
       </c>
       <c r="H378" s="3">
         <v>1.1399999999999999</v>
@@ -17285,19 +17277,19 @@
         <v>389</v>
       </c>
       <c r="B379" s="2">
-        <v>12125</v>
+        <v>12126</v>
       </c>
       <c r="C379" s="2">
-        <v>11958</v>
+        <v>11964</v>
       </c>
       <c r="D379" s="2">
-        <v>12291</v>
+        <v>12255</v>
       </c>
       <c r="E379" s="2">
-        <v>11886</v>
+        <v>11880</v>
       </c>
       <c r="F379" s="2">
-        <v>11739</v>
+        <v>11738</v>
       </c>
       <c r="G379" s="2">
         <v>12025</v>
@@ -17326,22 +17318,22 @@
         <v>390</v>
       </c>
       <c r="B380" s="2">
-        <v>15421</v>
+        <v>15427</v>
       </c>
       <c r="C380" s="2">
-        <v>15230</v>
+        <v>15284</v>
       </c>
       <c r="D380" s="2">
-        <v>15576</v>
+        <v>15619</v>
       </c>
       <c r="E380" s="2">
-        <v>12861</v>
+        <v>12860</v>
       </c>
       <c r="F380" s="2">
-        <v>12704</v>
+        <v>12717</v>
       </c>
       <c r="G380" s="2">
-        <v>13001</v>
+        <v>13019</v>
       </c>
       <c r="H380" s="3">
         <v>1.1100000000000001</v>
@@ -17367,22 +17359,22 @@
         <v>391</v>
       </c>
       <c r="B381" s="2">
-        <v>14893</v>
+        <v>14878</v>
       </c>
       <c r="C381" s="2">
-        <v>14665</v>
+        <v>14675</v>
       </c>
       <c r="D381" s="2">
-        <v>15118</v>
+        <v>15076</v>
       </c>
       <c r="E381" s="2">
-        <v>13569</v>
+        <v>13570</v>
       </c>
       <c r="F381" s="2">
-        <v>13390</v>
+        <v>13412</v>
       </c>
       <c r="G381" s="2">
-        <v>13736</v>
+        <v>13738</v>
       </c>
       <c r="H381" s="3">
         <v>1.1599999999999999</v>
@@ -17408,22 +17400,22 @@
         <v>392</v>
       </c>
       <c r="B382" s="2">
-        <v>15011</v>
+        <v>15025</v>
       </c>
       <c r="C382" s="2">
-        <v>14828</v>
+        <v>14809</v>
       </c>
       <c r="D382" s="2">
-        <v>15213</v>
+        <v>15219</v>
       </c>
       <c r="E382" s="2">
-        <v>14362</v>
+        <v>14364</v>
       </c>
       <c r="F382" s="2">
-        <v>14170</v>
+        <v>14183</v>
       </c>
       <c r="G382" s="2">
-        <v>14549</v>
+        <v>14542</v>
       </c>
       <c r="H382" s="3">
         <v>1.22</v>
@@ -17449,22 +17441,22 @@
         <v>393</v>
       </c>
       <c r="B383" s="2">
-        <v>14281</v>
+        <v>14277</v>
       </c>
       <c r="C383" s="2">
-        <v>14116</v>
+        <v>14063</v>
       </c>
       <c r="D383" s="2">
-        <v>14450</v>
+        <v>14484</v>
       </c>
       <c r="E383" s="2">
-        <v>14901</v>
+        <v>14902</v>
       </c>
       <c r="F383" s="2">
-        <v>14710</v>
+        <v>14708</v>
       </c>
       <c r="G383" s="2">
-        <v>15089</v>
+        <v>15099</v>
       </c>
       <c r="H383" s="3">
         <v>1.25</v>
@@ -17490,22 +17482,22 @@
         <v>394</v>
       </c>
       <c r="B384" s="2">
-        <v>14838</v>
+        <v>14858</v>
       </c>
       <c r="C384" s="2">
-        <v>14656</v>
+        <v>14637</v>
       </c>
       <c r="D384" s="2">
-        <v>15049</v>
+        <v>15090</v>
       </c>
       <c r="E384" s="2">
-        <v>14755</v>
+        <v>14759</v>
       </c>
       <c r="F384" s="2">
-        <v>14566</v>
+        <v>14546</v>
       </c>
       <c r="G384" s="2">
-        <v>14957</v>
+        <v>14967</v>
       </c>
       <c r="H384" s="3">
         <v>1.1499999999999999</v>
@@ -17531,22 +17523,22 @@
         <v>395</v>
       </c>
       <c r="B385" s="2">
-        <v>15005</v>
+        <v>15031</v>
       </c>
       <c r="C385" s="2">
-        <v>14787</v>
+        <v>14829</v>
       </c>
       <c r="D385" s="2">
-        <v>15208</v>
+        <v>15291</v>
       </c>
       <c r="E385" s="2">
-        <v>14784</v>
+        <v>14798</v>
       </c>
       <c r="F385" s="2">
-        <v>14597</v>
+        <v>14584</v>
       </c>
       <c r="G385" s="2">
-        <v>14980</v>
+        <v>15021</v>
       </c>
       <c r="H385" s="3">
         <v>1.0900000000000001</v>
@@ -17561,7 +17553,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="L385" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="M385" s="3">
         <v>1.1299999999999999</v>
@@ -17572,22 +17564,22 @@
         <v>396</v>
       </c>
       <c r="B386" s="2">
-        <v>15432</v>
+        <v>15426</v>
       </c>
       <c r="C386" s="2">
-        <v>15238</v>
+        <v>15190</v>
       </c>
       <c r="D386" s="2">
-        <v>15658</v>
+        <v>15694</v>
       </c>
       <c r="E386" s="2">
-        <v>14889</v>
+        <v>14898</v>
       </c>
       <c r="F386" s="2">
-        <v>14699</v>
+        <v>14679</v>
       </c>
       <c r="G386" s="2">
-        <v>15091</v>
+        <v>15140</v>
       </c>
       <c r="H386" s="3">
         <v>1.04</v>
@@ -17613,28 +17605,28 @@
         <v>397</v>
       </c>
       <c r="B387" s="2">
-        <v>18843</v>
+        <v>18839</v>
       </c>
       <c r="C387" s="2">
-        <v>18520</v>
+        <v>18587</v>
       </c>
       <c r="D387" s="2">
-        <v>19227</v>
+        <v>19086</v>
       </c>
       <c r="E387" s="2">
-        <v>16029</v>
+        <v>16038</v>
       </c>
       <c r="F387" s="2">
-        <v>15800</v>
+        <v>15810</v>
       </c>
       <c r="G387" s="2">
-        <v>16285</v>
+        <v>16290</v>
       </c>
       <c r="H387" s="3">
         <v>1.08</v>
       </c>
       <c r="I387" s="3">
-        <v>1.06</v>
+        <v>1.07</v>
       </c>
       <c r="J387" s="3">
         <v>1.0900000000000001</v>
@@ -17654,22 +17646,22 @@
         <v>398</v>
       </c>
       <c r="B388" s="2">
-        <v>18608</v>
+        <v>18578</v>
       </c>
       <c r="C388" s="2">
-        <v>18315</v>
+        <v>18242</v>
       </c>
       <c r="D388" s="2">
-        <v>18924</v>
+        <v>18843</v>
       </c>
       <c r="E388" s="2">
-        <v>16972</v>
+        <v>16969</v>
       </c>
       <c r="F388" s="2">
-        <v>16715</v>
+        <v>16712</v>
       </c>
       <c r="G388" s="2">
-        <v>17254</v>
+        <v>17228</v>
       </c>
       <c r="H388" s="3">
         <v>1.1499999999999999</v>
@@ -17695,28 +17687,28 @@
         <v>399</v>
       </c>
       <c r="B389" s="2">
-        <v>17952</v>
+        <v>17921</v>
       </c>
       <c r="C389" s="2">
-        <v>17610</v>
+        <v>17647</v>
       </c>
       <c r="D389" s="2">
-        <v>18301</v>
+        <v>18172</v>
       </c>
       <c r="E389" s="2">
-        <v>17709</v>
+        <v>17691</v>
       </c>
       <c r="F389" s="2">
-        <v>17421</v>
+        <v>17416</v>
       </c>
       <c r="G389" s="2">
-        <v>18028</v>
+        <v>17949</v>
       </c>
       <c r="H389" s="3">
         <v>1.2</v>
       </c>
       <c r="I389" s="3">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="J389" s="3">
         <v>1.21</v>
@@ -17736,22 +17728,22 @@
         <v>400</v>
       </c>
       <c r="B390" s="2">
-        <v>16557</v>
+        <v>16632</v>
       </c>
       <c r="C390" s="2">
-        <v>16256</v>
+        <v>16335</v>
       </c>
       <c r="D390" s="2">
-        <v>16933</v>
+        <v>16944</v>
       </c>
       <c r="E390" s="2">
-        <v>17990</v>
+        <v>17993</v>
       </c>
       <c r="F390" s="2">
-        <v>17675</v>
+        <v>17703</v>
       </c>
       <c r="G390" s="2">
-        <v>18346</v>
+        <v>18261</v>
       </c>
       <c r="H390" s="3">
         <v>1.21</v>
@@ -17777,22 +17769,22 @@
         <v>401</v>
       </c>
       <c r="B391" s="2">
-        <v>16252</v>
+        <v>16295</v>
       </c>
       <c r="C391" s="2">
-        <v>15899</v>
+        <v>15997</v>
       </c>
       <c r="D391" s="2">
-        <v>16563</v>
+        <v>16585</v>
       </c>
       <c r="E391" s="2">
-        <v>17342</v>
+        <v>17357</v>
       </c>
       <c r="F391" s="2">
-        <v>17020</v>
+        <v>17055</v>
       </c>
       <c r="G391" s="2">
-        <v>17680</v>
+        <v>17636</v>
       </c>
       <c r="H391" s="3">
         <v>1.08</v>
@@ -17818,22 +17810,22 @@
         <v>402</v>
       </c>
       <c r="B392" s="2">
-        <v>15236</v>
+        <v>15190</v>
       </c>
       <c r="C392" s="2">
-        <v>14834</v>
+        <v>14750</v>
       </c>
       <c r="D392" s="2">
-        <v>15705</v>
+        <v>15629</v>
       </c>
       <c r="E392" s="2">
-        <v>16499</v>
+        <v>16510</v>
       </c>
       <c r="F392" s="2">
-        <v>16150</v>
+        <v>16182</v>
       </c>
       <c r="G392" s="2">
-        <v>16876</v>
+        <v>16832</v>
       </c>
       <c r="H392" s="3">
         <v>0.97</v>
@@ -17859,28 +17851,28 @@
         <v>403</v>
       </c>
       <c r="B393" s="2">
-        <v>14803</v>
+        <v>14778</v>
       </c>
       <c r="C393" s="2">
-        <v>14283</v>
+        <v>14305</v>
       </c>
       <c r="D393" s="2">
-        <v>15334</v>
+        <v>15190</v>
       </c>
       <c r="E393" s="2">
-        <v>15712</v>
+        <v>15724</v>
       </c>
       <c r="F393" s="2">
-        <v>15318</v>
+        <v>15346</v>
       </c>
       <c r="G393" s="2">
-        <v>16134</v>
+        <v>16087</v>
       </c>
       <c r="H393" s="3">
         <v>0.89</v>
       </c>
       <c r="I393" s="3">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="J393" s="3">
         <v>0.9</v>
@@ -17900,22 +17892,22 @@
         <v>404</v>
       </c>
       <c r="B394" s="2">
-        <v>18089</v>
+        <v>18114</v>
       </c>
       <c r="C394" s="2">
-        <v>17408</v>
+        <v>17414</v>
       </c>
       <c r="D394" s="2">
-        <v>18994</v>
+        <v>18645</v>
       </c>
       <c r="E394" s="2">
-        <v>16095</v>
+        <v>16094</v>
       </c>
       <c r="F394" s="2">
-        <v>15606</v>
+        <v>15616</v>
       </c>
       <c r="G394" s="2">
-        <v>16649</v>
+        <v>16512</v>
       </c>
       <c r="H394" s="3">
         <v>0.89</v>
@@ -17930,7 +17922,7 @@
         <v>0.98</v>
       </c>
       <c r="L394" s="3">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="M394" s="3">
         <v>0.99</v>
@@ -17941,22 +17933,22 @@
         <v>405</v>
       </c>
       <c r="B395" s="2">
-        <v>16967</v>
+        <v>17003</v>
       </c>
       <c r="C395" s="2">
-        <v>16275</v>
+        <v>16334</v>
       </c>
       <c r="D395" s="2">
-        <v>17719</v>
+        <v>17830</v>
       </c>
       <c r="E395" s="2">
-        <v>16274</v>
+        <v>16271</v>
       </c>
       <c r="F395" s="2">
-        <v>15700</v>
+        <v>15701</v>
       </c>
       <c r="G395" s="2">
-        <v>16938</v>
+        <v>16823</v>
       </c>
       <c r="H395" s="3">
         <v>0.94</v>
@@ -17965,7 +17957,7 @@
         <v>0.92</v>
       </c>
       <c r="J395" s="3">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="K395" s="3">
         <v>0.96</v>
@@ -17982,22 +17974,22 @@
         <v>406</v>
       </c>
       <c r="B396" s="2">
-        <v>15728</v>
+        <v>15758</v>
       </c>
       <c r="C396" s="2">
-        <v>14986</v>
+        <v>14936</v>
       </c>
       <c r="D396" s="2">
-        <v>16488</v>
+        <v>16764</v>
       </c>
       <c r="E396" s="2">
-        <v>16397</v>
+        <v>16413</v>
       </c>
       <c r="F396" s="2">
-        <v>15738</v>
+        <v>15747</v>
       </c>
       <c r="G396" s="2">
-        <v>17134</v>
+        <v>17107</v>
       </c>
       <c r="H396" s="3">
         <v>0.99</v>
@@ -18012,10 +18004,10 @@
         <v>0.96</v>
       </c>
       <c r="L396" s="3">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="M396" s="3">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="397" spans="1:13">
@@ -18023,34 +18015,34 @@
         <v>407</v>
       </c>
       <c r="B397" s="2">
-        <v>16304</v>
+        <v>16426</v>
       </c>
       <c r="C397" s="2">
-        <v>15138</v>
+        <v>15573</v>
       </c>
       <c r="D397" s="2">
-        <v>17262</v>
+        <v>17278</v>
       </c>
       <c r="E397" s="2">
-        <v>16772</v>
+        <v>16825</v>
       </c>
       <c r="F397" s="2">
-        <v>15952</v>
+        <v>16064</v>
       </c>
       <c r="G397" s="2">
-        <v>17616</v>
+        <v>17629</v>
       </c>
       <c r="H397" s="3">
         <v>1.07</v>
       </c>
       <c r="I397" s="3">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
       <c r="J397" s="3">
-        <v>1.0900000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K397" s="3">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="L397" s="3">
         <v>0.94</v>
@@ -18064,28 +18056,28 @@
         <v>408</v>
       </c>
       <c r="B398" s="2">
-        <v>14911</v>
+        <v>14961</v>
       </c>
       <c r="C398" s="2">
-        <v>13743</v>
+        <v>14181</v>
       </c>
       <c r="D398" s="2">
-        <v>16054</v>
+        <v>15885</v>
       </c>
       <c r="E398" s="2">
-        <v>15978</v>
+        <v>16037</v>
       </c>
       <c r="F398" s="2">
-        <v>15035</v>
+        <v>15256</v>
       </c>
       <c r="G398" s="2">
-        <v>16881</v>
+        <v>16939</v>
       </c>
       <c r="H398" s="3">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="I398" s="3">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="J398" s="3">
         <v>1.02</v>
@@ -18105,22 +18097,22 @@
         <v>409</v>
       </c>
       <c r="B399" s="2">
-        <v>14268</v>
+        <v>14309</v>
       </c>
       <c r="C399" s="2">
-        <v>12866</v>
+        <v>13244</v>
       </c>
       <c r="D399" s="2">
-        <v>15538</v>
+        <v>15288</v>
       </c>
       <c r="E399" s="2">
-        <v>15303</v>
+        <v>15363</v>
       </c>
       <c r="F399" s="2">
-        <v>14183</v>
+        <v>14484</v>
       </c>
       <c r="G399" s="2">
-        <v>16335</v>
+        <v>16303</v>
       </c>
       <c r="H399" s="3">
         <v>0.94</v>
@@ -18132,13 +18124,13 @@
         <v>0.97</v>
       </c>
       <c r="K399" s="3">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="L399" s="3">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="M399" s="3">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="400" spans="1:13">
@@ -18146,28 +18138,28 @@
         <v>410</v>
       </c>
       <c r="B400" s="2">
-        <v>14475</v>
+        <v>14645</v>
       </c>
       <c r="C400" s="2">
-        <v>12470</v>
+        <v>13310</v>
       </c>
       <c r="D400" s="2">
-        <v>16429</v>
+        <v>15906</v>
       </c>
       <c r="E400" s="2">
-        <v>14990</v>
+        <v>15085</v>
       </c>
       <c r="F400" s="2">
-        <v>13554</v>
+        <v>14077</v>
       </c>
       <c r="G400" s="2">
-        <v>16321</v>
+        <v>16089</v>
       </c>
       <c r="H400" s="3">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="I400" s="3">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="J400" s="3">
         <v>0.96</v>
@@ -18176,10 +18168,10 @@
         <v>0.96</v>
       </c>
       <c r="L400" s="3">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="M400" s="3">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="401" spans="1:13">
@@ -18187,25 +18179,25 @@
         <v>411</v>
       </c>
       <c r="B401" s="2">
-        <v>16321</v>
+        <v>16462</v>
       </c>
       <c r="C401" s="2">
-        <v>13918</v>
+        <v>14235</v>
       </c>
       <c r="D401" s="2">
-        <v>18152</v>
+        <v>18312</v>
       </c>
       <c r="E401" s="2">
-        <v>14994</v>
+        <v>15094</v>
       </c>
       <c r="F401" s="2">
-        <v>13249</v>
+        <v>13742</v>
       </c>
       <c r="G401" s="2">
-        <v>16543</v>
+        <v>16348</v>
       </c>
       <c r="H401" s="3">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="I401" s="3">
         <v>0.85</v>
@@ -18220,7 +18212,7 @@
         <v>0.96</v>
       </c>
       <c r="M401" s="3">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="402" spans="1:13">
@@ -18228,22 +18220,22 @@
         <v>412</v>
       </c>
       <c r="B402" s="2">
-        <v>19551</v>
+        <v>19183</v>
       </c>
       <c r="C402" s="2">
-        <v>16062</v>
+        <v>15263</v>
       </c>
       <c r="D402" s="2">
-        <v>23710</v>
+        <v>22212</v>
       </c>
       <c r="E402" s="2">
-        <v>16154</v>
+        <v>16150</v>
       </c>
       <c r="F402" s="2">
-        <v>13829</v>
+        <v>14013</v>
       </c>
       <c r="G402" s="2">
-        <v>18457</v>
+        <v>17930</v>
       </c>
       <c r="H402" s="3">
         <v>1.01</v>
@@ -18252,16 +18244,16 @@
         <v>0.94</v>
       </c>
       <c r="J402" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="K402" s="3">
         <v>1.04</v>
       </c>
       <c r="L402" s="3">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="M402" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="403" spans="1:13">
@@ -18269,22 +18261,22 @@
         <v>413</v>
       </c>
       <c r="B403" s="2">
-        <v>20038</v>
+        <v>20093</v>
       </c>
       <c r="C403" s="2">
-        <v>14359</v>
+        <v>15976</v>
       </c>
       <c r="D403" s="2">
-        <v>24261</v>
+        <v>24985</v>
       </c>
       <c r="E403" s="2">
         <v>17596</v>
       </c>
       <c r="F403" s="2">
-        <v>14202</v>
+        <v>14696</v>
       </c>
       <c r="G403" s="2">
-        <v>20638</v>
+        <v>20354</v>
       </c>
       <c r="H403" s="3">
         <v>1.1499999999999999</v>
@@ -18293,16 +18285,16 @@
         <v>1.04</v>
       </c>
       <c r="J403" s="3">
-        <v>1.27</v>
+        <v>1.24</v>
       </c>
       <c r="K403" s="3">
         <v>1.07</v>
       </c>
       <c r="L403" s="3">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="M403" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="404" spans="1:13">
@@ -18310,40 +18302,40 @@
         <v>414</v>
       </c>
       <c r="B404" s="2">
-        <v>18408</v>
+        <v>19243</v>
       </c>
       <c r="C404" s="2">
-        <v>10749</v>
+        <v>12916</v>
       </c>
       <c r="D404" s="2">
-        <v>24300</v>
+        <v>24338</v>
       </c>
       <c r="E404" s="2">
-        <v>18580</v>
+        <v>18745</v>
       </c>
       <c r="F404" s="2">
-        <v>13772</v>
+        <v>14598</v>
       </c>
       <c r="G404" s="2">
-        <v>22606</v>
+        <v>22462</v>
       </c>
       <c r="H404" s="3">
         <v>1.24</v>
       </c>
       <c r="I404" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="J404" s="3">
-        <v>1.43</v>
+        <v>1.37</v>
       </c>
       <c r="K404" s="3">
-        <v>1.08</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="L404" s="3">
-        <v>0.97</v>
+        <v>1.01</v>
       </c>
       <c r="M404" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="405" spans="1:13">
@@ -18351,40 +18343,81 @@
         <v>415</v>
       </c>
       <c r="B405" s="2">
-        <v>14597</v>
+        <v>17256</v>
       </c>
       <c r="C405" s="2">
-        <v>8973</v>
+        <v>11317</v>
       </c>
       <c r="D405" s="2">
-        <v>20035</v>
+        <v>22948</v>
       </c>
       <c r="E405" s="2">
-        <v>18149</v>
+        <v>18944</v>
       </c>
       <c r="F405" s="2">
-        <v>12536</v>
+        <v>13868</v>
       </c>
       <c r="G405" s="2">
-        <v>23077</v>
+        <v>23621</v>
       </c>
       <c r="H405" s="3">
+        <v>1.26</v>
+      </c>
+      <c r="I405" s="3">
+        <v>1.08</v>
+      </c>
+      <c r="J405" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="K405" s="3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="L405" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="M405" s="3">
         <v>1.21</v>
       </c>
-      <c r="I405" s="3">
-        <v>0.98</v>
-      </c>
-      <c r="J405" s="3">
-        <v>1.39</v>
-      </c>
-      <c r="K405" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="L405" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="M405" s="3" t="s">
-        <v>420</v>
+    </row>
+    <row r="406" spans="1:13">
+      <c r="A406" t="s">
+        <v>416</v>
+      </c>
+      <c r="B406" s="2">
+        <v>16875</v>
+      </c>
+      <c r="C406" s="2">
+        <v>10288</v>
+      </c>
+      <c r="D406" s="2">
+        <v>23871</v>
+      </c>
+      <c r="E406" s="2">
+        <v>18367</v>
+      </c>
+      <c r="F406" s="2">
+        <v>12624</v>
+      </c>
+      <c r="G406" s="2">
+        <v>24036</v>
+      </c>
+      <c r="H406" s="3">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="I406" s="3">
+        <v>0.94</v>
+      </c>
+      <c r="J406" s="3">
+        <v>1.32</v>
+      </c>
+      <c r="K406" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="L406" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="M406" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
/home/ofenloch/workspaces/COVID19/rki-data-evaluation/getRKIData.sh: add data automatically downloaded at 2021-04-27--05-03-01
</commit_message>
<xml_diff>
--- a/rki-data/RKI-Nowcasting_Zahlen.xlsx
+++ b/rki-data/RKI-Nowcasting_Zahlen.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8708DC6-2CA6-42A2-BE81-9AFB8421B317}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4054224-2E5B-4822-A4B2-1332A555F077}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="7320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="457">
   <si>
     <t>Erläuterung</t>
   </si>
@@ -33,7 +33,7 @@
     <t/>
   </si>
   <si>
-    <t>Datenstand: 2021-04-25, 00:00 Uhr</t>
+    <t>Datenstand: 2021-04-26, 00:00 Uhr</t>
   </si>
   <si>
     <t/>
@@ -48,7 +48,7 @@
     <t/>
   </si>
   <si>
-    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-04-25 dargestellten Nowcasting-Kurve.</t>
+    <t>Die Schätzwerte entsprechen der im täglichen Lagebericht des Robert Koch-Instituts vom 2021-04-26 dargestellten Nowcasting-Kurve.</t>
   </si>
   <si>
     <t>Der letzte Schätzwert der Reproduktionszahl R wird ebenfalls im gleichen Lagebericht erwähnt.</t>
@@ -1321,6 +1321,9 @@
   </si>
   <si>
     <t>21.04.2021</t>
+  </si>
+  <si>
+    <t>22.04.2021</t>
   </si>
   <si>
     <t>Punktschätzer der Anzahl Neuerkrankungen (ohne Glättung)</t>
@@ -1741,7 +1744,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -1841,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M417"/>
+  <dimension ref="A1:M418"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:M417"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:M418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1857,40 +1860,40 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1916,22 +1919,22 @@
         <v>238</v>
       </c>
       <c r="H2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="M2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1957,22 +1960,22 @@
         <v>276</v>
       </c>
       <c r="H3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="M3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1998,22 +2001,22 @@
         <v>342</v>
       </c>
       <c r="H4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J4" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L4" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="M4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2039,22 +2042,22 @@
         <v>412</v>
       </c>
       <c r="H5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I5" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="J5" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="L5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="M5" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -16415,7 +16418,7 @@
         <v>7651</v>
       </c>
       <c r="C356" s="2">
-        <v>7541</v>
+        <v>7540</v>
       </c>
       <c r="D356" s="2">
         <v>7757</v>
@@ -16456,10 +16459,10 @@
         <v>7383</v>
       </c>
       <c r="C357" s="2">
-        <v>7277</v>
+        <v>7281</v>
       </c>
       <c r="D357" s="2">
-        <v>7491</v>
+        <v>7492</v>
       </c>
       <c r="E357" s="2">
         <v>7707</v>
@@ -16494,19 +16497,19 @@
         <v>375</v>
       </c>
       <c r="B358" s="2">
-        <v>7126</v>
+        <v>7125</v>
       </c>
       <c r="C358" s="2">
-        <v>7025</v>
+        <v>7024</v>
       </c>
       <c r="D358" s="2">
-        <v>7234</v>
+        <v>7233</v>
       </c>
       <c r="E358" s="2">
         <v>7470</v>
       </c>
       <c r="F358" s="2">
-        <v>7360</v>
+        <v>7361</v>
       </c>
       <c r="G358" s="2">
         <v>7578</v>
@@ -16535,13 +16538,13 @@
         <v>376</v>
       </c>
       <c r="B359" s="2">
-        <v>8955</v>
+        <v>8956</v>
       </c>
       <c r="C359" s="2">
-        <v>8826</v>
+        <v>8825</v>
       </c>
       <c r="D359" s="2">
-        <v>9067</v>
+        <v>9068</v>
       </c>
       <c r="E359" s="2">
         <v>7779</v>
@@ -16579,19 +16582,19 @@
         <v>8501</v>
       </c>
       <c r="C360" s="2">
-        <v>8388</v>
+        <v>8389</v>
       </c>
       <c r="D360" s="2">
-        <v>8599</v>
+        <v>8602</v>
       </c>
       <c r="E360" s="2">
         <v>7991</v>
       </c>
       <c r="F360" s="2">
-        <v>7879</v>
+        <v>7880</v>
       </c>
       <c r="G360" s="2">
-        <v>8097</v>
+        <v>8098</v>
       </c>
       <c r="H360" s="3">
         <v>1.01</v>
@@ -16620,19 +16623,19 @@
         <v>8089</v>
       </c>
       <c r="C361" s="2">
-        <v>7993</v>
+        <v>7989</v>
       </c>
       <c r="D361" s="2">
-        <v>8207</v>
+        <v>8205</v>
       </c>
       <c r="E361" s="2">
         <v>8168</v>
       </c>
       <c r="F361" s="2">
-        <v>8058</v>
+        <v>8057</v>
       </c>
       <c r="G361" s="2">
-        <v>8276</v>
+        <v>8277</v>
       </c>
       <c r="H361" s="3">
         <v>1.06</v>
@@ -16658,22 +16661,22 @@
         <v>379</v>
       </c>
       <c r="B362" s="2">
-        <v>7658</v>
+        <v>7659</v>
       </c>
       <c r="C362" s="2">
         <v>7547</v>
       </c>
       <c r="D362" s="2">
-        <v>7770</v>
+        <v>7771</v>
       </c>
       <c r="E362" s="2">
         <v>8301</v>
       </c>
       <c r="F362" s="2">
-        <v>8188</v>
+        <v>8187</v>
       </c>
       <c r="G362" s="2">
-        <v>8410</v>
+        <v>8411</v>
       </c>
       <c r="H362" s="3">
         <v>1.1100000000000001</v>
@@ -16702,10 +16705,10 @@
         <v>7940</v>
       </c>
       <c r="C363" s="2">
-        <v>7831</v>
+        <v>7832</v>
       </c>
       <c r="D363" s="2">
-        <v>8058</v>
+        <v>8061</v>
       </c>
       <c r="E363" s="2">
         <v>8047</v>
@@ -16714,7 +16717,7 @@
         <v>7939</v>
       </c>
       <c r="G363" s="2">
-        <v>8158</v>
+        <v>8160</v>
       </c>
       <c r="H363" s="3">
         <v>1.03</v>
@@ -16740,19 +16743,19 @@
         <v>381</v>
       </c>
       <c r="B364" s="2">
-        <v>7182</v>
+        <v>7181</v>
       </c>
       <c r="C364" s="2">
-        <v>7088</v>
+        <v>7083</v>
       </c>
       <c r="D364" s="2">
-        <v>7287</v>
+        <v>7282</v>
       </c>
       <c r="E364" s="2">
         <v>7717</v>
       </c>
       <c r="F364" s="2">
-        <v>7614</v>
+        <v>7613</v>
       </c>
       <c r="G364" s="2">
         <v>7830</v>
@@ -16781,19 +16784,19 @@
         <v>382</v>
       </c>
       <c r="B365" s="2">
-        <v>7343</v>
+        <v>7344</v>
       </c>
       <c r="C365" s="2">
         <v>7229</v>
       </c>
       <c r="D365" s="2">
-        <v>7430</v>
+        <v>7431</v>
       </c>
       <c r="E365" s="2">
         <v>7531</v>
       </c>
       <c r="F365" s="2">
-        <v>7423</v>
+        <v>7422</v>
       </c>
       <c r="G365" s="2">
         <v>7636</v>
@@ -16822,13 +16825,13 @@
         <v>383</v>
       </c>
       <c r="B366" s="2">
-        <v>9528</v>
+        <v>9527</v>
       </c>
       <c r="C366" s="2">
-        <v>9407</v>
+        <v>9408</v>
       </c>
       <c r="D366" s="2">
-        <v>9650</v>
+        <v>9651</v>
       </c>
       <c r="E366" s="2">
         <v>7998</v>
@@ -16863,22 +16866,22 @@
         <v>384</v>
       </c>
       <c r="B367" s="2">
-        <v>8913</v>
+        <v>8912</v>
       </c>
       <c r="C367" s="2">
-        <v>8809</v>
+        <v>8810</v>
       </c>
       <c r="D367" s="2">
-        <v>9040</v>
+        <v>9038</v>
       </c>
       <c r="E367" s="2">
         <v>8241</v>
       </c>
       <c r="F367" s="2">
-        <v>8133</v>
+        <v>8132</v>
       </c>
       <c r="G367" s="2">
-        <v>8352</v>
+        <v>8350</v>
       </c>
       <c r="H367" s="3">
         <v>1.02</v>
@@ -16904,13 +16907,13 @@
         <v>385</v>
       </c>
       <c r="B368" s="2">
-        <v>8997</v>
+        <v>8995</v>
       </c>
       <c r="C368" s="2">
-        <v>8866</v>
+        <v>8863</v>
       </c>
       <c r="D368" s="2">
-        <v>9107</v>
+        <v>9108</v>
       </c>
       <c r="E368" s="2">
         <v>8695</v>
@@ -16919,7 +16922,7 @@
         <v>8577</v>
       </c>
       <c r="G368" s="2">
-        <v>8806</v>
+        <v>8807</v>
       </c>
       <c r="H368" s="3">
         <v>1.1299999999999999</v>
@@ -16945,10 +16948,10 @@
         <v>386</v>
       </c>
       <c r="B369" s="2">
-        <v>8646</v>
+        <v>8647</v>
       </c>
       <c r="C369" s="2">
-        <v>8530</v>
+        <v>8531</v>
       </c>
       <c r="D369" s="2">
         <v>8756</v>
@@ -16978,7 +16981,7 @@
         <v>1.06</v>
       </c>
       <c r="M369" s="3">
-        <v>1.06</v>
+        <v>1.07</v>
       </c>
     </row>
     <row r="370" spans="1:13">
@@ -16986,22 +16989,22 @@
         <v>387</v>
       </c>
       <c r="B370" s="2">
-        <v>9018</v>
+        <v>9019</v>
       </c>
       <c r="C370" s="2">
         <v>8915</v>
       </c>
       <c r="D370" s="2">
-        <v>9141</v>
+        <v>9152</v>
       </c>
       <c r="E370" s="2">
-        <v>8894</v>
+        <v>8893</v>
       </c>
       <c r="F370" s="2">
-        <v>8780</v>
+        <v>8779</v>
       </c>
       <c r="G370" s="2">
-        <v>9011</v>
+        <v>9013</v>
       </c>
       <c r="H370" s="3">
         <v>1.1100000000000001</v>
@@ -17027,22 +17030,22 @@
         <v>388</v>
       </c>
       <c r="B371" s="2">
-        <v>8899</v>
+        <v>8901</v>
       </c>
       <c r="C371" s="2">
-        <v>8776</v>
+        <v>8775</v>
       </c>
       <c r="D371" s="2">
-        <v>9033</v>
+        <v>9025</v>
       </c>
       <c r="E371" s="2">
-        <v>8890</v>
+        <v>8891</v>
       </c>
       <c r="F371" s="2">
-        <v>8772</v>
+        <v>8771</v>
       </c>
       <c r="G371" s="2">
-        <v>9009</v>
+        <v>9010</v>
       </c>
       <c r="H371" s="3">
         <v>1.08</v>
@@ -17068,22 +17071,22 @@
         <v>389</v>
       </c>
       <c r="B372" s="2">
-        <v>9031</v>
+        <v>9032</v>
       </c>
       <c r="C372" s="2">
-        <v>8907</v>
+        <v>8899</v>
       </c>
       <c r="D372" s="2">
-        <v>9154</v>
+        <v>9157</v>
       </c>
       <c r="E372" s="2">
-        <v>8899</v>
+        <v>8900</v>
       </c>
       <c r="F372" s="2">
-        <v>8782</v>
+        <v>8780</v>
       </c>
       <c r="G372" s="2">
-        <v>9021</v>
+        <v>9022</v>
       </c>
       <c r="H372" s="3">
         <v>1.02</v>
@@ -17109,22 +17112,22 @@
         <v>390</v>
       </c>
       <c r="B373" s="2">
-        <v>11796</v>
+        <v>11793</v>
       </c>
       <c r="C373" s="2">
-        <v>11685</v>
+        <v>11665</v>
       </c>
       <c r="D373" s="2">
-        <v>11928</v>
+        <v>11934</v>
       </c>
       <c r="E373" s="2">
         <v>9686</v>
       </c>
       <c r="F373" s="2">
-        <v>9571</v>
+        <v>9563</v>
       </c>
       <c r="G373" s="2">
-        <v>9814</v>
+        <v>9817</v>
       </c>
       <c r="H373" s="3">
         <v>1.07</v>
@@ -17153,16 +17156,16 @@
         <v>11501</v>
       </c>
       <c r="C374" s="2">
-        <v>11361</v>
+        <v>11354</v>
       </c>
       <c r="D374" s="2">
-        <v>11634</v>
+        <v>11633</v>
       </c>
       <c r="E374" s="2">
         <v>10307</v>
       </c>
       <c r="F374" s="2">
-        <v>10182</v>
+        <v>10173</v>
       </c>
       <c r="G374" s="2">
         <v>10437</v>
@@ -17191,22 +17194,22 @@
         <v>392</v>
       </c>
       <c r="B375" s="2">
-        <v>11731</v>
+        <v>11730</v>
       </c>
       <c r="C375" s="2">
-        <v>11593</v>
+        <v>11590</v>
       </c>
       <c r="D375" s="2">
-        <v>11857</v>
+        <v>11863</v>
       </c>
       <c r="E375" s="2">
-        <v>11015</v>
+        <v>11014</v>
       </c>
       <c r="F375" s="2">
-        <v>10886</v>
+        <v>10877</v>
       </c>
       <c r="G375" s="2">
-        <v>11143</v>
+        <v>11146</v>
       </c>
       <c r="H375" s="3">
         <v>1.24</v>
@@ -17232,28 +17235,28 @@
         <v>393</v>
       </c>
       <c r="B376" s="2">
-        <v>11500</v>
+        <v>11497</v>
       </c>
       <c r="C376" s="2">
-        <v>11366</v>
+        <v>11349</v>
       </c>
       <c r="D376" s="2">
-        <v>11655</v>
+        <v>11647</v>
       </c>
       <c r="E376" s="2">
-        <v>11632</v>
+        <v>11630</v>
       </c>
       <c r="F376" s="2">
-        <v>11501</v>
+        <v>11489</v>
       </c>
       <c r="G376" s="2">
-        <v>11768</v>
+        <v>11769</v>
       </c>
       <c r="H376" s="3">
         <v>1.31</v>
       </c>
       <c r="I376" s="3">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="J376" s="3">
         <v>1.32</v>
@@ -17273,22 +17276,22 @@
         <v>394</v>
       </c>
       <c r="B377" s="2">
-        <v>12061</v>
+        <v>12059</v>
       </c>
       <c r="C377" s="2">
-        <v>11926</v>
+        <v>11927</v>
       </c>
       <c r="D377" s="2">
-        <v>12193</v>
+        <v>12203</v>
       </c>
       <c r="E377" s="2">
-        <v>11698</v>
+        <v>11697</v>
       </c>
       <c r="F377" s="2">
-        <v>11561</v>
+        <v>11555</v>
       </c>
       <c r="G377" s="2">
-        <v>11835</v>
+        <v>11836</v>
       </c>
       <c r="H377" s="3">
         <v>1.21</v>
@@ -17317,19 +17320,19 @@
         <v>11831</v>
       </c>
       <c r="C378" s="2">
-        <v>11709</v>
+        <v>11694</v>
       </c>
       <c r="D378" s="2">
-        <v>11994</v>
+        <v>11961</v>
       </c>
       <c r="E378" s="2">
-        <v>11781</v>
+        <v>11779</v>
       </c>
       <c r="F378" s="2">
-        <v>11648</v>
+        <v>11640</v>
       </c>
       <c r="G378" s="2">
-        <v>11925</v>
+        <v>11918</v>
       </c>
       <c r="H378" s="3">
         <v>1.1399999999999999</v>
@@ -17355,22 +17358,22 @@
         <v>396</v>
       </c>
       <c r="B379" s="2">
-        <v>12089</v>
+        <v>12082</v>
       </c>
       <c r="C379" s="2">
-        <v>11950</v>
+        <v>11962</v>
       </c>
       <c r="D379" s="2">
-        <v>12227</v>
+        <v>12212</v>
       </c>
       <c r="E379" s="2">
-        <v>11870</v>
+        <v>11867</v>
       </c>
       <c r="F379" s="2">
-        <v>11737</v>
+        <v>11733</v>
       </c>
       <c r="G379" s="2">
-        <v>12017</v>
+        <v>12006</v>
       </c>
       <c r="H379" s="3">
         <v>1.08</v>
@@ -17379,7 +17382,7 @@
         <v>1.07</v>
       </c>
       <c r="J379" s="3">
-        <v>1.0900000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="K379" s="3">
         <v>1.17</v>
@@ -17396,25 +17399,25 @@
         <v>397</v>
       </c>
       <c r="B380" s="2">
-        <v>15432</v>
+        <v>15434</v>
       </c>
       <c r="C380" s="2">
-        <v>15303</v>
+        <v>15285</v>
       </c>
       <c r="D380" s="2">
-        <v>15567</v>
+        <v>15596</v>
       </c>
       <c r="E380" s="2">
-        <v>12853</v>
+        <v>12851</v>
       </c>
       <c r="F380" s="2">
-        <v>12722</v>
+        <v>12717</v>
       </c>
       <c r="G380" s="2">
-        <v>12995</v>
+        <v>12993</v>
       </c>
       <c r="H380" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I380" s="3">
         <v>1.1000000000000001</v>
@@ -17437,19 +17440,19 @@
         <v>398</v>
       </c>
       <c r="B381" s="2">
-        <v>14878</v>
+        <v>14887</v>
       </c>
       <c r="C381" s="2">
-        <v>14724</v>
+        <v>14749</v>
       </c>
       <c r="D381" s="2">
-        <v>15043</v>
+        <v>15059</v>
       </c>
       <c r="E381" s="2">
         <v>13558</v>
       </c>
       <c r="F381" s="2">
-        <v>13421</v>
+        <v>13422</v>
       </c>
       <c r="G381" s="2">
         <v>13707</v>
@@ -17478,22 +17481,22 @@
         <v>399</v>
       </c>
       <c r="B382" s="2">
-        <v>15010</v>
+        <v>15023</v>
       </c>
       <c r="C382" s="2">
-        <v>14876</v>
+        <v>14862</v>
       </c>
       <c r="D382" s="2">
-        <v>15151</v>
+        <v>15228</v>
       </c>
       <c r="E382" s="2">
-        <v>14352</v>
+        <v>14356</v>
       </c>
       <c r="F382" s="2">
-        <v>14213</v>
+        <v>14214</v>
       </c>
       <c r="G382" s="2">
-        <v>14497</v>
+        <v>14524</v>
       </c>
       <c r="H382" s="3">
         <v>1.22</v>
@@ -17519,22 +17522,22 @@
         <v>400</v>
       </c>
       <c r="B383" s="2">
-        <v>14273</v>
+        <v>14266</v>
       </c>
       <c r="C383" s="2">
-        <v>14142</v>
+        <v>14102</v>
       </c>
       <c r="D383" s="2">
-        <v>14391</v>
+        <v>14394</v>
       </c>
       <c r="E383" s="2">
-        <v>14898</v>
+        <v>14902</v>
       </c>
       <c r="F383" s="2">
-        <v>14761</v>
+        <v>14749</v>
       </c>
       <c r="G383" s="2">
-        <v>15038</v>
+        <v>15069</v>
       </c>
       <c r="H383" s="3">
         <v>1.26</v>
@@ -17543,7 +17546,7 @@
         <v>1.25</v>
       </c>
       <c r="J383" s="3">
-        <v>1.26</v>
+        <v>1.27</v>
       </c>
       <c r="K383" s="3">
         <v>1.1399999999999999</v>
@@ -17560,22 +17563,22 @@
         <v>401</v>
       </c>
       <c r="B384" s="2">
-        <v>14840</v>
+        <v>14836</v>
       </c>
       <c r="C384" s="2">
-        <v>14708</v>
+        <v>14684</v>
       </c>
       <c r="D384" s="2">
-        <v>14952</v>
+        <v>14962</v>
       </c>
       <c r="E384" s="2">
-        <v>14750</v>
+        <v>14753</v>
       </c>
       <c r="F384" s="2">
-        <v>14613</v>
+        <v>14599</v>
       </c>
       <c r="G384" s="2">
-        <v>14884</v>
+        <v>14911</v>
       </c>
       <c r="H384" s="3">
         <v>1.1499999999999999</v>
@@ -17601,22 +17604,22 @@
         <v>402</v>
       </c>
       <c r="B385" s="2">
-        <v>14994</v>
+        <v>14997</v>
       </c>
       <c r="C385" s="2">
-        <v>14835</v>
+        <v>14860</v>
       </c>
       <c r="D385" s="2">
-        <v>15143</v>
+        <v>15138</v>
       </c>
       <c r="E385" s="2">
-        <v>14779</v>
+        <v>14780</v>
       </c>
       <c r="F385" s="2">
-        <v>14640</v>
+        <v>14627</v>
       </c>
       <c r="G385" s="2">
-        <v>14909</v>
+        <v>14930</v>
       </c>
       <c r="H385" s="3">
         <v>1.0900000000000001</v>
@@ -17642,22 +17645,22 @@
         <v>403</v>
       </c>
       <c r="B386" s="2">
-        <v>15344</v>
+        <v>15340</v>
       </c>
       <c r="C386" s="2">
-        <v>15182</v>
+        <v>15186</v>
       </c>
       <c r="D386" s="2">
-        <v>15490</v>
+        <v>15492</v>
       </c>
       <c r="E386" s="2">
-        <v>14863</v>
+        <v>14860</v>
       </c>
       <c r="F386" s="2">
-        <v>14717</v>
+        <v>14708</v>
       </c>
       <c r="G386" s="2">
-        <v>14994</v>
+        <v>14996</v>
       </c>
       <c r="H386" s="3">
         <v>1.04</v>
@@ -17683,22 +17686,22 @@
         <v>404</v>
       </c>
       <c r="B387" s="2">
-        <v>18827</v>
+        <v>18836</v>
       </c>
       <c r="C387" s="2">
-        <v>18611</v>
+        <v>18670</v>
       </c>
       <c r="D387" s="2">
-        <v>18996</v>
+        <v>18992</v>
       </c>
       <c r="E387" s="2">
-        <v>16001</v>
+        <v>16002</v>
       </c>
       <c r="F387" s="2">
-        <v>15834</v>
+        <v>15850</v>
       </c>
       <c r="G387" s="2">
-        <v>16145</v>
+        <v>16146</v>
       </c>
       <c r="H387" s="3">
         <v>1.07</v>
@@ -17724,22 +17727,22 @@
         <v>405</v>
       </c>
       <c r="B388" s="2">
-        <v>18482</v>
+        <v>18475</v>
       </c>
       <c r="C388" s="2">
-        <v>18306</v>
+        <v>18247</v>
       </c>
       <c r="D388" s="2">
-        <v>18642</v>
+        <v>18632</v>
       </c>
       <c r="E388" s="2">
         <v>16912</v>
       </c>
       <c r="F388" s="2">
-        <v>16733</v>
+        <v>16741</v>
       </c>
       <c r="G388" s="2">
-        <v>17068</v>
+        <v>17063</v>
       </c>
       <c r="H388" s="3">
         <v>1.1499999999999999</v>
@@ -17754,7 +17757,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="L388" s="3">
-        <v>1.1299999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="M388" s="3">
         <v>1.1299999999999999</v>
@@ -17765,19 +17768,19 @@
         <v>406</v>
       </c>
       <c r="B389" s="2">
-        <v>17870</v>
+        <v>17875</v>
       </c>
       <c r="C389" s="2">
-        <v>17683</v>
+        <v>17657</v>
       </c>
       <c r="D389" s="2">
-        <v>18026</v>
+        <v>18036</v>
       </c>
       <c r="E389" s="2">
-        <v>17631</v>
+        <v>17632</v>
       </c>
       <c r="F389" s="2">
-        <v>17445</v>
+        <v>17440</v>
       </c>
       <c r="G389" s="2">
         <v>17788</v>
@@ -17806,22 +17809,22 @@
         <v>407</v>
       </c>
       <c r="B390" s="2">
-        <v>16671</v>
+        <v>16669</v>
       </c>
       <c r="C390" s="2">
-        <v>16519</v>
+        <v>16484</v>
       </c>
       <c r="D390" s="2">
-        <v>16825</v>
+        <v>16850</v>
       </c>
       <c r="E390" s="2">
-        <v>17962</v>
+        <v>17964</v>
       </c>
       <c r="F390" s="2">
-        <v>17780</v>
+        <v>17764</v>
       </c>
       <c r="G390" s="2">
-        <v>18122</v>
+        <v>18127</v>
       </c>
       <c r="H390" s="3">
         <v>1.21</v>
@@ -17847,22 +17850,22 @@
         <v>408</v>
       </c>
       <c r="B391" s="2">
-        <v>16336</v>
+        <v>16321</v>
       </c>
       <c r="C391" s="2">
-        <v>16107</v>
+        <v>16167</v>
       </c>
       <c r="D391" s="2">
-        <v>16539</v>
+        <v>16454</v>
       </c>
       <c r="E391" s="2">
-        <v>17340</v>
+        <v>17335</v>
       </c>
       <c r="F391" s="2">
-        <v>17154</v>
+        <v>17139</v>
       </c>
       <c r="G391" s="2">
-        <v>17508</v>
+        <v>17493</v>
       </c>
       <c r="H391" s="3">
         <v>1.08</v>
@@ -17888,22 +17891,22 @@
         <v>409</v>
       </c>
       <c r="B392" s="2">
-        <v>15163</v>
+        <v>15178</v>
       </c>
       <c r="C392" s="2">
-        <v>14937</v>
+        <v>15017</v>
       </c>
       <c r="D392" s="2">
-        <v>15384</v>
+        <v>15359</v>
       </c>
       <c r="E392" s="2">
-        <v>16510</v>
+        <v>16511</v>
       </c>
       <c r="F392" s="2">
-        <v>16311</v>
+        <v>16331</v>
       </c>
       <c r="G392" s="2">
-        <v>16693</v>
+        <v>16675</v>
       </c>
       <c r="H392" s="3">
         <v>0.98</v>
@@ -17929,28 +17932,28 @@
         <v>410</v>
       </c>
       <c r="B393" s="2">
-        <v>14734</v>
+        <v>14705</v>
       </c>
       <c r="C393" s="2">
-        <v>14491</v>
+        <v>14477</v>
       </c>
       <c r="D393" s="2">
-        <v>14915</v>
+        <v>14944</v>
       </c>
       <c r="E393" s="2">
-        <v>15726</v>
+        <v>15718</v>
       </c>
       <c r="F393" s="2">
-        <v>15513</v>
+        <v>15536</v>
       </c>
       <c r="G393" s="2">
-        <v>15916</v>
+        <v>15902</v>
       </c>
       <c r="H393" s="3">
         <v>0.89</v>
       </c>
       <c r="I393" s="3">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="J393" s="3">
         <v>0.9</v>
@@ -17970,22 +17973,22 @@
         <v>411</v>
       </c>
       <c r="B394" s="2">
-        <v>18255</v>
+        <v>18246</v>
       </c>
       <c r="C394" s="2">
-        <v>17955</v>
+        <v>18001</v>
       </c>
       <c r="D394" s="2">
-        <v>18512</v>
+        <v>18461</v>
       </c>
       <c r="E394" s="2">
-        <v>16122</v>
+        <v>16113</v>
       </c>
       <c r="F394" s="2">
-        <v>15872</v>
+        <v>15915</v>
       </c>
       <c r="G394" s="2">
-        <v>16337</v>
+        <v>16304</v>
       </c>
       <c r="H394" s="3">
         <v>0.9</v>
@@ -18011,22 +18014,22 @@
         <v>412</v>
       </c>
       <c r="B395" s="2">
-        <v>17004</v>
+        <v>17007</v>
       </c>
       <c r="C395" s="2">
-        <v>16833</v>
+        <v>16778</v>
       </c>
       <c r="D395" s="2">
-        <v>17211</v>
+        <v>17290</v>
       </c>
       <c r="E395" s="2">
-        <v>16289</v>
+        <v>16284</v>
       </c>
       <c r="F395" s="2">
-        <v>16054</v>
+        <v>16068</v>
       </c>
       <c r="G395" s="2">
-        <v>16505</v>
+        <v>16513</v>
       </c>
       <c r="H395" s="3">
         <v>0.94</v>
@@ -18052,22 +18055,22 @@
         <v>413</v>
       </c>
       <c r="B396" s="2">
-        <v>15847</v>
+        <v>15827</v>
       </c>
       <c r="C396" s="2">
-        <v>15564</v>
+        <v>15688</v>
       </c>
       <c r="D396" s="2">
-        <v>16062</v>
+        <v>16018</v>
       </c>
       <c r="E396" s="2">
-        <v>16460</v>
+        <v>16446</v>
       </c>
       <c r="F396" s="2">
-        <v>16211</v>
+        <v>16236</v>
       </c>
       <c r="G396" s="2">
-        <v>16675</v>
+        <v>16678</v>
       </c>
       <c r="H396" s="3">
         <v>1</v>
@@ -18076,10 +18079,10 @@
         <v>0.99</v>
       </c>
       <c r="J396" s="3">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="K396" s="3">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="L396" s="3">
         <v>0.96</v>
@@ -18093,22 +18096,22 @@
         <v>414</v>
       </c>
       <c r="B397" s="2">
-        <v>16621</v>
+        <v>16597</v>
       </c>
       <c r="C397" s="2">
-        <v>16333</v>
+        <v>16339</v>
       </c>
       <c r="D397" s="2">
-        <v>16853</v>
+        <v>16856</v>
       </c>
       <c r="E397" s="2">
-        <v>16932</v>
+        <v>16919</v>
       </c>
       <c r="F397" s="2">
-        <v>16671</v>
+        <v>16702</v>
       </c>
       <c r="G397" s="2">
-        <v>17159</v>
+        <v>17156</v>
       </c>
       <c r="H397" s="3">
         <v>1.08</v>
@@ -18134,22 +18137,22 @@
         <v>415</v>
       </c>
       <c r="B398" s="2">
-        <v>15197</v>
+        <v>15192</v>
       </c>
       <c r="C398" s="2">
-        <v>14958</v>
+        <v>14907</v>
       </c>
       <c r="D398" s="2">
-        <v>15497</v>
+        <v>15457</v>
       </c>
       <c r="E398" s="2">
-        <v>16167</v>
+        <v>16156</v>
       </c>
       <c r="F398" s="2">
-        <v>15922</v>
+        <v>15928</v>
       </c>
       <c r="G398" s="2">
-        <v>16406</v>
+        <v>16405</v>
       </c>
       <c r="H398" s="3">
         <v>1</v>
@@ -18175,22 +18178,22 @@
         <v>416</v>
       </c>
       <c r="B399" s="2">
-        <v>14455</v>
+        <v>14475</v>
       </c>
       <c r="C399" s="2">
-        <v>14150</v>
+        <v>14259</v>
       </c>
       <c r="D399" s="2">
-        <v>14720</v>
+        <v>14684</v>
       </c>
       <c r="E399" s="2">
-        <v>15530</v>
+        <v>15523</v>
       </c>
       <c r="F399" s="2">
-        <v>15251</v>
+        <v>15298</v>
       </c>
       <c r="G399" s="2">
-        <v>15783</v>
+        <v>15754</v>
       </c>
       <c r="H399" s="3">
         <v>0.95</v>
@@ -18216,22 +18219,22 @@
         <v>417</v>
       </c>
       <c r="B400" s="2">
-        <v>14658</v>
+        <v>14664</v>
       </c>
       <c r="C400" s="2">
-        <v>14339</v>
+        <v>14368</v>
       </c>
       <c r="D400" s="2">
-        <v>14960</v>
+        <v>14916</v>
       </c>
       <c r="E400" s="2">
-        <v>15233</v>
+        <v>15232</v>
       </c>
       <c r="F400" s="2">
-        <v>14945</v>
+        <v>14968</v>
       </c>
       <c r="G400" s="2">
-        <v>15507</v>
+        <v>15478</v>
       </c>
       <c r="H400" s="3">
         <v>0.93</v>
@@ -18240,7 +18243,7 @@
         <v>0.92</v>
       </c>
       <c r="J400" s="3">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="K400" s="3">
         <v>0.97</v>
@@ -18249,7 +18252,7 @@
         <v>0.96</v>
       </c>
       <c r="M400" s="3">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="401" spans="1:13">
@@ -18257,22 +18260,22 @@
         <v>418</v>
       </c>
       <c r="B401" s="2">
-        <v>16674</v>
+        <v>16664</v>
       </c>
       <c r="C401" s="2">
-        <v>16267</v>
+        <v>16337</v>
       </c>
       <c r="D401" s="2">
-        <v>17004</v>
+        <v>17064</v>
       </c>
       <c r="E401" s="2">
-        <v>15246</v>
+        <v>15249</v>
       </c>
       <c r="F401" s="2">
-        <v>14928</v>
+        <v>14968</v>
       </c>
       <c r="G401" s="2">
-        <v>15545</v>
+        <v>15530</v>
       </c>
       <c r="H401" s="3">
         <v>0.9</v>
@@ -18298,22 +18301,22 @@
         <v>419</v>
       </c>
       <c r="B402" s="2">
-        <v>19098</v>
+        <v>19100</v>
       </c>
       <c r="C402" s="2">
-        <v>18638</v>
+        <v>18798</v>
       </c>
       <c r="D402" s="2">
-        <v>19569</v>
+        <v>19506</v>
       </c>
       <c r="E402" s="2">
-        <v>16222</v>
+        <v>16226</v>
       </c>
       <c r="F402" s="2">
-        <v>15848</v>
+        <v>15941</v>
       </c>
       <c r="G402" s="2">
-        <v>16563</v>
+        <v>16543</v>
       </c>
       <c r="H402" s="3">
         <v>1</v>
@@ -18322,7 +18325,7 @@
         <v>0.99</v>
       </c>
       <c r="J402" s="3">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="K402" s="3">
         <v>1.04</v>
@@ -18339,19 +18342,19 @@
         <v>420</v>
       </c>
       <c r="B403" s="2">
-        <v>19489</v>
+        <v>19474</v>
       </c>
       <c r="C403" s="2">
-        <v>19050</v>
+        <v>18995</v>
       </c>
       <c r="D403" s="2">
-        <v>19929</v>
+        <v>19976</v>
       </c>
       <c r="E403" s="2">
-        <v>17480</v>
+        <v>17475</v>
       </c>
       <c r="F403" s="2">
-        <v>17073</v>
+        <v>17125</v>
       </c>
       <c r="G403" s="2">
         <v>17865</v>
@@ -18380,22 +18383,22 @@
         <v>421</v>
       </c>
       <c r="B404" s="2">
-        <v>19073</v>
+        <v>19017</v>
       </c>
       <c r="C404" s="2">
+        <v>18599</v>
+      </c>
+      <c r="D404" s="2">
+        <v>19507</v>
+      </c>
+      <c r="E404" s="2">
         <v>18564</v>
       </c>
-      <c r="D404" s="2">
-        <v>19521</v>
-      </c>
-      <c r="E404" s="2">
-        <v>18584</v>
-      </c>
       <c r="F404" s="2">
-        <v>18130</v>
+        <v>18182</v>
       </c>
       <c r="G404" s="2">
-        <v>19006</v>
+        <v>19013</v>
       </c>
       <c r="H404" s="3">
         <v>1.22</v>
@@ -18421,22 +18424,22 @@
         <v>422</v>
       </c>
       <c r="B405" s="2">
-        <v>18725</v>
+        <v>18713</v>
       </c>
       <c r="C405" s="2">
-        <v>18070</v>
+        <v>18224</v>
       </c>
       <c r="D405" s="2">
-        <v>19288</v>
+        <v>19195</v>
       </c>
       <c r="E405" s="2">
-        <v>19096</v>
+        <v>19076</v>
       </c>
       <c r="F405" s="2">
-        <v>18580</v>
+        <v>18654</v>
       </c>
       <c r="G405" s="2">
-        <v>19577</v>
+        <v>19546</v>
       </c>
       <c r="H405" s="3">
         <v>1.25</v>
@@ -18462,22 +18465,22 @@
         <v>423</v>
       </c>
       <c r="B406" s="2">
-        <v>18639</v>
+        <v>18621</v>
       </c>
       <c r="C406" s="2">
-        <v>17959</v>
+        <v>18034</v>
       </c>
       <c r="D406" s="2">
-        <v>19398</v>
+        <v>19165</v>
       </c>
       <c r="E406" s="2">
-        <v>18982</v>
+        <v>18956</v>
       </c>
       <c r="F406" s="2">
-        <v>18411</v>
+        <v>18463</v>
       </c>
       <c r="G406" s="2">
-        <v>19534</v>
+        <v>19461</v>
       </c>
       <c r="H406" s="3">
         <v>1.17</v>
@@ -18486,13 +18489,13 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="J406" s="3">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="K406" s="3">
         <v>1.1200000000000001</v>
       </c>
       <c r="L406" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="M406" s="3">
         <v>1.1299999999999999</v>
@@ -18503,22 +18506,22 @@
         <v>424</v>
       </c>
       <c r="B407" s="2">
-        <v>18130</v>
+        <v>18093</v>
       </c>
       <c r="C407" s="2">
-        <v>17311</v>
+        <v>17430</v>
       </c>
       <c r="D407" s="2">
-        <v>18795</v>
+        <v>18699</v>
       </c>
       <c r="E407" s="2">
-        <v>18642</v>
+        <v>18611</v>
       </c>
       <c r="F407" s="2">
-        <v>17976</v>
+        <v>18072</v>
       </c>
       <c r="G407" s="2">
-        <v>19250</v>
+        <v>19142</v>
       </c>
       <c r="H407" s="3">
         <v>1.07</v>
@@ -18536,7 +18539,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="M407" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="408" spans="1:13">
@@ -18544,22 +18547,22 @@
         <v>425</v>
       </c>
       <c r="B408" s="2">
-        <v>22207</v>
+        <v>22255</v>
       </c>
       <c r="C408" s="2">
-        <v>21175</v>
+        <v>21374</v>
       </c>
       <c r="D408" s="2">
-        <v>22962</v>
+        <v>23093</v>
       </c>
       <c r="E408" s="2">
-        <v>19425</v>
+        <v>19421</v>
       </c>
       <c r="F408" s="2">
-        <v>18629</v>
+        <v>18765</v>
       </c>
       <c r="G408" s="2">
-        <v>20111</v>
+        <v>20038</v>
       </c>
       <c r="H408" s="3">
         <v>1.05</v>
@@ -18574,10 +18577,10 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="L408" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="M408" s="3">
-        <v>1.1399999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="409" spans="1:13">
@@ -18585,22 +18588,22 @@
         <v>426</v>
       </c>
       <c r="B409" s="2">
-        <v>20879</v>
+        <v>20805</v>
       </c>
       <c r="C409" s="2">
-        <v>19759</v>
+        <v>19698</v>
       </c>
       <c r="D409" s="2">
-        <v>21872</v>
+        <v>21889</v>
       </c>
       <c r="E409" s="2">
-        <v>19964</v>
+        <v>19944</v>
       </c>
       <c r="F409" s="2">
-        <v>19051</v>
+        <v>19134</v>
       </c>
       <c r="G409" s="2">
-        <v>20757</v>
+        <v>20711</v>
       </c>
       <c r="H409" s="3">
         <v>1.05</v>
@@ -18618,7 +18621,7 @@
         <v>1.07</v>
       </c>
       <c r="M409" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="410" spans="1:13">
@@ -18626,22 +18629,22 @@
         <v>427</v>
       </c>
       <c r="B410" s="2">
-        <v>20131</v>
+        <v>20102</v>
       </c>
       <c r="C410" s="2">
-        <v>18818</v>
+        <v>18832</v>
       </c>
       <c r="D410" s="2">
-        <v>21276</v>
+        <v>21275</v>
       </c>
       <c r="E410" s="2">
-        <v>20337</v>
+        <v>20314</v>
       </c>
       <c r="F410" s="2">
-        <v>19266</v>
+        <v>19333</v>
       </c>
       <c r="G410" s="2">
-        <v>21226</v>
+        <v>21239</v>
       </c>
       <c r="H410" s="3">
         <v>1.07</v>
@@ -18667,22 +18670,22 @@
         <v>428</v>
       </c>
       <c r="B411" s="2">
-        <v>19020</v>
+        <v>19043</v>
       </c>
       <c r="C411" s="2">
-        <v>17558</v>
+        <v>17891</v>
       </c>
       <c r="D411" s="2">
-        <v>20413</v>
+        <v>20145</v>
       </c>
       <c r="E411" s="2">
-        <v>20559</v>
+        <v>20551</v>
       </c>
       <c r="F411" s="2">
-        <v>19328</v>
+        <v>19449</v>
       </c>
       <c r="G411" s="2">
-        <v>21631</v>
+        <v>21600</v>
       </c>
       <c r="H411" s="3">
         <v>1.1000000000000001</v>
@@ -18697,7 +18700,7 @@
         <v>1.03</v>
       </c>
       <c r="L411" s="3">
-        <v>1.01</v>
+        <v>1</v>
       </c>
       <c r="M411" s="3">
         <v>1.05</v>
@@ -18708,31 +18711,31 @@
         <v>429</v>
       </c>
       <c r="B412" s="2">
-        <v>19943</v>
+        <v>19985</v>
       </c>
       <c r="C412" s="2">
-        <v>17991</v>
+        <v>18156</v>
       </c>
       <c r="D412" s="2">
-        <v>21909</v>
+        <v>21433</v>
       </c>
       <c r="E412" s="2">
-        <v>19993</v>
+        <v>19984</v>
       </c>
       <c r="F412" s="2">
-        <v>18531</v>
+        <v>18644</v>
       </c>
       <c r="G412" s="2">
-        <v>21368</v>
+        <v>21185</v>
       </c>
       <c r="H412" s="3">
         <v>1.03</v>
       </c>
       <c r="I412" s="3">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="J412" s="3">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="K412" s="3">
         <v>1.02</v>
@@ -18741,7 +18744,7 @@
         <v>0.99</v>
       </c>
       <c r="M412" s="3">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
     </row>
     <row r="413" spans="1:13">
@@ -18749,31 +18752,31 @@
         <v>430</v>
       </c>
       <c r="B413" s="2">
-        <v>19417</v>
+        <v>19266</v>
       </c>
       <c r="C413" s="2">
-        <v>16966</v>
+        <v>17427</v>
       </c>
       <c r="D413" s="2">
-        <v>21559</v>
+        <v>20644</v>
       </c>
       <c r="E413" s="2">
-        <v>19628</v>
+        <v>19599</v>
       </c>
       <c r="F413" s="2">
-        <v>17833</v>
+        <v>18077</v>
       </c>
       <c r="G413" s="2">
-        <v>21289</v>
+        <v>20874</v>
       </c>
       <c r="H413" s="3">
         <v>0.98</v>
       </c>
       <c r="I413" s="3">
-        <v>0.93</v>
+        <v>0.94</v>
       </c>
       <c r="J413" s="3">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="K413" s="3">
         <v>1.03</v>
@@ -18782,7 +18785,7 @@
         <v>1</v>
       </c>
       <c r="M413" s="3">
-        <v>1.08</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="414" spans="1:13">
@@ -18790,40 +18793,40 @@
         <v>431</v>
       </c>
       <c r="B414" s="2">
-        <v>20834</v>
+        <v>20180</v>
       </c>
       <c r="C414" s="2">
-        <v>17493</v>
+        <v>17758</v>
       </c>
       <c r="D414" s="2">
-        <v>24821</v>
+        <v>22509</v>
       </c>
       <c r="E414" s="2">
-        <v>19804</v>
+        <v>19619</v>
       </c>
       <c r="F414" s="2">
-        <v>17502</v>
+        <v>17808</v>
       </c>
       <c r="G414" s="2">
-        <v>22176</v>
+        <v>21183</v>
       </c>
       <c r="H414" s="3">
         <v>0.97</v>
       </c>
       <c r="I414" s="3">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="J414" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="K414" s="3">
         <v>1.04</v>
       </c>
-      <c r="K414" s="3">
-        <v>1.05</v>
-      </c>
       <c r="L414" s="3">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="M414" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="415" spans="1:13">
@@ -18831,40 +18834,40 @@
         <v>432</v>
       </c>
       <c r="B415" s="2">
-        <v>24536</v>
+        <v>23735</v>
       </c>
       <c r="C415" s="2">
-        <v>19247</v>
+        <v>20330</v>
       </c>
       <c r="D415" s="2">
-        <v>29448</v>
+        <v>26584</v>
       </c>
       <c r="E415" s="2">
-        <v>21183</v>
+        <v>20792</v>
       </c>
       <c r="F415" s="2">
-        <v>17924</v>
+        <v>18418</v>
       </c>
       <c r="G415" s="2">
-        <v>24434</v>
+        <v>22792</v>
       </c>
       <c r="H415" s="3">
-        <v>1.03</v>
+        <v>1.01</v>
       </c>
       <c r="I415" s="3">
-        <v>0.94</v>
+        <v>0.96</v>
       </c>
       <c r="J415" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="K415" s="3">
-        <v>1.07</v>
+        <v>1.04</v>
       </c>
       <c r="L415" s="3">
         <v>1</v>
       </c>
       <c r="M415" s="3">
-        <v>1.1299999999999999</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="416" spans="1:13">
@@ -18872,40 +18875,40 @@
         <v>433</v>
       </c>
       <c r="B416" s="2">
-        <v>24135</v>
+        <v>22213</v>
       </c>
       <c r="C416" s="2">
-        <v>16684</v>
+        <v>17395</v>
       </c>
       <c r="D416" s="2">
-        <v>31201</v>
+        <v>26882</v>
       </c>
       <c r="E416" s="2">
-        <v>22230</v>
+        <v>21348</v>
       </c>
       <c r="F416" s="2">
-        <v>17597</v>
+        <v>18227</v>
       </c>
       <c r="G416" s="2">
-        <v>26757</v>
+        <v>24155</v>
       </c>
       <c r="H416" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="I416" s="3">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="J416" s="3">
-        <v>1.22</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="K416" s="3">
-        <v>1.08</v>
+        <v>1.04</v>
       </c>
       <c r="L416" s="3">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="M416" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="417" spans="1:13">
@@ -18913,40 +18916,81 @@
         <v>434</v>
       </c>
       <c r="B417" s="2">
-        <v>22368</v>
+        <v>20284</v>
       </c>
       <c r="C417" s="2">
-        <v>14989</v>
+        <v>14454</v>
       </c>
       <c r="D417" s="2">
-        <v>29828</v>
+        <v>25907</v>
       </c>
       <c r="E417" s="2">
-        <v>22968</v>
+        <v>21603</v>
       </c>
       <c r="F417" s="2">
-        <v>17103</v>
+        <v>17484</v>
       </c>
       <c r="G417" s="2">
-        <v>28824</v>
+        <v>25470</v>
       </c>
       <c r="H417" s="3">
-        <v>1.17</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I417" s="3">
-        <v>1.02</v>
+        <v>1</v>
       </c>
       <c r="J417" s="3">
-        <v>1.32</v>
-      </c>
-      <c r="K417" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="L417" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="M417" s="3" t="s">
-        <v>453</v>
+        <v>1.23</v>
+      </c>
+      <c r="K417" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="L417" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="M417" s="3">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="418" spans="1:13">
+      <c r="A418" t="s">
+        <v>435</v>
+      </c>
+      <c r="B418" s="2">
+        <v>17763</v>
+      </c>
+      <c r="C418" s="2">
+        <v>11684</v>
+      </c>
+      <c r="D418" s="2">
+        <v>24243</v>
+      </c>
+      <c r="E418" s="2">
+        <v>20999</v>
+      </c>
+      <c r="F418" s="2">
+        <v>15966</v>
+      </c>
+      <c r="G418" s="2">
+        <v>25904</v>
+      </c>
+      <c r="H418" s="3">
+        <v>1.07</v>
+      </c>
+      <c r="I418" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="J418" s="3">
+        <v>1.22</v>
+      </c>
+      <c r="K418" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="L418" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="M418" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>